<commit_message>
Parte Antenna+ Headend acabada
</commit_message>
<xml_diff>
--- a/3C/ITSIT/CTI3.xlsx
+++ b/3C/ITSIT/CTI3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upvedues-my.sharepoint.com/personal/cribella_upv_edu_es/Documents/6-1/ITSIT/Trabajo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="366" documentId="11_AA5C2796D14A585BA2449CEF5E30AD8D88D2DDCB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE7FBE07-E5D4-4D92-ACA9-0CA65F00F29F}"/>
+  <xr:revisionPtr revIDLastSave="695" documentId="11_AA5C2796D14A585BA2449CEF5E30AD8D88D2DDCB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{776C1050-FA1C-4FD6-A824-12D7802EBF2C}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Network" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="321">
   <si>
     <t>TECHNICAL CHARACTERISTICS OF ELEMENTS FROM CATALOGUE</t>
   </si>
@@ -904,9 +904,6 @@
     <t>PREGUNTAR LO DE LOS CANALES 28 y 29 si se ponen juntos o se puede dejar asi</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>HEADEND LOSSES</t>
   </si>
   <si>
@@ -920,6 +917,90 @@
   </si>
   <si>
     <t>Amplificador input level, Sin (dBuV)</t>
+  </si>
+  <si>
+    <t>Preguntar que tipo de cable es este para buscar los valores que corresponden</t>
+  </si>
+  <si>
+    <t>Preguntar si los valores de Outdoor cable length son estos (Me tienen que decir Josepe estos valores a que altura estan las antenas estas)</t>
+  </si>
+  <si>
+    <t>AMPLIFIER GAIN</t>
+  </si>
+  <si>
+    <t>WITHOUT MAST AMPLIFIER</t>
+  </si>
+  <si>
+    <t>Required gain of Z-module amplifier, GT(dB)</t>
+  </si>
+  <si>
+    <t>Gain without mast amplifier?</t>
+  </si>
+  <si>
+    <t>WITH MAST AMPLIFIER</t>
+  </si>
+  <si>
+    <t>Adjusted gain of Z-module amplifier, Gamp(dB)</t>
+  </si>
+  <si>
+    <t>Adjusted gain of mast amplifier, Gpre(dB)</t>
+  </si>
+  <si>
+    <t>Gain with mast amplifier?</t>
+  </si>
+  <si>
+    <t>REVISAR ESTO</t>
+  </si>
+  <si>
+    <t>NOISE PARAMETERS</t>
+  </si>
+  <si>
+    <t>Noise equivalent bandwitdth (MHz)</t>
+  </si>
+  <si>
+    <t>Source noise temperature (satelite antenna)</t>
+  </si>
+  <si>
+    <t>Noise level (dBuV)</t>
+  </si>
+  <si>
+    <t>Minimum C/N (dB)</t>
+  </si>
+  <si>
+    <t>THERMAL NOISE</t>
+  </si>
+  <si>
+    <t>Equivalent noise figure Feq(dB)</t>
+  </si>
+  <si>
+    <t>C/N at outlet (dB)</t>
+  </si>
+  <si>
+    <t>C/N without mast amplifier?</t>
+  </si>
+  <si>
+    <t>C/N with mast amplifier?</t>
+  </si>
+  <si>
+    <t>PREGUNTAR SI LA FORMULA ESTA BIEN</t>
+  </si>
+  <si>
+    <t>REVISAR</t>
+  </si>
+  <si>
+    <t>S/I without mast amplifier (dB)</t>
+  </si>
+  <si>
+    <t>S/I without mast amplifier?</t>
+  </si>
+  <si>
+    <t>Output level of mast amplifier, Spre(dBuV)</t>
+  </si>
+  <si>
+    <t>S/I with mast amplifier (dB)</t>
+  </si>
+  <si>
+    <t>S/I with mast amplifier?</t>
   </si>
 </sst>
 </file>
@@ -929,7 +1010,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1817,10 +1898,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </right>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1834,7 +1915,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2163,21 +2244,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2190,7 +2256,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2224,8 +2289,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2251,7 +2316,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="9" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="9" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2259,9 +2323,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2273,6 +2334,36 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -2601,8 +2692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O308"/>
   <sheetViews>
-    <sheetView topLeftCell="B288" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G299" sqref="G299"/>
+    <sheetView topLeftCell="D260" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F178" sqref="F178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2612,8 +2703,8 @@
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" customWidth="1"/>
     <col min="5" max="5" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" customWidth="1"/>
-    <col min="14" max="14" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12201,16 +12292,16 @@
       <c r="A280" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="C280" s="136" t="s">
+      <c r="C280" s="186" t="s">
         <v>198</v>
       </c>
-      <c r="D280" s="137"/>
-      <c r="E280" s="138"/>
-      <c r="G280" s="136" t="s">
+      <c r="D280" s="187"/>
+      <c r="E280" s="188"/>
+      <c r="G280" s="186" t="s">
         <v>199</v>
       </c>
-      <c r="H280" s="137"/>
-      <c r="I280" s="138"/>
+      <c r="H280" s="187"/>
+      <c r="I280" s="188"/>
     </row>
     <row r="281" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A281" s="81" t="s">
@@ -12324,10 +12415,10 @@
     </row>
     <row r="286" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="287" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C287" s="146" t="s">
+      <c r="C287" s="140" t="s">
         <v>252</v>
       </c>
-      <c r="D287" s="146" t="s">
+      <c r="D287" s="140" t="s">
         <v>253</v>
       </c>
     </row>
@@ -12364,24 +12455,24 @@
       </c>
     </row>
     <row r="293" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C293" s="147" t="s">
+      <c r="C293" s="141" t="s">
         <v>49</v>
       </c>
-      <c r="D293" s="148" t="s">
+      <c r="D293" s="142" t="s">
         <v>50</v>
       </c>
-      <c r="E293" s="148" t="s">
+      <c r="E293" s="142" t="s">
         <v>255</v>
       </c>
-      <c r="F293" s="149" t="s">
+      <c r="F293" s="143" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A294" s="143" t="s">
+      <c r="A294" s="138" t="s">
         <v>256</v>
       </c>
-      <c r="C294" s="150">
+      <c r="C294" s="144">
         <v>40</v>
       </c>
       <c r="D294" s="115">
@@ -12390,71 +12481,71 @@
       <c r="E294" s="115">
         <v>47</v>
       </c>
-      <c r="F294" s="151">
+      <c r="F294" s="145">
         <v>47</v>
       </c>
     </row>
     <row r="295" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A295" s="144" t="s">
+      <c r="A295" s="139" t="s">
         <v>257</v>
       </c>
-      <c r="C295" s="152">
+      <c r="C295" s="146">
         <v>70</v>
       </c>
-      <c r="D295" s="153">
+      <c r="D295" s="147">
         <v>70</v>
       </c>
-      <c r="E295" s="153">
+      <c r="E295" s="147">
         <v>70</v>
       </c>
-      <c r="F295" s="154">
+      <c r="F295" s="148">
         <v>70</v>
       </c>
     </row>
     <row r="296" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="297" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A297" s="146" t="s">
+      <c r="A297" s="140" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A298" s="143" t="s">
+      <c r="A298" s="138" t="s">
         <v>259</v>
       </c>
-      <c r="C298" s="155">
+      <c r="C298" s="149">
         <f>MAX(H167:H273)+C294</f>
         <v>84.808999999999997</v>
       </c>
-      <c r="D298" s="156">
+      <c r="D298" s="150">
         <f>MAX(I167:I273)+D294</f>
         <v>75.03</v>
       </c>
-      <c r="E298" s="156">
+      <c r="E298" s="150">
         <f>MAX(K167:K273)+E294</f>
         <v>96.51</v>
       </c>
-      <c r="F298" s="157">
+      <c r="F298" s="151">
         <f>MAX(M167:M273)+F294</f>
         <v>104.52500000000001</v>
       </c>
     </row>
     <row r="299" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A299" s="144" t="s">
+      <c r="A299" s="139" t="s">
         <v>260</v>
       </c>
-      <c r="C299" s="158">
+      <c r="C299" s="152">
         <f>MIN(H167:H273)+C295</f>
         <v>104.16200000000001</v>
       </c>
-      <c r="D299" s="159">
+      <c r="D299" s="153">
         <f>MIN(I167:I273)+D295</f>
         <v>104.675</v>
       </c>
-      <c r="E299" s="159">
+      <c r="E299" s="153">
         <f>MIN(K167:K273)+E295</f>
         <v>106.358</v>
       </c>
-      <c r="F299" s="160">
+      <c r="F299" s="154">
         <f>MIN(M167:M273)+F295</f>
         <v>105.26300000000001</v>
       </c>
@@ -12464,19 +12555,19 @@
       <c r="A301" s="135" t="s">
         <v>261</v>
       </c>
-      <c r="C301" s="161">
+      <c r="C301" s="155">
         <f>0.25*C298+0.75*C299</f>
         <v>99.32374999999999</v>
       </c>
-      <c r="D301" s="162">
+      <c r="D301" s="156">
         <f>0.25*D298+0.75*D299</f>
         <v>97.263749999999987</v>
       </c>
-      <c r="E301" s="156">
+      <c r="E301" s="150">
         <f>0.25*E298+0.75*E299</f>
         <v>103.896</v>
       </c>
-      <c r="F301" s="157">
+      <c r="F301" s="151">
         <f>0.25*F298+0.75*F299</f>
         <v>105.07849999999999</v>
       </c>
@@ -12485,7 +12576,7 @@
       <c r="A302" s="135" t="s">
         <v>262</v>
       </c>
-      <c r="C302" s="167">
+      <c r="C302" s="161">
         <v>97</v>
       </c>
       <c r="D302" s="21">
@@ -12494,24 +12585,24 @@
       <c r="E302" s="21">
         <v>101</v>
       </c>
-      <c r="F302" s="170">
+      <c r="F302" s="164">
         <v>110</v>
       </c>
     </row>
     <row r="303" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A303" s="145" t="s">
+      <c r="A303" t="s">
         <v>263</v>
       </c>
-      <c r="C303" s="166" t="s">
+      <c r="C303" s="160" t="s">
         <v>267</v>
       </c>
-      <c r="D303" s="168" t="s">
+      <c r="D303" s="162" t="s">
         <v>268</v>
       </c>
-      <c r="E303" s="168" t="s">
+      <c r="E303" s="162" t="s">
         <v>269</v>
       </c>
-      <c r="F303" s="169" t="s">
+      <c r="F303" s="163" t="s">
         <v>270</v>
       </c>
     </row>
@@ -12526,12 +12617,12 @@
       </c>
     </row>
     <row r="306" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A306" s="146" t="s">
+      <c r="A306" s="140" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A307" s="143" t="s">
+      <c r="A307" s="138" t="s">
         <v>77</v>
       </c>
       <c r="C307" s="58">
@@ -12540,7 +12631,7 @@
       </c>
     </row>
     <row r="308" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A308" s="144" t="s">
+      <c r="A308" s="139" t="s">
         <v>78</v>
       </c>
       <c r="C308" s="60">
@@ -12564,15 +12655,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R82"/>
+  <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" customWidth="1"/>
     <col min="9" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12611,7 +12702,7 @@
       <c r="N1" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="141" t="s">
+      <c r="O1" s="136" t="s">
         <v>69</v>
       </c>
       <c r="P1" s="45" t="s">
@@ -12653,7 +12744,7 @@
       <c r="N2" s="44">
         <v>650</v>
       </c>
-      <c r="O2" s="142">
+      <c r="O2" s="137">
         <v>674</v>
       </c>
       <c r="P2" s="46">
@@ -12702,10 +12793,13 @@
         <v>0.11</v>
       </c>
       <c r="O5" s="2">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="P5" s="2">
         <v>0.23</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12778,7 +12872,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H13" t="s">
+      <c r="H13" s="1" t="s">
         <v>287</v>
       </c>
     </row>
@@ -13325,75 +13419,75 @@
     </row>
     <row r="38" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="147" t="s">
+      <c r="C39" s="141" t="s">
         <v>278</v>
       </c>
-      <c r="D39" s="149" t="s">
+      <c r="D39" s="143" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="146" t="s">
+      <c r="A40" s="140" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A41" s="143" t="s">
+      <c r="A41" s="138" t="s">
         <v>275</v>
       </c>
-      <c r="F41" s="183">
+      <c r="F41" s="176">
         <f>Network!C302</f>
         <v>97</v>
       </c>
-      <c r="G41" s="184">
+      <c r="G41" s="177">
         <f>Network!D302</f>
         <v>95</v>
       </c>
-      <c r="H41" s="185">
+      <c r="H41" s="178">
         <f>Network!E302</f>
         <v>101</v>
       </c>
-      <c r="I41" s="185">
+      <c r="I41" s="178">
         <f>Network!E302</f>
         <v>101</v>
       </c>
-      <c r="J41" s="185">
+      <c r="J41" s="178">
         <f>Network!E302</f>
         <v>101</v>
       </c>
-      <c r="K41" s="185">
+      <c r="K41" s="178">
         <f>Network!E302</f>
         <v>101</v>
       </c>
-      <c r="L41" s="185">
+      <c r="L41" s="178">
         <f>Network!E302</f>
         <v>101</v>
       </c>
-      <c r="M41" s="185">
+      <c r="M41" s="178">
         <f>Network!E302</f>
         <v>101</v>
       </c>
-      <c r="N41" s="185">
+      <c r="N41" s="178">
         <f>Network!E302</f>
         <v>101</v>
       </c>
-      <c r="O41" s="185">
+      <c r="O41" s="178">
         <f>Network!E302</f>
         <v>101</v>
       </c>
-      <c r="P41" s="186">
+      <c r="P41" s="179">
         <f>Network!F302</f>
         <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="172" t="s">
+      <c r="A42" s="166" t="s">
         <v>276</v>
       </c>
-      <c r="F42" s="167">
+      <c r="F42" s="161">
         <v>8</v>
       </c>
-      <c r="G42" s="181">
+      <c r="G42" s="174">
         <v>7</v>
       </c>
       <c r="H42" s="21">
@@ -13420,25 +13514,25 @@
       <c r="O42" s="21">
         <v>0</v>
       </c>
-      <c r="P42" s="170">
+      <c r="P42" s="164">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="172" t="s">
+      <c r="A43" s="166" t="s">
         <v>277</v>
       </c>
-      <c r="C43" s="164">
+      <c r="C43" s="158">
         <v>0.3</v>
       </c>
-      <c r="D43" s="165">
+      <c r="D43" s="159">
         <v>0.5</v>
       </c>
-      <c r="F43" s="167">
+      <c r="F43" s="161">
         <f>F42*C43</f>
         <v>2.4</v>
       </c>
-      <c r="G43" s="181">
+      <c r="G43" s="174">
         <f>G42*C43</f>
         <v>2.1</v>
       </c>
@@ -13474,300 +13568,1261 @@
         <f>O42*D43</f>
         <v>0</v>
       </c>
-      <c r="P43" s="170">
+      <c r="P43" s="164">
         <f>P42*D43</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A44" s="178" t="s">
+      <c r="A44" s="172" t="s">
         <v>280</v>
       </c>
-      <c r="F44" s="191">
-        <f>F41+F43</f>
+      <c r="F44" s="183">
+        <f t="shared" ref="F44:P44" si="1">F41+F43</f>
         <v>99.4</v>
       </c>
-      <c r="G44" s="192">
-        <f>G41+G43</f>
+      <c r="G44" s="184">
+        <f t="shared" si="1"/>
         <v>97.1</v>
       </c>
       <c r="H44" s="90">
-        <f>H41+H43</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
       <c r="I44" s="90">
-        <f>I41+I43</f>
+        <f t="shared" si="1"/>
         <v>103.5</v>
       </c>
       <c r="J44" s="90">
-        <f>J41+J43</f>
+        <f t="shared" si="1"/>
         <v>103.5</v>
       </c>
       <c r="K44" s="90">
-        <f>K41+K43</f>
+        <f t="shared" si="1"/>
         <v>103</v>
       </c>
       <c r="L44" s="90">
-        <f>L41+L43</f>
+        <f t="shared" si="1"/>
         <v>102.5</v>
       </c>
       <c r="M44" s="90">
-        <f>M41+M43</f>
+        <f t="shared" si="1"/>
         <v>102</v>
       </c>
       <c r="N44" s="90">
-        <f>N41+N43</f>
+        <f t="shared" si="1"/>
         <v>101.5</v>
       </c>
       <c r="O44" s="90">
-        <f>O41+O43</f>
+        <f t="shared" si="1"/>
         <v>101</v>
       </c>
-      <c r="P44" s="193">
-        <f>P41+P43</f>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A45" s="172" t="s">
-        <v>281</v>
-      </c>
-      <c r="F45" s="179">
-        <f>F19-F81</f>
-        <v>99.032015015757835</v>
-      </c>
-      <c r="G45" s="182">
-        <f t="shared" ref="G45:P45" si="1">G19-G81</f>
-        <v>101.17931555708239</v>
-      </c>
-      <c r="H45" s="174">
+      <c r="P44" s="185">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="I45" s="174">
-        <f t="shared" si="1"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="166" t="s">
+        <v>281</v>
+      </c>
+      <c r="F45" s="173">
+        <f>F19-F87</f>
+        <v>99.032015015757835</v>
+      </c>
+      <c r="G45" s="175">
+        <f t="shared" ref="G45:P45" si="2">G19-G87</f>
+        <v>101.17931555708239</v>
+      </c>
+      <c r="H45" s="168">
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="J45" s="174">
-        <f t="shared" si="1"/>
+      <c r="I45" s="168">
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="K45" s="174">
-        <f t="shared" si="1"/>
+      <c r="J45" s="168">
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="L45" s="174">
-        <f t="shared" si="1"/>
+      <c r="K45" s="168">
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="M45" s="174">
-        <f t="shared" si="1"/>
+      <c r="L45" s="168">
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="N45" s="174">
-        <f t="shared" si="1"/>
+      <c r="M45" s="168">
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="O45" s="174">
-        <f t="shared" si="1"/>
+      <c r="N45" s="168">
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="P45" s="180">
-        <f t="shared" si="1"/>
+      <c r="O45" s="168">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="P45" s="171">
+        <f t="shared" si="2"/>
         <v>113.03201501575784</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="144" t="s">
+      <c r="A46" s="139" t="s">
         <v>282</v>
       </c>
-      <c r="F46" s="187" t="s">
-        <v>288</v>
-      </c>
-      <c r="G46" s="188" t="s">
-        <v>171</v>
-      </c>
-      <c r="H46" s="189" t="s">
-        <v>171</v>
-      </c>
-      <c r="I46" s="189" t="s">
-        <v>171</v>
-      </c>
-      <c r="J46" s="189" t="s">
-        <v>171</v>
-      </c>
-      <c r="K46" s="189" t="s">
-        <v>171</v>
-      </c>
-      <c r="L46" s="189" t="s">
-        <v>171</v>
-      </c>
-      <c r="M46" s="189" t="s">
-        <v>171</v>
-      </c>
-      <c r="N46" s="189" t="s">
-        <v>171</v>
-      </c>
-      <c r="O46" s="189" t="s">
-        <v>171</v>
-      </c>
-      <c r="P46" s="190" t="s">
-        <v>171</v>
+      <c r="F46" s="180" t="str">
+        <f>IF(F44&lt;=(F19-F87),"OK","NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="G46" s="181" t="str">
+        <f>IF(G44&lt;=(G19-G87),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="H46" s="181" t="str">
+        <f>IF(H44&lt;=(H19-H87),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="I46" s="181" t="str">
+        <f>IF(I44&lt;=(I19-I87),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="J46" s="181" t="str">
+        <f>IF(J44&lt;=(J19-J87),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="K46" s="181" t="str">
+        <f>IF(K44&lt;=(K19-K87),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="L46" s="181" t="str">
+        <f>IF(L44&lt;=(L19-L87),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="M46" s="181" t="str">
+        <f>IF(M44&lt;=(M19-M87),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="N46" s="181" t="str">
+        <f>IF(N44&lt;=(N19-N87),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="O46" s="191" t="str">
+        <f>IF(O44&lt;=(O19-O87),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="P46" s="182" t="str">
+        <f>IF(P44&lt;=(P19-P87),"OK","NO")</f>
+        <v>OK</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="48" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="146" t="s">
+      <c r="A48" s="140" t="s">
+        <v>288</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A49" s="165" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="171" t="s">
+      <c r="F49" s="149">
+        <v>6</v>
+      </c>
+      <c r="G49" s="150">
+        <v>8</v>
+      </c>
+      <c r="H49" s="150">
+        <v>8</v>
+      </c>
+      <c r="I49" s="150">
+        <v>8</v>
+      </c>
+      <c r="J49" s="150">
+        <v>8</v>
+      </c>
+      <c r="K49" s="150">
+        <v>8</v>
+      </c>
+      <c r="L49" s="150">
+        <v>8</v>
+      </c>
+      <c r="M49" s="150">
+        <v>8</v>
+      </c>
+      <c r="N49" s="150">
+        <v>8</v>
+      </c>
+      <c r="O49" s="151">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A50" s="166" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="172" t="s">
+      <c r="F50" s="161">
+        <f>F5*F49</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G50" s="21">
+        <f>G5*G49</f>
+        <v>0.48</v>
+      </c>
+      <c r="H50" s="21">
+        <f>H5*H49</f>
+        <v>0.8</v>
+      </c>
+      <c r="I50" s="21">
+        <f t="shared" ref="I50:N50" si="3">I5*I49</f>
+        <v>0.8</v>
+      </c>
+      <c r="J50" s="21">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="K50" s="21">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="L50" s="21">
+        <f t="shared" si="3"/>
+        <v>0.88</v>
+      </c>
+      <c r="M50" s="21">
+        <f t="shared" si="3"/>
+        <v>0.88</v>
+      </c>
+      <c r="N50" s="21">
+        <f t="shared" si="3"/>
+        <v>0.88</v>
+      </c>
+      <c r="O50" s="164">
+        <f>O5*O49</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="166" t="s">
+        <v>276</v>
+      </c>
+      <c r="F51" s="161">
+        <v>8</v>
+      </c>
+      <c r="G51" s="21">
+        <v>7</v>
+      </c>
+      <c r="H51" s="21">
+        <v>6</v>
+      </c>
+      <c r="I51" s="21">
+        <v>5</v>
+      </c>
+      <c r="J51" s="21">
+        <v>5</v>
+      </c>
+      <c r="K51" s="21">
+        <v>4</v>
+      </c>
+      <c r="L51" s="21">
+        <v>3</v>
+      </c>
+      <c r="M51" s="21">
+        <v>2</v>
+      </c>
+      <c r="N51" s="21">
+        <v>1</v>
+      </c>
+      <c r="O51" s="164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="166" t="s">
+        <v>277</v>
+      </c>
+      <c r="C52" s="158">
+        <v>0.3</v>
+      </c>
+      <c r="D52" s="159">
+        <v>0.5</v>
+      </c>
+      <c r="F52" s="161">
+        <f>C52*F51</f>
+        <v>2.4</v>
+      </c>
+      <c r="G52" s="21">
+        <f>C52*G51</f>
+        <v>2.1</v>
+      </c>
+      <c r="H52" s="21">
+        <f>H51*D52</f>
+        <v>3</v>
+      </c>
+      <c r="I52" s="21">
+        <f>D52*I51</f>
+        <v>2.5</v>
+      </c>
+      <c r="J52" s="21">
+        <f>D52*J51</f>
+        <v>2.5</v>
+      </c>
+      <c r="K52" s="21">
+        <f>D52*K51</f>
+        <v>2</v>
+      </c>
+      <c r="L52" s="21">
+        <f>D52*L51</f>
+        <v>1.5</v>
+      </c>
+      <c r="M52" s="21">
+        <f>D52*M51</f>
+        <v>1</v>
+      </c>
+      <c r="N52" s="21">
+        <f>D52*N51</f>
+        <v>0.5</v>
+      </c>
+      <c r="O52" s="164">
+        <f>D52*O51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A53" s="166" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="172" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="172" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="172" t="s">
+      <c r="F53" s="161">
+        <f>F52+F50</f>
+        <v>2.7</v>
+      </c>
+      <c r="G53" s="21">
+        <f>G52+G50</f>
+        <v>2.58</v>
+      </c>
+      <c r="H53" s="21">
+        <f>H52+H50</f>
+        <v>3.8</v>
+      </c>
+      <c r="I53" s="21">
+        <f>I52+I50</f>
+        <v>3.3</v>
+      </c>
+      <c r="J53" s="21">
+        <f>J52+J50</f>
+        <v>3.3</v>
+      </c>
+      <c r="K53" s="21">
+        <f>K52+K50</f>
+        <v>2.8</v>
+      </c>
+      <c r="L53" s="21">
+        <f>L52+L50</f>
+        <v>2.38</v>
+      </c>
+      <c r="M53" s="21">
+        <f>M52+M50</f>
+        <v>1.88</v>
+      </c>
+      <c r="N53" s="21">
+        <f>N52+N50</f>
+        <v>1.38</v>
+      </c>
+      <c r="O53" s="164">
+        <f>O52+O50</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="167" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="173" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="79" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="146" t="s">
+      <c r="F54" s="152">
+        <f>F32-F53</f>
+        <v>67.3</v>
+      </c>
+      <c r="G54" s="153">
+        <f>G32-G53</f>
+        <v>55.42</v>
+      </c>
+      <c r="H54" s="153">
+        <f>H32-H53</f>
+        <v>46.2</v>
+      </c>
+      <c r="I54" s="153">
+        <f>I32-I53</f>
+        <v>46.7</v>
+      </c>
+      <c r="J54" s="153">
+        <f>J32-J53</f>
+        <v>46.7</v>
+      </c>
+      <c r="K54" s="153">
+        <f>K32-K53</f>
+        <v>47.2</v>
+      </c>
+      <c r="L54" s="153">
+        <f>L32-L53</f>
+        <v>47.62</v>
+      </c>
+      <c r="M54" s="153">
+        <f>M32-M53</f>
+        <v>48.12</v>
+      </c>
+      <c r="N54" s="153">
+        <f>N32-N53</f>
+        <v>48.62</v>
+      </c>
+      <c r="O54" s="154">
+        <f>O32-O53</f>
+        <v>49.12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="140" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A58" s="165" t="s">
+        <v>297</v>
+      </c>
+      <c r="F58" s="192">
+        <f>F44-(F32-F53)</f>
+        <v>32.100000000000009</v>
+      </c>
+      <c r="G58" s="193">
+        <f>G44-(G32-G53)</f>
+        <v>41.679999999999993</v>
+      </c>
+      <c r="H58" s="193">
+        <f>H44-(H32-H53)</f>
+        <v>57.8</v>
+      </c>
+      <c r="I58" s="193">
+        <f>I44-(I32-I53)</f>
+        <v>56.8</v>
+      </c>
+      <c r="J58" s="193">
+        <f>J44-(J32-J53)</f>
+        <v>56.8</v>
+      </c>
+      <c r="K58" s="193">
+        <f t="shared" ref="K58:O58" si="4">K44-(K32-K53)</f>
+        <v>55.8</v>
+      </c>
+      <c r="L58" s="193">
+        <f t="shared" si="4"/>
+        <v>54.88</v>
+      </c>
+      <c r="M58" s="193">
+        <f t="shared" si="4"/>
+        <v>53.88</v>
+      </c>
+      <c r="N58" s="193">
+        <f t="shared" si="4"/>
+        <v>52.88</v>
+      </c>
+      <c r="O58" s="194">
+        <f t="shared" si="4"/>
+        <v>51.88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="167" t="s">
+        <v>298</v>
+      </c>
+      <c r="F59" s="180" t="str">
+        <f>IF(AND(F16&gt;F58,(F16-F17)&lt;F58),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="G59" s="181" t="str">
+        <f t="shared" ref="G59:O59" si="5">IF(AND(G16&gt;G58,(G16-G17)&lt;G58),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="H59" s="181" t="str">
+        <f t="shared" si="5"/>
+        <v>NO</v>
+      </c>
+      <c r="I59" s="181" t="str">
+        <f t="shared" si="5"/>
+        <v>NO</v>
+      </c>
+      <c r="J59" s="181" t="str">
+        <f t="shared" si="5"/>
+        <v>NO</v>
+      </c>
+      <c r="K59" s="181" t="str">
+        <f t="shared" si="5"/>
+        <v>NO</v>
+      </c>
+      <c r="L59" s="181" t="str">
+        <f t="shared" si="5"/>
+        <v>NO</v>
+      </c>
+      <c r="M59" s="181" t="str">
+        <f t="shared" si="5"/>
+        <v>NO</v>
+      </c>
+      <c r="N59" s="181" t="str">
+        <f t="shared" si="5"/>
+        <v>NO</v>
+      </c>
+      <c r="O59" s="182" t="str">
+        <f t="shared" si="5"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="140" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A62" s="165" t="s">
+        <v>300</v>
+      </c>
+      <c r="F62" s="149">
+        <f>IF(F58-F24&gt;F16-F17,F58-F24,F16-F17)</f>
+        <v>32.100000000000009</v>
+      </c>
+      <c r="G62" s="150">
+        <f t="shared" ref="G62:O62" si="6">IF(G58-G24&gt;G16-G17,G58-G24,G16-G17)</f>
+        <v>41.679999999999993</v>
+      </c>
+      <c r="H62" s="150">
+        <f t="shared" si="6"/>
+        <v>29.799999999999997</v>
+      </c>
+      <c r="I62" s="150">
+        <f>IF(I58-I24&gt;I16-I17,I58-I24,I16-I17)</f>
+        <v>28.799999999999997</v>
+      </c>
+      <c r="J62" s="150">
+        <f t="shared" si="6"/>
+        <v>28.799999999999997</v>
+      </c>
+      <c r="K62" s="150">
+        <f t="shared" si="6"/>
+        <v>27.799999999999997</v>
+      </c>
+      <c r="L62" s="150">
+        <f t="shared" si="6"/>
+        <v>26.880000000000003</v>
+      </c>
+      <c r="M62" s="150">
+        <f t="shared" si="6"/>
+        <v>25.880000000000003</v>
+      </c>
+      <c r="N62" s="150">
+        <f t="shared" si="6"/>
+        <v>24.880000000000003</v>
+      </c>
+      <c r="O62" s="151">
+        <f t="shared" si="6"/>
+        <v>23.880000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63" s="166" t="s">
+        <v>301</v>
+      </c>
+      <c r="F63" s="161">
+        <f>F58-F62</f>
+        <v>0</v>
+      </c>
+      <c r="G63" s="21">
+        <f t="shared" ref="G63:O63" si="7">G58-G62</f>
+        <v>0</v>
+      </c>
+      <c r="H63" s="21">
+        <f>H58-H62</f>
+        <v>28</v>
+      </c>
+      <c r="I63" s="21">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+      <c r="J63" s="21">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+      <c r="K63" s="21">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+      <c r="L63" s="21">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+      <c r="M63" s="21">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+      <c r="N63" s="21">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+      <c r="O63" s="164">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+      <c r="P63" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="167" t="s">
+        <v>302</v>
+      </c>
+      <c r="F64" s="180" t="str">
+        <f>IF(AND(F16&gt;F62,(F16-F17)&lt;F62),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="G64" s="181" t="str">
+        <f t="shared" ref="G64:O64" si="8">IF(AND(G16&gt;G62,(G16-G17)&lt;G62),"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="H64" s="181" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="I64" s="181" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="J64" s="181" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="K64" s="181" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="L64" s="181" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="M64" s="181" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="N64" s="181" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+      <c r="O64" s="182" t="str">
+        <f t="shared" si="8"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="66" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="195" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A67" s="166" t="s">
+        <v>305</v>
+      </c>
+      <c r="F67" s="149">
+        <v>0.15</v>
+      </c>
+      <c r="G67" s="150">
+        <v>1.536</v>
+      </c>
+      <c r="H67" s="150">
+        <v>8</v>
+      </c>
+      <c r="I67" s="150">
+        <v>8</v>
+      </c>
+      <c r="J67" s="150">
+        <v>8</v>
+      </c>
+      <c r="K67" s="150">
+        <v>8</v>
+      </c>
+      <c r="L67" s="150">
+        <v>8</v>
+      </c>
+      <c r="M67" s="150">
+        <v>8</v>
+      </c>
+      <c r="N67" s="150">
+        <v>8</v>
+      </c>
+      <c r="O67" s="151">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A68" s="166" t="s">
+        <v>306</v>
+      </c>
+      <c r="F68" s="161">
+        <v>290</v>
+      </c>
+      <c r="G68" s="21">
+        <v>290</v>
+      </c>
+      <c r="H68" s="21">
+        <v>290</v>
+      </c>
+      <c r="I68" s="21">
+        <v>290</v>
+      </c>
+      <c r="J68" s="21">
+        <v>290</v>
+      </c>
+      <c r="K68" s="21">
+        <v>290</v>
+      </c>
+      <c r="L68" s="21">
+        <v>290</v>
+      </c>
+      <c r="M68" s="21">
+        <v>290</v>
+      </c>
+      <c r="N68" s="21">
+        <v>290</v>
+      </c>
+      <c r="O68" s="164">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A69" s="166" t="s">
+        <v>307</v>
+      </c>
+      <c r="F69" s="161">
+        <v>-13</v>
+      </c>
+      <c r="G69" s="21">
+        <v>-3</v>
+      </c>
+      <c r="H69" s="21">
+        <v>4</v>
+      </c>
+      <c r="I69" s="21">
+        <v>4</v>
+      </c>
+      <c r="J69" s="21">
+        <v>4</v>
+      </c>
+      <c r="K69" s="21">
+        <v>4</v>
+      </c>
+      <c r="L69" s="21">
+        <v>4</v>
+      </c>
+      <c r="M69" s="21">
+        <v>4</v>
+      </c>
+      <c r="N69" s="21">
+        <v>4</v>
+      </c>
+      <c r="O69" s="164">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="167" t="s">
+        <v>308</v>
+      </c>
+      <c r="F70" s="152">
+        <v>38</v>
+      </c>
+      <c r="G70" s="153">
+        <v>18</v>
+      </c>
+      <c r="H70" s="153">
+        <v>25</v>
+      </c>
+      <c r="I70" s="153">
+        <v>25</v>
+      </c>
+      <c r="J70" s="153">
+        <v>25</v>
+      </c>
+      <c r="K70" s="153">
+        <v>25</v>
+      </c>
+      <c r="L70" s="153">
+        <v>25</v>
+      </c>
+      <c r="M70" s="153">
+        <v>25</v>
+      </c>
+      <c r="N70" s="153">
+        <v>25</v>
+      </c>
+      <c r="O70" s="154">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A72" s="196" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="197" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A74" s="166" t="s">
+        <v>310</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F74" s="149">
+        <f>10*LOG10(10^((F18+F53)/10)+10^((F53-F58)/10)*(10^((F43+Network!H277)/10)-1))</f>
+        <v>18.760497143477163</v>
+      </c>
+      <c r="G74" s="150">
+        <f>10*LOG10(10^((G18+G53)/10)+10^((G53-G58)/10)*(10^((G43+Network!I277)/10)-1))</f>
+        <v>13.16833294530084</v>
+      </c>
+      <c r="H74" s="150">
+        <f>10*LOG10(10^((H18+H53)/10)+10^((H53-H58)/10)*(10^((H43+Network!J277)/10)-1))</f>
+        <v>12.873754086854778</v>
+      </c>
+      <c r="I74" s="150">
+        <f>10*LOG10(10^((I18+I53)/10)+10^((I53-I58)/10)*(10^((I43+Network!J277)/10)-1))</f>
+        <v>12.382668184740464</v>
+      </c>
+      <c r="J74" s="150">
+        <f>10*LOG10(10^((J18+J53)/10)+10^((J53-J58)/10)*(10^((J43+Network!J277)/10)-1))</f>
+        <v>12.382668184740464</v>
+      </c>
+      <c r="K74" s="150">
+        <f>10*LOG10(10^((K18+K53)/10)+10^((K53-K58)/10)*(10^((K43+Network!J277)/10)-1))</f>
+        <v>11.892648202220018</v>
+      </c>
+      <c r="L74" s="150">
+        <f>10*LOG10(10^((L18+L53)/10)+10^((L53-L58)/10)*(10^((L43+Network!J277)/10)-1))</f>
+        <v>11.481945853076247</v>
+      </c>
+      <c r="M74" s="150">
+        <f>10*LOG10(10^((M18+M53)/10)+10^((M53-M58)/10)*(10^((M43+Network!K277)/10)-1))</f>
+        <v>11.124620043324962</v>
+      </c>
+      <c r="N74" s="150">
+        <f>10*LOG10(10^((N18+N53)/10)+10^((N53-N58)/10)*(10^((N43+Network!K277)/10)-1))</f>
+        <v>10.653546318599503</v>
+      </c>
+      <c r="O74" s="151">
+        <f>10*LOG10(10^((O18+O53)/10)+10^((O53-O58)/10)*(10^((O43+Network!K277)/10)-1))</f>
+        <v>10.185774337262743</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A75" s="166" t="s">
+        <v>311</v>
+      </c>
+      <c r="F75" s="183">
+        <f>F32-F69-10*LOG10(10^((F18+F53)/10)+10^((F53-F58)/10)*(10^((F43+Network!H277)/10)-1))</f>
+        <v>64.239502856522833</v>
+      </c>
+      <c r="G75" s="90">
+        <f>G32-G69-10*LOG10(10^((G18+G53)/10)+10^((G53-G58)/10)*(10^((G43+Network!I277)/10)-1))</f>
+        <v>47.83166705469916</v>
+      </c>
+      <c r="H75" s="90">
+        <f>H32-H69-10*LOG10(10^((H18+H53)/10)+10^((H53-H58)/10)*(10^((H43+Network!J277)/10)-1))</f>
+        <v>33.126245913145226</v>
+      </c>
+      <c r="I75" s="90">
+        <f>I32-I69-10*LOG10(10^((I18+I53)/10)+10^((I53-I58)/10)*(10^((I43+Network!J277)/10)-1))</f>
+        <v>33.617331815259533</v>
+      </c>
+      <c r="J75" s="90">
+        <f>J32-J69-10*LOG10(10^((J18+J53)/10)+10^((J53-J58)/10)*(10^((J43+Network!J277)/10)-1))</f>
+        <v>33.617331815259533</v>
+      </c>
+      <c r="K75" s="90">
+        <f>K32-K69-10*LOG10(10^((K18+K53)/10)+10^((K53-K58)/10)*(10^((K43+Network!J277)/10)-1))</f>
+        <v>34.107351797779984</v>
+      </c>
+      <c r="L75" s="90">
+        <f>L32-L69-10*LOG10(10^((L18+L53)/10)+10^((L53-L58)/10)*(10^((L43+Network!J277)/10)-1))</f>
+        <v>34.518054146923753</v>
+      </c>
+      <c r="M75" s="90">
+        <f>M32-M69-10*LOG10(10^((M18+M53)/10)+10^((M53-M58)/10)*(10^((K43+Network!O277)/10)-1))</f>
+        <v>35.119959601026046</v>
+      </c>
+      <c r="N75" s="90">
+        <f>N32-N69-10*LOG10(10^((N18+N53)/10)+10^((N53-N58)/10)*(10^((K43+Network!P277)/10)-1))</f>
+        <v>35.619998352365812</v>
+      </c>
+      <c r="O75" s="185">
+        <f>O32-O69-10*LOG10(10^((O18+O53)/10)+10^((O53-O58)/10)*(10^((K43+Network!Q277)/10)-1))</f>
+        <v>36.119997925751548</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="167" t="s">
+        <v>312</v>
+      </c>
+      <c r="F76" s="180" t="str">
+        <f>IF(F75&gt;=F70,"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="G76" s="181" t="str">
+        <f t="shared" ref="G76:O76" si="9">IF(G75&gt;=G70,"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="H76" s="181" t="str">
+        <f t="shared" si="9"/>
+        <v>OK</v>
+      </c>
+      <c r="I76" s="181" t="str">
+        <f t="shared" si="9"/>
+        <v>OK</v>
+      </c>
+      <c r="J76" s="181" t="str">
+        <f t="shared" si="9"/>
+        <v>OK</v>
+      </c>
+      <c r="K76" s="181" t="str">
+        <f t="shared" si="9"/>
+        <v>OK</v>
+      </c>
+      <c r="L76" s="181" t="str">
+        <f t="shared" si="9"/>
+        <v>OK</v>
+      </c>
+      <c r="M76" s="181" t="str">
+        <f t="shared" si="9"/>
+        <v>OK</v>
+      </c>
+      <c r="N76" s="181" t="str">
+        <f t="shared" si="9"/>
+        <v>OK</v>
+      </c>
+      <c r="O76" s="182" t="str">
+        <f t="shared" si="9"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="78" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="195" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A79" s="166" t="s">
+        <v>310</v>
+      </c>
+      <c r="F79" s="149">
+        <f>10*LOG10(10^(F26/10)+(10^(F53/10)-1)/10^(F63/10)+(10^(F18/10)-1)*10^(F53/10)/10^(F63/10)+10^((F53-F62-F63)/10)*(10^((F43+Network!H277)/10)-1))</f>
+        <v>18.760497143477167</v>
+      </c>
+      <c r="G79" s="150">
+        <f>10*LOG10(10^(G26/10)+(10^(G53/10)-1)/10^(G63/10)+(10^(G18/10)-1)*10^(G53/10)/10^(G63/10)+10^((G53-G62-G63)/10)*(10^((G43+Network!I277)/10)-1))</f>
+        <v>13.16833294530084</v>
+      </c>
+      <c r="H79" s="150">
+        <f>10*LOG10(10^(H26/10)+(10^(H53/10)-1)/10^(H63/10)+(10^(H18/10)-1)*10^(H53/10)/10^(H63/10)+10^((H53-H62-H63)/10)*(10^((H43+Network!J277)/10)-1))</f>
+        <v>6.8320999204318209</v>
+      </c>
+      <c r="I79" s="150">
+        <f>10*LOG10(10^(I26/10)+(10^(I53/10)-1)/10^(I63/10)+(10^(I18/10)-1)*10^(I53/10)/10^(I63/10)+10^((I53-I62-I63)/10)*(10^((I43+Network!J277)/10)-1))</f>
+        <v>6.8291404634264445</v>
+      </c>
+      <c r="J79" s="150">
+        <f>10*LOG10(10^(J26/10)+(10^(J53/10)-1)/10^(J63/10)+(10^(J18/10)-1)*10^(J53/10)/10^(J63/10)+10^((J53-J62-J63)/10)*(10^((J43+Network!J277)/10)-1))</f>
+        <v>6.8291404634264445</v>
+      </c>
+      <c r="K79" s="150">
+        <f>10*LOG10(10^(K26/10)+(10^(K53/10)-1)/10^(K63/10)+(10^(K18/10)-1)*10^(K53/10)/10^(K63/10)+10^((K53-K62-K63)/10)*(10^((K43+Network!J277)/10)-1))</f>
+        <v>6.8265010427752344</v>
+      </c>
+      <c r="L79" s="150">
+        <f>10*LOG10(10^(L26/10)+(10^(L53/10)-1)/10^(L63/10)+(10^(L18/10)-1)*10^(L53/10)/10^(L63/10)+10^((L53-L62-L63)/10)*(10^((L43+Network!J277)/10)-1))</f>
+        <v>6.8245058343871996</v>
+      </c>
+      <c r="M79" s="150">
+        <f>10*LOG10(10^(M26/10)+(10^(M53/10)-1)/10^(M63/10)+(10^(M18/10)-1)*10^(M53/10)/10^(M63/10)+10^((M53-M62-M63)/10)*(10^((M43+Network!K277)/10)-1))</f>
+        <v>7.1552128873363943</v>
+      </c>
+      <c r="N79" s="150">
+        <f>10*LOG10(10^(N26/10)+(10^(N53/10)-1)/10^(N63/10)+(10^(N18/10)-1)*10^(N53/10)/10^(N63/10)+10^((N53-N62-N63)/10)*(10^((N43+Network!K277)/10)-1))</f>
+        <v>7.1534471129647628</v>
+      </c>
+      <c r="O79" s="151">
+        <f>10*LOG10(10^(O26/10)+(10^(O53/10)-1)/10^(O63/10)+(10^(O18/10)-1)*10^(O53/10)/10^(O63/10)+10^((O53-O62-O63)/10)*(10^((O43+Network!K277)/10)-1))</f>
+        <v>7.1518726109406714</v>
+      </c>
+      <c r="P79" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A80" s="166" t="s">
+        <v>311</v>
+      </c>
+      <c r="F80" s="183">
+        <f>F32-F69-10*LOG10(10^(F26/10)+(10^(F53/10)-1)/10^(F63/10)+(10^(F18/10)-1)*10^(F53/10)/10^(F63/10)+10^((F53-F62-F63)/10)*(10^((F43+Network!H277)/10)-1))</f>
+        <v>64.239502856522833</v>
+      </c>
+      <c r="G80" s="90">
+        <f>G32-G69-10*LOG10(10^(G26/10)+(10^(G53/10)-1)/10^(G63/10)+(10^(G18/10)-1)*10^(G53/10)/10^(G63/10)+10^((G53-G62-G63)/10)*(10^((G43+Network!I277)/10)-1))</f>
+        <v>47.83166705469916</v>
+      </c>
+      <c r="H80" s="90">
+        <f>H32-H69-10*LOG10(10^(H26/10)+(10^(H53/10)-1)/10^(H63/10)+(10^(H18/10)-1)*10^(H53/10)/10^(H63/10)+10^((H53-H62-H63)/10)*(10^((H43+Network!J277)/10)-1))</f>
+        <v>39.167900079568177</v>
+      </c>
+      <c r="I80" s="90">
+        <f>I32-I69-10*LOG10(10^(I26/10)+(10^(I53/10)-1)/10^(I63/10)+(10^(I18/10)-1)*10^(I53/10)/10^(I63/10)+10^((I53-I62-I63)/10)*(10^((I43+Network!J277)/10)-1))</f>
+        <v>39.170859536573559</v>
+      </c>
+      <c r="J80" s="90">
+        <f>J32-J69-10*LOG10(10^(J26/10)+(10^(J53/10)-1)/10^(J63/10)+(10^(J18/10)-1)*10^(J53/10)/10^(J63/10)+10^((J53-J62-J63)/10)*(10^((J43+Network!J277)/10)-1))</f>
+        <v>39.170859536573559</v>
+      </c>
+      <c r="K80" s="90">
+        <f>K32-K69-10*LOG10(10^(K26/10)+(10^(K53/10)-1)/10^(K63/10)+(10^(K18/10)-1)*10^(K53/10)/10^(K63/10)+10^((K53-K62-K63)/10)*(10^((K43+Network!J277)/10)-1))</f>
+        <v>39.173498957224766</v>
+      </c>
+      <c r="L80" s="90">
+        <f>L32-L69-10*LOG10(10^(L26/10)+(10^(L53/10)-1)/10^(L63/10)+(10^(L18/10)-1)*10^(L53/10)/10^(L63/10)+10^((L53-L62-L63)/10)*(10^((L43+Network!J277)/10)-1))</f>
+        <v>39.175494165612804</v>
+      </c>
+      <c r="M80" s="90">
+        <f>M32-M69-10*LOG10(10^(M26/10)+(10^(M53/10)-1)/10^(M63/10)+(10^(M18/10)-1)*10^(M53/10)/10^(M63/10)+10^((M53-M62-M63)/10)*(10^((M43+Network!K277)/10)-1))</f>
+        <v>38.844787112663603</v>
+      </c>
+      <c r="N80" s="90">
+        <f>N32-N69-10*LOG10(10^(N26/10)+(10^(N53/10)-1)/10^(N63/10)+(10^(N18/10)-1)*10^(N53/10)/10^(N63/10)+10^((N53-N62-N63)/10)*(10^((N43+Network!K277)/10)-1))</f>
+        <v>38.846552887035237</v>
+      </c>
+      <c r="O80" s="185">
+        <f>O32-O69-10*LOG10(10^(O26/10)+(10^(O53/10)-1)/10^(O63/10)+(10^(O18/10)-1)*10^(O53/10)/10^(O63/10)+10^((O53-O62-O63)/10)*(10^((O43+Network!K277)/10)-1))</f>
+        <v>38.848127389059329</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="167" t="s">
+        <v>313</v>
+      </c>
+      <c r="F81" s="180" t="str">
+        <f>IF(F80&gt;=F70,"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="G81" s="181" t="str">
+        <f t="shared" ref="G81:O81" si="10">IF(G80&gt;=G70,"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="H81" s="181" t="str">
+        <f t="shared" si="10"/>
+        <v>OK</v>
+      </c>
+      <c r="I81" s="181" t="str">
+        <f t="shared" si="10"/>
+        <v>OK</v>
+      </c>
+      <c r="J81" s="181" t="str">
+        <f t="shared" si="10"/>
+        <v>OK</v>
+      </c>
+      <c r="K81" s="181" t="str">
+        <f t="shared" si="10"/>
+        <v>OK</v>
+      </c>
+      <c r="L81" s="181" t="str">
+        <f t="shared" si="10"/>
+        <v>OK</v>
+      </c>
+      <c r="M81" s="181" t="str">
+        <f t="shared" si="10"/>
+        <v>OK</v>
+      </c>
+      <c r="N81" s="181" t="str">
+        <f t="shared" si="10"/>
+        <v>OK</v>
+      </c>
+      <c r="O81" s="182" t="str">
+        <f t="shared" si="10"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="85" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="140" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A80" s="171" t="s">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A86" s="165" t="s">
         <v>284</v>
       </c>
-      <c r="F80" s="155">
+      <c r="F86" s="149">
         <v>30</v>
       </c>
-      <c r="G80" s="156">
+      <c r="G86" s="150">
         <v>16</v>
       </c>
-      <c r="H80" s="156">
+      <c r="H86" s="150">
         <v>1</v>
       </c>
-      <c r="I80" s="156">
+      <c r="I86" s="150">
         <v>2</v>
       </c>
-      <c r="J80" s="156">
+      <c r="J86" s="150">
         <v>2</v>
       </c>
-      <c r="K80" s="156">
+      <c r="K86" s="150">
         <v>1</v>
       </c>
-      <c r="L80" s="156">
+      <c r="L86" s="150">
         <v>1</v>
       </c>
-      <c r="M80" s="156">
+      <c r="M86" s="150">
         <v>1</v>
       </c>
-      <c r="N80" s="156">
+      <c r="N86" s="150">
         <v>1</v>
       </c>
-      <c r="O80" s="156">
+      <c r="O86" s="150">
         <v>1</v>
       </c>
-      <c r="P80" s="157">
+      <c r="P86" s="151">
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="172" t="s">
+    <row r="87" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="166" t="s">
         <v>285</v>
       </c>
-      <c r="F81" s="175">
-        <f>7.5*LOG10((F80-1))</f>
+      <c r="F87" s="169">
+        <f>7.5*LOG10((F86-1))</f>
         <v>10.96798498424217</v>
       </c>
-      <c r="G81" s="176">
-        <f>7.5*LOG10(G80-1)</f>
+      <c r="G87" s="170">
+        <f>7.5*LOG10(G86-1)</f>
         <v>8.8206844429176101</v>
       </c>
-      <c r="H81" s="163">
+      <c r="H87" s="157">
         <v>0</v>
       </c>
-      <c r="I81" s="163">
-        <f>7.5*LOG10(I80-1)</f>
+      <c r="I87" s="157">
+        <f>7.5*LOG10(I86-1)</f>
         <v>0</v>
       </c>
-      <c r="J81" s="163">
-        <f>7.5*LOG10(J80-1)</f>
+      <c r="J87" s="157">
+        <f>7.5*LOG10(J86-1)</f>
         <v>0</v>
       </c>
-      <c r="K81" s="163">
+      <c r="K87" s="157">
         <v>0</v>
       </c>
-      <c r="L81" s="163">
+      <c r="L87" s="157">
         <v>0</v>
       </c>
-      <c r="M81" s="163">
+      <c r="M87" s="157">
         <v>0</v>
       </c>
-      <c r="N81" s="163">
+      <c r="N87" s="157">
         <v>0</v>
       </c>
-      <c r="O81" s="163">
+      <c r="O87" s="157">
         <v>0</v>
       </c>
-      <c r="P81" s="177">
-        <f t="shared" ref="K81:P81" si="2">7.5*LOG10(P80-1)</f>
+      <c r="P87" s="171">
+        <f t="shared" ref="P87" si="11">7.5*LOG10(P86-1)</f>
         <v>10.96798498424217</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="173" t="s">
+    <row r="88" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="167" t="s">
         <v>286</v>
       </c>
-      <c r="H82" s="158">
+      <c r="H88" s="152">
         <v>30</v>
       </c>
-      <c r="I82" s="159">
+      <c r="I88" s="153">
         <v>30</v>
       </c>
-      <c r="J82" s="159">
+      <c r="J88" s="153">
         <v>30</v>
       </c>
-      <c r="K82" s="159">
+      <c r="K88" s="153">
         <v>30</v>
       </c>
-      <c r="L82" s="159">
+      <c r="L88" s="153">
         <v>30</v>
       </c>
-      <c r="M82" s="159">
+      <c r="M88" s="153">
         <v>30</v>
       </c>
-      <c r="N82" s="159">
+      <c r="N88" s="153">
         <v>30</v>
       </c>
-      <c r="O82" s="159">
+      <c r="O88" s="153">
         <v>30</v>
       </c>
-      <c r="P82" s="160">
+      <c r="P88" s="154">
         <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A90" s="195" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A91" s="172" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="139" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A94" s="195" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A95" s="166" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A96" s="172" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="139" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -13787,16 +14842,16 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="32"/>
-      <c r="B2" s="139" t="s">
+      <c r="B2" s="189" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="140"/>
+      <c r="C2" s="190"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="118"/>

</xml_diff>

<commit_message>
CTI acabada a falta de revisión
</commit_message>
<xml_diff>
--- a/3C/ITSIT/CTI3.xlsx
+++ b/3C/ITSIT/CTI3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upvedues-my.sharepoint.com/personal/cribella_upv_edu_es/Documents/6-1/ITSIT/Trabajo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="695" documentId="11_AA5C2796D14A585BA2449CEF5E30AD8D88D2DDCB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{776C1050-FA1C-4FD6-A824-12D7802EBF2C}"/>
+  <xr:revisionPtr revIDLastSave="745" documentId="11_AA5C2796D14A585BA2449CEF5E30AD8D88D2DDCB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{791C70DE-19BB-4459-A970-F2EAEFC92140}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Network" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="321">
   <si>
     <t>TECHNICAL CHARACTERISTICS OF ELEMENTS FROM CATALOGUE</t>
   </si>
@@ -2334,6 +2334,18 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2349,21 +2361,9 @@
     <xf numFmtId="0" fontId="3" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -2696,18 +2696,18 @@
       <selection activeCell="F178" sqref="F178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2748,13 +2748,13 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -2894,8 +2894,8 @@
         <v>7.8E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>57</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>74</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>65</v>
       </c>
@@ -3038,16 +3038,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="30"/>
     </row>
-    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="53" t="s">
         <v>58</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="54" t="s">
         <v>159</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>5.335</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="55" t="s">
         <v>158</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="55" t="s">
         <v>157</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="55" t="s">
         <v>187</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>3.0350000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="56" t="s">
         <v>156</v>
       </c>
@@ -3302,12 +3302,12 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="52"/>
       <c r="N24" s="91"/>
       <c r="O24" s="91"/>
     </row>
-    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="54" t="s">
         <v>155</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>5.335</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="55" t="s">
         <v>154</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="55" t="s">
         <v>153</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="55" t="s">
         <v>188</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>3.0350000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="56" t="s">
         <v>152</v>
       </c>
@@ -3530,12 +3530,12 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="52"/>
       <c r="N30" s="91"/>
       <c r="O30" s="91"/>
     </row>
-    <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="54" t="s">
         <v>127</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>4.3000000000000007</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="55" t="s">
         <v>126</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="55" t="s">
         <v>125</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="55" t="s">
         <v>124</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>6.6000000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="55" t="s">
         <v>194</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="56" t="s">
         <v>123</v>
       </c>
@@ -3803,12 +3803,12 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="52"/>
       <c r="N37" s="91"/>
       <c r="O37" s="91"/>
     </row>
-    <row r="38" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="54" t="s">
         <v>122</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>4.3000000000000007</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="55" t="s">
         <v>121</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="55" t="s">
         <v>120</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="55" t="s">
         <v>119</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>6.6000000000000005</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="55" t="s">
         <v>194</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="56" t="s">
         <v>118</v>
       </c>
@@ -4075,12 +4075,12 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="52"/>
       <c r="N44" s="91"/>
       <c r="O44" s="91"/>
     </row>
-    <row r="45" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="54" t="s">
         <v>151</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>5.335</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="55" t="s">
         <v>150</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="55" t="s">
         <v>149</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="55" t="s">
         <v>189</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>3.0350000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="56" t="s">
         <v>148</v>
       </c>
@@ -4303,12 +4303,12 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="52"/>
       <c r="N50" s="91"/>
       <c r="O50" s="91"/>
     </row>
-    <row r="51" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="54" t="s">
         <v>147</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>5.335</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="55" t="s">
         <v>146</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="55" t="s">
         <v>145</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="55" t="s">
         <v>190</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>3.0350000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="56" t="s">
         <v>144</v>
       </c>
@@ -4531,12 +4531,12 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="52"/>
       <c r="N56" s="91"/>
       <c r="O56" s="91"/>
     </row>
-    <row r="57" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="54" t="s">
         <v>117</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>4.3000000000000007</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="55" t="s">
         <v>116</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="55" t="s">
         <v>115</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="55" t="s">
         <v>114</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>6.6000000000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="55" t="s">
         <v>195</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="56" t="s">
         <v>113</v>
       </c>
@@ -4803,12 +4803,12 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="52"/>
       <c r="N63" s="91"/>
       <c r="O63" s="91"/>
     </row>
-    <row r="64" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="54" t="s">
         <v>112</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>4.3000000000000007</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="55" t="s">
         <v>111</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="55" t="s">
         <v>110</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="55" t="s">
         <v>109</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="55" t="s">
         <v>194</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="56" t="s">
         <v>108</v>
       </c>
@@ -5075,12 +5075,12 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="52"/>
       <c r="N70" s="91"/>
       <c r="O70" s="91"/>
     </row>
-    <row r="71" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="54" t="s">
         <v>143</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>5.335</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="55" t="s">
         <v>142</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="55" t="s">
         <v>141</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="55" t="s">
         <v>140</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>3.0350000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="56" t="s">
         <v>139</v>
       </c>
@@ -5303,12 +5303,12 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="52"/>
       <c r="N76" s="91"/>
       <c r="O76" s="91"/>
     </row>
-    <row r="77" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="54" t="s">
         <v>138</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>5.335</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="55" t="s">
         <v>137</v>
       </c>
@@ -5399,7 +5399,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="55" t="s">
         <v>136</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="55" t="s">
         <v>191</v>
       </c>
@@ -5487,7 +5487,7 @@
         <v>3.0350000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="56" t="s">
         <v>135</v>
       </c>
@@ -5531,12 +5531,12 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="52"/>
       <c r="N82" s="91"/>
       <c r="O82" s="91"/>
     </row>
-    <row r="83" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="54" t="s">
         <v>107</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>4.3000000000000007</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="55" t="s">
         <v>106</v>
       </c>
@@ -5627,7 +5627,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="55" t="s">
         <v>105</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="55" t="s">
         <v>104</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>6.6000000000000005</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="55" t="s">
         <v>196</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="56" t="s">
         <v>103</v>
       </c>
@@ -5819,7 +5819,7 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="52"/>
       <c r="B89" s="52"/>
       <c r="C89" s="52"/>
@@ -5835,7 +5835,7 @@
       <c r="N89" s="91"/>
       <c r="O89" s="91"/>
     </row>
-    <row r="90" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="54" t="s">
         <v>102</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>4.3000000000000007</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="55" t="s">
         <v>101</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="92" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="55" t="s">
         <v>100</v>
       </c>
@@ -5977,7 +5977,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="93" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="55" t="s">
         <v>99</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="94" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="55" t="s">
         <v>196</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="95" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="56" t="s">
         <v>98</v>
       </c>
@@ -6109,11 +6109,11 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="96" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N96" s="92"/>
       <c r="O96" s="92"/>
     </row>
-    <row r="97" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="54" t="s">
         <v>134</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>5.335</v>
       </c>
     </row>
-    <row r="98" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="55" t="s">
         <v>133</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="99" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="55" t="s">
         <v>132</v>
       </c>
@@ -6248,7 +6248,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="100" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="55" t="s">
         <v>192</v>
       </c>
@@ -6292,7 +6292,7 @@
         <v>3.0350000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="56" t="s">
         <v>131</v>
       </c>
@@ -6336,11 +6336,11 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="102" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N102" s="92"/>
       <c r="O102" s="92"/>
     </row>
-    <row r="103" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="54" t="s">
         <v>130</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>5.335</v>
       </c>
     </row>
-    <row r="104" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="55" t="s">
         <v>129</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="105" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="55" t="s">
         <v>128</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="106" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="55" t="s">
         <v>193</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>3.0350000000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="56" t="s">
         <v>97</v>
       </c>
@@ -6563,11 +6563,11 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="108" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N108" s="92"/>
       <c r="O108" s="92"/>
     </row>
-    <row r="109" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="54" t="s">
         <v>96</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>4.3000000000000007</v>
       </c>
     </row>
-    <row r="110" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="55" t="s">
         <v>95</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="111" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="55" t="s">
         <v>94</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="112" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="55" t="s">
         <v>93</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>6.6000000000000005</v>
       </c>
     </row>
-    <row r="113" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="55" t="s">
         <v>197</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="114" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="56" t="s">
         <v>92</v>
       </c>
@@ -6834,11 +6834,11 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="115" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N115" s="92"/>
       <c r="O115" s="92"/>
     </row>
-    <row r="116" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="54" t="s">
         <v>91</v>
       </c>
@@ -6885,7 +6885,7 @@
         <v>4.3000000000000007</v>
       </c>
     </row>
-    <row r="117" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="55" t="s">
         <v>90</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="118" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="55" t="s">
         <v>89</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="119" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="55" t="s">
         <v>88</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>6.6000000000000005</v>
       </c>
     </row>
-    <row r="120" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="55" t="s">
         <v>197</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="121" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="56" t="s">
         <v>87</v>
       </c>
@@ -7105,11 +7105,11 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="122" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N122" s="92"/>
       <c r="O122" s="92"/>
     </row>
-    <row r="123" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="54" t="s">
         <v>62</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>3.7250000000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="55" t="s">
         <v>63</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>4.1850000000000005</v>
       </c>
     </row>
-    <row r="125" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="56" t="s">
         <v>64</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="126" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B126"/>
       <c r="C126"/>
       <c r="D126"/>
@@ -7261,7 +7261,7 @@
       <c r="K126"/>
       <c r="L126"/>
     </row>
-    <row r="127" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127"/>
       <c r="C127"/>
       <c r="D127"/>
@@ -7274,7 +7274,7 @@
       <c r="K127"/>
       <c r="L127"/>
     </row>
-    <row r="128" spans="1:15" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:15" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B128"/>
       <c r="C128"/>
       <c r="D128"/>
@@ -7287,7 +7287,7 @@
       <c r="K128"/>
       <c r="L128"/>
     </row>
-    <row r="129" spans="1:13" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:13" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="64" t="s">
         <v>10</v>
       </c>
@@ -7307,7 +7307,7 @@
       <c r="K129"/>
       <c r="L129"/>
     </row>
-    <row r="130" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="26" t="s">
         <v>13</v>
       </c>
@@ -7342,7 +7342,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="131" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="27" t="s">
         <v>20</v>
       </c>
@@ -7379,7 +7379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="24"/>
       <c r="B132" s="22" t="s">
         <v>36</v>
@@ -7414,7 +7414,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="36" t="s">
         <v>34</v>
       </c>
@@ -7449,7 +7449,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="37"/>
       <c r="B134" s="35" t="s">
         <v>38</v>
@@ -7482,7 +7482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="38" t="s">
         <v>39</v>
       </c>
@@ -7517,7 +7517,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="39"/>
       <c r="B136" s="35" t="s">
         <v>41</v>
@@ -7550,7 +7550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="38" t="s">
         <v>42</v>
       </c>
@@ -7585,7 +7585,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="39"/>
       <c r="B138" s="35" t="s">
         <v>44</v>
@@ -7618,7 +7618,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="38" t="s">
         <v>24</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="39"/>
       <c r="B140" s="35" t="s">
         <v>14</v>
@@ -7686,7 +7686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="38" t="s">
         <v>27</v>
       </c>
@@ -7721,7 +7721,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="39"/>
       <c r="B142" s="35" t="s">
         <v>26</v>
@@ -7754,8 +7754,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="145" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="145" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="12" t="s">
         <v>15</v>
       </c>
@@ -7763,7 +7763,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="33" t="s">
         <v>29</v>
       </c>
@@ -7779,7 +7779,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="47" t="s">
         <v>56</v>
       </c>
@@ -7817,7 +7817,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="48"/>
       <c r="B148" s="35" t="s">
         <v>36</v>
@@ -7850,7 +7850,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="33" t="s">
         <v>29</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="47" t="s">
         <v>34</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="25"/>
       <c r="B151" s="35" t="s">
         <v>38</v>
@@ -7965,7 +7965,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="33" t="s">
         <v>29</v>
       </c>
@@ -8009,7 +8009,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="47" t="s">
         <v>34</v>
       </c>
@@ -8047,7 +8047,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="48"/>
       <c r="B154" s="35" t="s">
         <v>38</v>
@@ -8081,7 +8081,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="33" t="s">
         <v>29</v>
       </c>
@@ -8125,7 +8125,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="47" t="s">
         <v>39</v>
       </c>
@@ -8163,7 +8163,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="34"/>
       <c r="B157" s="35" t="s">
         <v>41</v>
@@ -8197,7 +8197,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="33" t="s">
         <v>29</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="47" t="s">
         <v>27</v>
       </c>
@@ -8279,7 +8279,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="48"/>
       <c r="B160" s="35" t="s">
         <v>26</v>
@@ -8313,7 +8313,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="33" t="s">
         <v>17</v>
       </c>
@@ -8357,7 +8357,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="74" t="s">
         <v>16</v>
       </c>
@@ -8391,8 +8391,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="166" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="166" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="13" t="s">
         <v>19</v>
       </c>
@@ -8424,7 +8424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="54" t="s">
         <v>86</v>
       </c>
@@ -8465,7 +8465,7 @@
         <v>9.625</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="55" t="s">
         <v>85</v>
       </c>
@@ -8506,7 +8506,7 @@
         <v>9.2850000000000001</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="56" t="s">
         <v>84</v>
       </c>
@@ -8547,8 +8547,8 @@
         <v>10.129999999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="171" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="171" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="54" t="s">
         <v>159</v>
       </c>
@@ -8589,7 +8589,7 @@
         <v>9.5350000000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="55" t="s">
         <v>158</v>
       </c>
@@ -8630,7 +8630,7 @@
         <v>9.1900000000000013</v>
       </c>
     </row>
-    <row r="173" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="55" t="s">
         <v>157</v>
       </c>
@@ -8671,7 +8671,7 @@
         <v>8.73</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="55" t="s">
         <v>160</v>
       </c>
@@ -8712,7 +8712,7 @@
         <v>7.2350000000000003</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="56" t="s">
         <v>156</v>
       </c>
@@ -8753,10 +8753,10 @@
         <v>8.9600000000000009</v>
       </c>
     </row>
-    <row r="176" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="52"/>
     </row>
-    <row r="177" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="54" t="s">
         <v>155</v>
       </c>
@@ -8797,7 +8797,7 @@
         <v>9.5350000000000001</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="55" t="s">
         <v>154</v>
       </c>
@@ -8838,7 +8838,7 @@
         <v>8.73</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="55" t="s">
         <v>153</v>
       </c>
@@ -8879,7 +8879,7 @@
         <v>8.73</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="55" t="s">
         <v>161</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>7.2350000000000003</v>
       </c>
     </row>
-    <row r="181" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="56" t="s">
         <v>152</v>
       </c>
@@ -8961,10 +8961,10 @@
         <v>8.9600000000000009</v>
       </c>
     </row>
-    <row r="182" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="52"/>
     </row>
-    <row r="183" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="54" t="s">
         <v>127</v>
       </c>
@@ -9005,7 +9005,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="55" t="s">
         <v>126</v>
       </c>
@@ -9046,7 +9046,7 @@
         <v>10.57</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="55" t="s">
         <v>125</v>
       </c>
@@ -9087,7 +9087,7 @@
         <v>8.3850000000000016</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="55" t="s">
         <v>124</v>
       </c>
@@ -9128,7 +9128,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="55" t="s">
         <v>162</v>
       </c>
@@ -9169,7 +9169,7 @@
         <v>8.3850000000000016</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="56" t="s">
         <v>123</v>
       </c>
@@ -9210,10 +9210,10 @@
         <v>7.35</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="52"/>
     </row>
-    <row r="190" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="54" t="s">
         <v>122</v>
       </c>
@@ -9254,7 +9254,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="55" t="s">
         <v>121</v>
       </c>
@@ -9295,7 +9295,7 @@
         <v>10.57</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="55" t="s">
         <v>120</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>8.3850000000000016</v>
       </c>
     </row>
-    <row r="193" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="55" t="s">
         <v>119</v>
       </c>
@@ -9377,7 +9377,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="194" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="55" t="s">
         <v>162</v>
       </c>
@@ -9418,7 +9418,7 @@
         <v>8.3850000000000016</v>
       </c>
     </row>
-    <row r="195" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="56" t="s">
         <v>118</v>
       </c>
@@ -9459,10 +9459,10 @@
         <v>7.35</v>
       </c>
     </row>
-    <row r="196" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="52"/>
     </row>
-    <row r="197" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="54" t="s">
         <v>151</v>
       </c>
@@ -9503,7 +9503,7 @@
         <v>8.7349999999999994</v>
       </c>
     </row>
-    <row r="198" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="55" t="s">
         <v>150</v>
       </c>
@@ -9544,7 +9544,7 @@
         <v>8.39</v>
       </c>
     </row>
-    <row r="199" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="55" t="s">
         <v>149</v>
       </c>
@@ -9585,7 +9585,7 @@
         <v>7.9300000000000006</v>
       </c>
     </row>
-    <row r="200" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="55" t="s">
         <v>163</v>
       </c>
@@ -9626,7 +9626,7 @@
         <v>6.4350000000000005</v>
       </c>
     </row>
-    <row r="201" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="56" t="s">
         <v>148</v>
       </c>
@@ -9667,10 +9667,10 @@
         <v>8.16</v>
       </c>
     </row>
-    <row r="202" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="52"/>
     </row>
-    <row r="203" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="54" t="s">
         <v>147</v>
       </c>
@@ -9711,7 +9711,7 @@
         <v>8.7349999999999994</v>
       </c>
     </row>
-    <row r="204" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="55" t="s">
         <v>146</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>7.9300000000000006</v>
       </c>
     </row>
-    <row r="205" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="55" t="s">
         <v>145</v>
       </c>
@@ -9793,7 +9793,7 @@
         <v>7.9300000000000006</v>
       </c>
     </row>
-    <row r="206" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="55" t="s">
         <v>164</v>
       </c>
@@ -9834,7 +9834,7 @@
         <v>6.4350000000000005</v>
       </c>
     </row>
-    <row r="207" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="56" t="s">
         <v>144</v>
       </c>
@@ -9875,10 +9875,10 @@
         <v>8.16</v>
       </c>
     </row>
-    <row r="208" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="52"/>
     </row>
-    <row r="209" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="54" t="s">
         <v>117</v>
       </c>
@@ -9919,7 +9919,7 @@
         <v>7.7000000000000011</v>
       </c>
     </row>
-    <row r="210" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="55" t="s">
         <v>116</v>
       </c>
@@ -9960,7 +9960,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="211" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="55" t="s">
         <v>115</v>
       </c>
@@ -10001,7 +10001,7 @@
         <v>7.5850000000000009</v>
       </c>
     </row>
-    <row r="212" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="55" t="s">
         <v>114</v>
       </c>
@@ -10042,7 +10042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="55" t="s">
         <v>165</v>
       </c>
@@ -10083,7 +10083,7 @@
         <v>7.5850000000000009</v>
       </c>
     </row>
-    <row r="214" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="56" t="s">
         <v>113</v>
       </c>
@@ -10124,10 +10124,10 @@
         <v>6.5500000000000007</v>
       </c>
     </row>
-    <row r="215" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="52"/>
     </row>
-    <row r="216" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="54" t="s">
         <v>112</v>
       </c>
@@ -10168,7 +10168,7 @@
         <v>7.7000000000000011</v>
       </c>
     </row>
-    <row r="217" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="55" t="s">
         <v>111</v>
       </c>
@@ -10209,7 +10209,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="218" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="55" t="s">
         <v>110</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>7.5850000000000009</v>
       </c>
     </row>
-    <row r="219" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="55" t="s">
         <v>109</v>
       </c>
@@ -10291,7 +10291,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="220" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="55" t="s">
         <v>165</v>
       </c>
@@ -10332,7 +10332,7 @@
         <v>7.5850000000000009</v>
       </c>
     </row>
-    <row r="221" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="56" t="s">
         <v>108</v>
       </c>
@@ -10373,10 +10373,10 @@
         <v>6.5500000000000007</v>
       </c>
     </row>
-    <row r="222" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="52"/>
     </row>
-    <row r="223" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="54" t="s">
         <v>143</v>
       </c>
@@ -10417,7 +10417,7 @@
         <v>7.9350000000000005</v>
       </c>
     </row>
-    <row r="224" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="55" t="s">
         <v>142</v>
       </c>
@@ -10458,7 +10458,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="225" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="55" t="s">
         <v>141</v>
       </c>
@@ -10499,7 +10499,7 @@
         <v>7.1300000000000008</v>
       </c>
     </row>
-    <row r="226" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="55" t="s">
         <v>140</v>
       </c>
@@ -10540,7 +10540,7 @@
         <v>5.6349999999999998</v>
       </c>
     </row>
-    <row r="227" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="56" t="s">
         <v>139</v>
       </c>
@@ -10581,10 +10581,10 @@
         <v>7.3599999999999994</v>
       </c>
     </row>
-    <row r="228" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="52"/>
     </row>
-    <row r="229" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="54" t="s">
         <v>138</v>
       </c>
@@ -10625,7 +10625,7 @@
         <v>7.9350000000000005</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="55" t="s">
         <v>137</v>
       </c>
@@ -10666,7 +10666,7 @@
         <v>7.1300000000000008</v>
       </c>
     </row>
-    <row r="231" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="55" t="s">
         <v>136</v>
       </c>
@@ -10707,7 +10707,7 @@
         <v>7.1300000000000008</v>
       </c>
     </row>
-    <row r="232" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="55" t="s">
         <v>166</v>
       </c>
@@ -10748,7 +10748,7 @@
         <v>5.6349999999999998</v>
       </c>
     </row>
-    <row r="233" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="56" t="s">
         <v>135</v>
       </c>
@@ -10789,10 +10789,10 @@
         <v>7.3599999999999994</v>
       </c>
     </row>
-    <row r="234" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="52"/>
     </row>
-    <row r="235" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="54" t="s">
         <v>107</v>
       </c>
@@ -10833,7 +10833,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="236" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="55" t="s">
         <v>106</v>
       </c>
@@ -10874,7 +10874,7 @@
         <v>8.9700000000000006</v>
       </c>
     </row>
-    <row r="237" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="55" t="s">
         <v>105</v>
       </c>
@@ -10915,7 +10915,7 @@
         <v>6.7850000000000001</v>
       </c>
     </row>
-    <row r="238" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="55" t="s">
         <v>104</v>
       </c>
@@ -10956,7 +10956,7 @@
         <v>9.2000000000000011</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="55" t="s">
         <v>167</v>
       </c>
@@ -10997,7 +10997,7 @@
         <v>6.7850000000000001</v>
       </c>
     </row>
-    <row r="240" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="56" t="s">
         <v>103</v>
       </c>
@@ -11038,10 +11038,10 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="241" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="52"/>
     </row>
-    <row r="242" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="54" t="s">
         <v>102</v>
       </c>
@@ -11082,7 +11082,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="243" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="55" t="s">
         <v>101</v>
       </c>
@@ -11123,7 +11123,7 @@
         <v>8.9700000000000006</v>
       </c>
     </row>
-    <row r="244" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="55" t="s">
         <v>100</v>
       </c>
@@ -11164,7 +11164,7 @@
         <v>6.7850000000000001</v>
       </c>
     </row>
-    <row r="245" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="55" t="s">
         <v>99</v>
       </c>
@@ -11205,7 +11205,7 @@
         <v>8.9700000000000006</v>
       </c>
     </row>
-    <row r="246" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="55" t="s">
         <v>167</v>
       </c>
@@ -11246,7 +11246,7 @@
         <v>6.7850000000000001</v>
       </c>
     </row>
-    <row r="247" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="56" t="s">
         <v>98</v>
       </c>
@@ -11287,10 +11287,10 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="248" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="52"/>
     </row>
-    <row r="249" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="54" t="s">
         <v>134</v>
       </c>
@@ -11331,7 +11331,7 @@
         <v>7.1349999999999998</v>
       </c>
     </row>
-    <row r="250" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="55" t="s">
         <v>133</v>
       </c>
@@ -11372,7 +11372,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="251" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="55" t="s">
         <v>132</v>
       </c>
@@ -11413,7 +11413,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="252" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="55" t="s">
         <v>168</v>
       </c>
@@ -11454,7 +11454,7 @@
         <v>4.835</v>
       </c>
     </row>
-    <row r="253" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="56" t="s">
         <v>131</v>
       </c>
@@ -11495,10 +11495,10 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="254" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="52"/>
     </row>
-    <row r="255" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="54" t="s">
         <v>130</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>7.1349999999999998</v>
       </c>
     </row>
-    <row r="256" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="55" t="s">
         <v>129</v>
       </c>
@@ -11580,7 +11580,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="257" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="55" t="s">
         <v>128</v>
       </c>
@@ -11621,7 +11621,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="258" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="55" t="s">
         <v>169</v>
       </c>
@@ -11662,7 +11662,7 @@
         <v>4.835</v>
       </c>
     </row>
-    <row r="259" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="56" t="s">
         <v>97</v>
       </c>
@@ -11703,10 +11703,10 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="260" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="52"/>
     </row>
-    <row r="261" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="54" t="s">
         <v>96</v>
       </c>
@@ -11747,7 +11747,7 @@
         <v>6.1000000000000005</v>
       </c>
     </row>
-    <row r="262" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="55" t="s">
         <v>95</v>
       </c>
@@ -11788,7 +11788,7 @@
         <v>8.17</v>
       </c>
     </row>
-    <row r="263" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="55" t="s">
         <v>94</v>
       </c>
@@ -11829,7 +11829,7 @@
         <v>5.9850000000000003</v>
       </c>
     </row>
-    <row r="264" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="55" t="s">
         <v>93</v>
       </c>
@@ -11870,7 +11870,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="265" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="55" t="s">
         <v>170</v>
       </c>
@@ -11911,7 +11911,7 @@
         <v>5.9850000000000003</v>
       </c>
     </row>
-    <row r="266" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="56" t="s">
         <v>92</v>
       </c>
@@ -11952,10 +11952,10 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="267" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="52"/>
     </row>
-    <row r="268" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="54" t="s">
         <v>91</v>
       </c>
@@ -11996,7 +11996,7 @@
         <v>6.1000000000000005</v>
       </c>
     </row>
-    <row r="269" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="55" t="s">
         <v>90</v>
       </c>
@@ -12037,7 +12037,7 @@
         <v>8.17</v>
       </c>
     </row>
-    <row r="270" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="55" t="s">
         <v>89</v>
       </c>
@@ -12078,7 +12078,7 @@
         <v>5.9850000000000003</v>
       </c>
     </row>
-    <row r="271" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="55" t="s">
         <v>88</v>
       </c>
@@ -12119,7 +12119,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="272" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="55" t="s">
         <v>170</v>
       </c>
@@ -12160,7 +12160,7 @@
         <v>5.9850000000000003</v>
       </c>
     </row>
-    <row r="273" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="56" t="s">
         <v>87</v>
       </c>
@@ -12201,11 +12201,11 @@
         <v>4.95</v>
       </c>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A274" s="52"/>
     </row>
-    <row r="275" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="276" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="276" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A276" s="54" t="s">
         <v>77</v>
       </c>
@@ -12246,7 +12246,7 @@
         <v>4.835</v>
       </c>
     </row>
-    <row r="277" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="56" t="s">
         <v>78</v>
       </c>
@@ -12287,23 +12287,23 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="279" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="280" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="280" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="C280" s="186" t="s">
+      <c r="C280" s="190" t="s">
         <v>198</v>
       </c>
-      <c r="D280" s="187"/>
-      <c r="E280" s="188"/>
-      <c r="G280" s="186" t="s">
+      <c r="D280" s="191"/>
+      <c r="E280" s="192"/>
+      <c r="G280" s="190" t="s">
         <v>199</v>
       </c>
-      <c r="H280" s="187"/>
-      <c r="I280" s="188"/>
-    </row>
-    <row r="281" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H280" s="191"/>
+      <c r="I280" s="192"/>
+    </row>
+    <row r="281" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="81" t="s">
         <v>83</v>
       </c>
@@ -12326,7 +12326,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="282" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="79" t="s">
         <v>80</v>
       </c>
@@ -12355,7 +12355,7 @@
         <v>2.8019999999999996</v>
       </c>
     </row>
-    <row r="283" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="78" t="s">
         <v>81</v>
       </c>
@@ -12384,7 +12384,7 @@
         <v>4.2000000000000028</v>
       </c>
     </row>
-    <row r="284" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="78" t="s">
         <v>82</v>
       </c>
@@ -12413,8 +12413,8 @@
         <v>19.460000000000008</v>
       </c>
     </row>
-    <row r="286" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="287" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="287" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C287" s="140" t="s">
         <v>252</v>
       </c>
@@ -12422,7 +12422,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="288" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A288" s="114" t="s">
         <v>172</v>
       </c>
@@ -12435,7 +12435,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C289" s="83" t="s">
         <v>171</v>
       </c>
@@ -12443,18 +12443,18 @@
         <v>171</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="291" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="291" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A291" s="114" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="292" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="78" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="293" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C293" s="141" t="s">
         <v>49</v>
       </c>
@@ -12468,7 +12468,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="138" t="s">
         <v>256</v>
       </c>
@@ -12485,7 +12485,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="295" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="139" t="s">
         <v>257</v>
       </c>
@@ -12502,13 +12502,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="296" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="297" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="297" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="140" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="138" t="s">
         <v>259</v>
       </c>
@@ -12529,7 +12529,7 @@
         <v>104.52500000000001</v>
       </c>
     </row>
-    <row r="299" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="139" t="s">
         <v>260</v>
       </c>
@@ -12550,8 +12550,8 @@
         <v>105.26300000000001</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="135" t="s">
         <v>261</v>
       </c>
@@ -12572,7 +12572,7 @@
         <v>105.07849999999999</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="135" t="s">
         <v>262</v>
       </c>
@@ -12589,7 +12589,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="303" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>263</v>
       </c>
@@ -12606,22 +12606,22 @@
         <v>270</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="305" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="306" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="140" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="138" t="s">
         <v>77</v>
       </c>
@@ -12630,7 +12630,7 @@
         <v>51.489999999999995</v>
       </c>
     </row>
-    <row r="308" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A308" s="139" t="s">
         <v>78</v>
       </c>
@@ -12657,17 +12657,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" customWidth="1"/>
-    <col min="9" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" customWidth="1"/>
+    <col min="9" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>47</v>
       </c>
@@ -12709,7 +12709,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
@@ -12751,17 +12751,17 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="72" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="73" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="70" t="s">
         <v>53</v>
       </c>
@@ -12802,15 +12802,15 @@
         <v>293</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32"/>
     </row>
-    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="73" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="70" t="s">
         <v>71</v>
       </c>
@@ -12818,7 +12818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>72</v>
       </c>
@@ -12826,7 +12826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>73</v>
       </c>
@@ -12855,7 +12855,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>203</v>
       </c>
@@ -12863,7 +12863,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>204</v>
       </c>
@@ -12871,18 +12871,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H13" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="101" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>174</v>
       </c>
@@ -12923,7 +12923,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>175</v>
       </c>
@@ -12961,7 +12961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>176</v>
       </c>
@@ -12999,7 +12999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>177</v>
       </c>
@@ -13037,7 +13037,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>178</v>
       </c>
@@ -13075,13 +13075,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="101" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>174</v>
       </c>
@@ -13110,7 +13110,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>175</v>
       </c>
@@ -13139,7 +13139,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>176</v>
       </c>
@@ -13168,7 +13168,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>180</v>
       </c>
@@ -13197,7 +13197,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>178</v>
       </c>
@@ -13226,13 +13226,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="105" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="107" t="s">
         <v>182</v>
       </c>
@@ -13267,7 +13267,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="107" t="s">
         <v>183</v>
       </c>
@@ -13302,7 +13302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="107" t="s">
         <v>184</v>
       </c>
@@ -13347,7 +13347,7 @@
         <v>60.0331979307064</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="107" t="s">
         <v>185</v>
       </c>
@@ -13382,7 +13382,7 @@
         <v>60.73</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="109" t="s">
         <v>186</v>
       </c>
@@ -13417,8 +13417,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="141" t="s">
         <v>278</v>
       </c>
@@ -13426,12 +13426,12 @@
         <v>279</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="140" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="138" t="s">
         <v>275</v>
       </c>
@@ -13480,7 +13480,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="166" t="s">
         <v>276</v>
       </c>
@@ -13518,7 +13518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="166" t="s">
         <v>277</v>
       </c>
@@ -13573,7 +13573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="172" t="s">
         <v>280</v>
       </c>
@@ -13622,7 +13622,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="166" t="s">
         <v>281</v>
       </c>
@@ -13671,57 +13671,57 @@
         <v>113.03201501575784</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="139" t="s">
         <v>282</v>
       </c>
       <c r="F46" s="180" t="str">
-        <f>IF(F44&lt;=(F19-F87),"OK","NO")</f>
+        <f t="shared" ref="F46:P46" si="3">IF(F44&lt;=(F19-F87),"OK","NO")</f>
         <v>NO</v>
       </c>
       <c r="G46" s="181" t="str">
-        <f>IF(G44&lt;=(G19-G87),"OK","NO")</f>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="H46" s="181" t="str">
-        <f>IF(H44&lt;=(H19-H87),"OK","NO")</f>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="I46" s="181" t="str">
-        <f>IF(I44&lt;=(I19-I87),"OK","NO")</f>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="J46" s="181" t="str">
-        <f>IF(J44&lt;=(J19-J87),"OK","NO")</f>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="K46" s="181" t="str">
-        <f>IF(K44&lt;=(K19-K87),"OK","NO")</f>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="L46" s="181" t="str">
-        <f>IF(L44&lt;=(L19-L87),"OK","NO")</f>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="M46" s="181" t="str">
-        <f>IF(M44&lt;=(M19-M87),"OK","NO")</f>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="N46" s="181" t="str">
-        <f>IF(N44&lt;=(N19-N87),"OK","NO")</f>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="O46" s="191" t="str">
-        <f>IF(O44&lt;=(O19-O87),"OK","NO")</f>
+      <c r="O46" s="186" t="str">
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
       <c r="P46" s="182" t="str">
-        <f>IF(P44&lt;=(P19-P87),"OK","NO")</f>
+        <f t="shared" si="3"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="140" t="s">
         <v>288</v>
       </c>
@@ -13729,7 +13729,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="165" t="s">
         <v>289</v>
       </c>
@@ -13764,7 +13764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="166" t="s">
         <v>290</v>
       </c>
@@ -13781,27 +13781,27 @@
         <v>0.8</v>
       </c>
       <c r="I50" s="21">
-        <f t="shared" ref="I50:N50" si="3">I5*I49</f>
+        <f t="shared" ref="I50:N50" si="4">I5*I49</f>
         <v>0.8</v>
       </c>
       <c r="J50" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
       <c r="K50" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
       <c r="L50" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.88</v>
       </c>
       <c r="M50" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.88</v>
       </c>
       <c r="N50" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.88</v>
       </c>
       <c r="O50" s="164">
@@ -13809,7 +13809,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="166" t="s">
         <v>276</v>
       </c>
@@ -13844,7 +13844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="166" t="s">
         <v>277</v>
       </c>
@@ -13895,153 +13895,153 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="166" t="s">
         <v>291</v>
       </c>
       <c r="F53" s="161">
-        <f>F52+F50</f>
+        <f t="shared" ref="F53:O53" si="5">F52+F50</f>
         <v>2.7</v>
       </c>
       <c r="G53" s="21">
-        <f>G52+G50</f>
+        <f t="shared" si="5"/>
         <v>2.58</v>
       </c>
       <c r="H53" s="21">
-        <f>H52+H50</f>
+        <f t="shared" si="5"/>
         <v>3.8</v>
       </c>
       <c r="I53" s="21">
-        <f>I52+I50</f>
+        <f t="shared" si="5"/>
         <v>3.3</v>
       </c>
       <c r="J53" s="21">
-        <f>J52+J50</f>
+        <f t="shared" si="5"/>
         <v>3.3</v>
       </c>
       <c r="K53" s="21">
-        <f>K52+K50</f>
+        <f t="shared" si="5"/>
         <v>2.8</v>
       </c>
       <c r="L53" s="21">
-        <f>L52+L50</f>
+        <f t="shared" si="5"/>
         <v>2.38</v>
       </c>
       <c r="M53" s="21">
-        <f>M52+M50</f>
+        <f t="shared" si="5"/>
         <v>1.88</v>
       </c>
       <c r="N53" s="21">
-        <f>N52+N50</f>
+        <f t="shared" si="5"/>
         <v>1.38</v>
       </c>
       <c r="O53" s="164">
-        <f>O52+O50</f>
+        <f t="shared" si="5"/>
         <v>0.88</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="167" t="s">
         <v>292</v>
       </c>
       <c r="F54" s="152">
-        <f>F32-F53</f>
+        <f t="shared" ref="F54:O54" si="6">F32-F53</f>
         <v>67.3</v>
       </c>
       <c r="G54" s="153">
-        <f>G32-G53</f>
+        <f t="shared" si="6"/>
         <v>55.42</v>
       </c>
       <c r="H54" s="153">
-        <f>H32-H53</f>
+        <f t="shared" si="6"/>
         <v>46.2</v>
       </c>
       <c r="I54" s="153">
-        <f>I32-I53</f>
+        <f t="shared" si="6"/>
         <v>46.7</v>
       </c>
       <c r="J54" s="153">
-        <f>J32-J53</f>
+        <f t="shared" si="6"/>
         <v>46.7</v>
       </c>
       <c r="K54" s="153">
-        <f>K32-K53</f>
+        <f t="shared" si="6"/>
         <v>47.2</v>
       </c>
       <c r="L54" s="153">
-        <f>L32-L53</f>
+        <f t="shared" si="6"/>
         <v>47.62</v>
       </c>
       <c r="M54" s="153">
-        <f>M32-M53</f>
+        <f t="shared" si="6"/>
         <v>48.12</v>
       </c>
       <c r="N54" s="153">
-        <f>N32-N53</f>
+        <f t="shared" si="6"/>
         <v>48.62</v>
       </c>
       <c r="O54" s="154">
-        <f>O32-O53</f>
+        <f t="shared" si="6"/>
         <v>49.12</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="56" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="140" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="165" t="s">
         <v>297</v>
       </c>
-      <c r="F58" s="192">
+      <c r="F58" s="149">
         <f>F44-(F32-F53)</f>
         <v>32.100000000000009</v>
       </c>
-      <c r="G58" s="193">
+      <c r="G58" s="150">
         <f>G44-(G32-G53)</f>
         <v>41.679999999999993</v>
       </c>
-      <c r="H58" s="193">
+      <c r="H58" s="150">
         <f>H44-(H32-H53)</f>
         <v>57.8</v>
       </c>
-      <c r="I58" s="193">
+      <c r="I58" s="150">
         <f>I44-(I32-I53)</f>
         <v>56.8</v>
       </c>
-      <c r="J58" s="193">
+      <c r="J58" s="150">
         <f>J44-(J32-J53)</f>
         <v>56.8</v>
       </c>
-      <c r="K58" s="193">
-        <f t="shared" ref="K58:O58" si="4">K44-(K32-K53)</f>
+      <c r="K58" s="150">
+        <f t="shared" ref="K58:O58" si="7">K44-(K32-K53)</f>
         <v>55.8</v>
       </c>
-      <c r="L58" s="193">
-        <f t="shared" si="4"/>
+      <c r="L58" s="150">
+        <f t="shared" si="7"/>
         <v>54.88</v>
       </c>
-      <c r="M58" s="193">
-        <f t="shared" si="4"/>
+      <c r="M58" s="150">
+        <f t="shared" si="7"/>
         <v>53.88</v>
       </c>
-      <c r="N58" s="193">
-        <f t="shared" si="4"/>
+      <c r="N58" s="150">
+        <f t="shared" si="7"/>
         <v>52.88</v>
       </c>
-      <c r="O58" s="194">
-        <f t="shared" si="4"/>
+      <c r="O58" s="151">
+        <f t="shared" si="7"/>
         <v>51.88</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="167" t="s">
         <v>298</v>
       </c>
@@ -14050,49 +14050,49 @@
         <v>OK</v>
       </c>
       <c r="G59" s="181" t="str">
-        <f t="shared" ref="G59:O59" si="5">IF(AND(G16&gt;G58,(G16-G17)&lt;G58),"OK","NO")</f>
+        <f t="shared" ref="G59:O59" si="8">IF(AND(G16&gt;G58,(G16-G17)&lt;G58),"OK","NO")</f>
         <v>OK</v>
       </c>
       <c r="H59" s="181" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>NO</v>
       </c>
       <c r="I59" s="181" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>NO</v>
       </c>
       <c r="J59" s="181" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>NO</v>
       </c>
       <c r="K59" s="181" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>NO</v>
       </c>
       <c r="L59" s="181" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>NO</v>
       </c>
       <c r="M59" s="181" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>NO</v>
       </c>
       <c r="N59" s="181" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>NO</v>
       </c>
       <c r="O59" s="182" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="140" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="165" t="s">
         <v>300</v>
       </c>
@@ -14101,11 +14101,11 @@
         <v>32.100000000000009</v>
       </c>
       <c r="G62" s="150">
-        <f t="shared" ref="G62:O62" si="6">IF(G58-G24&gt;G16-G17,G58-G24,G16-G17)</f>
+        <f t="shared" ref="G62:O62" si="9">IF(G58-G24&gt;G16-G17,G58-G24,G16-G17)</f>
         <v>41.679999999999993</v>
       </c>
       <c r="H62" s="150">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>29.799999999999997</v>
       </c>
       <c r="I62" s="150">
@@ -14113,31 +14113,31 @@
         <v>28.799999999999997</v>
       </c>
       <c r="J62" s="150">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>28.799999999999997</v>
       </c>
       <c r="K62" s="150">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>27.799999999999997</v>
       </c>
       <c r="L62" s="150">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>26.880000000000003</v>
       </c>
       <c r="M62" s="150">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>25.880000000000003</v>
       </c>
       <c r="N62" s="150">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>24.880000000000003</v>
       </c>
       <c r="O62" s="151">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>23.880000000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="166" t="s">
         <v>301</v>
       </c>
@@ -14146,7 +14146,7 @@
         <v>0</v>
       </c>
       <c r="G63" s="21">
-        <f t="shared" ref="G63:O63" si="7">G58-G62</f>
+        <f t="shared" ref="G63:O63" si="10">G58-G62</f>
         <v>0</v>
       </c>
       <c r="H63" s="21">
@@ -14154,38 +14154,38 @@
         <v>28</v>
       </c>
       <c r="I63" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="J63" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="K63" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="L63" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="M63" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="N63" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="O63" s="164">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="P63" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="167" t="s">
         <v>302</v>
       </c>
@@ -14194,49 +14194,49 @@
         <v>OK</v>
       </c>
       <c r="G64" s="181" t="str">
-        <f t="shared" ref="G64:O64" si="8">IF(AND(G16&gt;G62,(G16-G17)&lt;G62),"OK","NO")</f>
+        <f t="shared" ref="G64:O64" si="11">IF(AND(G16&gt;G62,(G16-G17)&lt;G62),"OK","NO")</f>
         <v>OK</v>
       </c>
       <c r="H64" s="181" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="I64" s="181" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="J64" s="181" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="K64" s="181" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="L64" s="181" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="M64" s="181" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="N64" s="181" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
       <c r="O64" s="182" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="66" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="195" t="s">
+    <row r="65" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="187" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="166" t="s">
         <v>305</v>
       </c>
@@ -14271,7 +14271,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="166" t="s">
         <v>306</v>
       </c>
@@ -14306,7 +14306,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="166" t="s">
         <v>307</v>
       </c>
@@ -14341,7 +14341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="167" t="s">
         <v>308</v>
       </c>
@@ -14376,18 +14376,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A72" s="196" t="s">
+    <row r="71" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="188" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="197" t="s">
+    <row r="73" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="189" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="166" t="s">
         <v>310</v>
       </c>
@@ -14435,7 +14435,7 @@
         <v>10.185774337262743</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="166" t="s">
         <v>311</v>
       </c>
@@ -14480,7 +14480,7 @@
         <v>36.119997925751548</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="167" t="s">
         <v>312</v>
       </c>
@@ -14489,49 +14489,49 @@
         <v>OK</v>
       </c>
       <c r="G76" s="181" t="str">
-        <f t="shared" ref="G76:O76" si="9">IF(G75&gt;=G70,"OK","NO")</f>
+        <f t="shared" ref="G76:O76" si="12">IF(G75&gt;=G70,"OK","NO")</f>
         <v>OK</v>
       </c>
       <c r="H76" s="181" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>OK</v>
       </c>
       <c r="I76" s="181" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>OK</v>
       </c>
       <c r="J76" s="181" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>OK</v>
       </c>
       <c r="K76" s="181" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>OK</v>
       </c>
       <c r="L76" s="181" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>OK</v>
       </c>
       <c r="M76" s="181" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>OK</v>
       </c>
       <c r="N76" s="181" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>OK</v>
       </c>
       <c r="O76" s="182" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="78" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="195" t="s">
+    <row r="77" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="187" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="166" t="s">
         <v>310</v>
       </c>
@@ -14579,7 +14579,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="166" t="s">
         <v>311</v>
       </c>
@@ -14624,7 +14624,7 @@
         <v>38.848127389059329</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="167" t="s">
         <v>313</v>
       </c>
@@ -14633,49 +14633,49 @@
         <v>OK</v>
       </c>
       <c r="G81" s="181" t="str">
-        <f t="shared" ref="G81:O81" si="10">IF(G80&gt;=G70,"OK","NO")</f>
+        <f t="shared" ref="G81:O81" si="13">IF(G80&gt;=G70,"OK","NO")</f>
         <v>OK</v>
       </c>
       <c r="H81" s="181" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>OK</v>
       </c>
       <c r="I81" s="181" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>OK</v>
       </c>
       <c r="J81" s="181" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>OK</v>
       </c>
       <c r="K81" s="181" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>OK</v>
       </c>
       <c r="L81" s="181" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>OK</v>
       </c>
       <c r="M81" s="181" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>OK</v>
       </c>
       <c r="N81" s="181" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>OK</v>
       </c>
       <c r="O81" s="182" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="85" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="140" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="165" t="s">
         <v>284</v>
       </c>
@@ -14713,7 +14713,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="166" t="s">
         <v>285</v>
       </c>
@@ -14752,11 +14752,11 @@
         <v>0</v>
       </c>
       <c r="P87" s="171">
-        <f t="shared" ref="P87" si="11">7.5*LOG10(P86-1)</f>
+        <f t="shared" ref="P87" si="14">7.5*LOG10(P86-1)</f>
         <v>10.96798498424217</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="167" t="s">
         <v>286</v>
       </c>
@@ -14788,41 +14788,204 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A90" s="195" t="s">
+    <row r="89" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="187" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="172" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="92" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H91" s="176">
+        <f>H28+2*(H27-H87-H44)</f>
+        <v>39</v>
+      </c>
+      <c r="I91" s="178">
+        <f t="shared" ref="I91:O91" si="15">I28+2*(I27-H87-I44)</f>
+        <v>40</v>
+      </c>
+      <c r="J91" s="178">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="K91" s="178">
+        <f t="shared" si="15"/>
+        <v>41</v>
+      </c>
+      <c r="L91" s="178">
+        <f t="shared" si="15"/>
+        <v>42</v>
+      </c>
+      <c r="M91" s="178">
+        <f t="shared" si="15"/>
+        <v>43</v>
+      </c>
+      <c r="N91" s="178">
+        <f t="shared" si="15"/>
+        <v>44</v>
+      </c>
+      <c r="O91" s="179">
+        <f t="shared" si="15"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="139" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="93" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A94" s="195" t="s">
+      <c r="H92" s="180" t="str">
+        <f>IF(H91&gt;=H88,"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="I92" s="181" t="str">
+        <f t="shared" ref="I92:O92" si="16">IF(I91&gt;=I88,"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="J92" s="181" t="str">
+        <f t="shared" si="16"/>
+        <v>OK</v>
+      </c>
+      <c r="K92" s="181" t="str">
+        <f t="shared" si="16"/>
+        <v>OK</v>
+      </c>
+      <c r="L92" s="181" t="str">
+        <f t="shared" si="16"/>
+        <v>OK</v>
+      </c>
+      <c r="M92" s="181" t="str">
+        <f t="shared" si="16"/>
+        <v>OK</v>
+      </c>
+      <c r="N92" s="181" t="str">
+        <f t="shared" si="16"/>
+        <v>OK</v>
+      </c>
+      <c r="O92" s="182" t="str">
+        <f t="shared" si="16"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="187" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="166" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H95" s="149">
+        <f>H32+H63</f>
+        <v>78</v>
+      </c>
+      <c r="I95" s="150">
+        <f t="shared" ref="I95:O95" si="17">I32+I63</f>
+        <v>78</v>
+      </c>
+      <c r="J95" s="150">
+        <f t="shared" si="17"/>
+        <v>78</v>
+      </c>
+      <c r="K95" s="150">
+        <f t="shared" si="17"/>
+        <v>78</v>
+      </c>
+      <c r="L95" s="150">
+        <f t="shared" si="17"/>
+        <v>78</v>
+      </c>
+      <c r="M95" s="150">
+        <f t="shared" si="17"/>
+        <v>78</v>
+      </c>
+      <c r="N95" s="150">
+        <f t="shared" si="17"/>
+        <v>78</v>
+      </c>
+      <c r="O95" s="151">
+        <f t="shared" si="17"/>
+        <v>78</v>
+      </c>
+      <c r="P95" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="172" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H96" s="196">
+        <f>-20*LOG10(10^(-H91/20)+10^(-(H28+2*(H27-7.5*LOG10(SUM(H86:O86)-1)-H32-H63))/20))</f>
+        <v>38.887363993059452</v>
+      </c>
+      <c r="I96" s="195">
+        <f>-20*LOG10(10^(-I91/20)+10^(-(I28+2*(I27-7.5*LOG10(SUM(H86:O86)-1)-I32-I63))/20))</f>
+        <v>39.873719771667787</v>
+      </c>
+      <c r="J96" s="195">
+        <f>-20*LOG10(10^(-J91/20)+10^(-(J28+2*(J27-7.5*LOG10(SUM(H86:O86)-1)-J32-J63))/20))</f>
+        <v>39.873719771667787</v>
+      </c>
+      <c r="K96" s="195">
+        <f>-20*LOG10(10^(-K91/20)+10^(-(K28+2*(K27-7.5*LOG10(SUM(H86:O86)-1)-K32-K63))/20))</f>
+        <v>40.858436175609853</v>
+      </c>
+      <c r="L96" s="195">
+        <f>-20*LOG10(10^(-L91/20)+10^(-(L28+2*(L27-7.5*LOG10(SUM(H86:O86)-1)-L32-L63))/20))</f>
+        <v>41.841319653175255</v>
+      </c>
+      <c r="M96" s="195">
+        <f>-20*LOG10(10^(-M91/20)+10^(-(M28+2*(M27-7.5*LOG10(SUM(H86:O86)-1)-M32-M63))/20))</f>
+        <v>42.822154668419266</v>
+      </c>
+      <c r="N96" s="195">
+        <f>-20*LOG10(10^(-N91/20)+10^(-(N28+2*(N27-7.5*LOG10(SUM(H86:O86)-1)-N32-N63))/20))</f>
+        <v>43.800701423044323</v>
+      </c>
+      <c r="O96" s="197">
+        <f>-20*LOG10(10^(-O91/20)+10^(-(O28+2*(O27-7.5*LOG10(SUM(H86:O86)-1)-O32-O63))/20))</f>
+        <v>44.776693397722497</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="139" t="s">
         <v>320</v>
+      </c>
+      <c r="H97" s="180" t="str">
+        <f>IF(H96&gt;=H88,"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="I97" s="181" t="str">
+        <f t="shared" ref="I97:O97" si="18">IF(I96&gt;=I88,"OK","NO")</f>
+        <v>OK</v>
+      </c>
+      <c r="J97" s="181" t="str">
+        <f t="shared" si="18"/>
+        <v>OK</v>
+      </c>
+      <c r="K97" s="181" t="str">
+        <f t="shared" si="18"/>
+        <v>OK</v>
+      </c>
+      <c r="L97" s="181" t="str">
+        <f t="shared" si="18"/>
+        <v>OK</v>
+      </c>
+      <c r="M97" s="181" t="str">
+        <f t="shared" si="18"/>
+        <v>OK</v>
+      </c>
+      <c r="N97" s="181" t="str">
+        <f t="shared" si="18"/>
+        <v>OK</v>
+      </c>
+      <c r="O97" s="182" t="str">
+        <f t="shared" si="18"/>
+        <v>OK</v>
       </c>
     </row>
   </sheetData>
@@ -14839,21 +15002,21 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="32"/>
-      <c r="B2" s="189" t="s">
+      <c r="B2" s="193" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="190"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="194"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="118"/>
       <c r="B3" s="119" t="s">
         <v>206</v>
@@ -14862,7 +15025,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="120" t="s">
         <v>208</v>
       </c>
@@ -14873,7 +15036,7 @@
         <v>39.49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="122" t="s">
         <v>209</v>
       </c>
@@ -14884,7 +15047,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="122" t="s">
         <v>210</v>
       </c>
@@ -14897,7 +15060,7 @@
         <v>-19.559999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="122" t="s">
         <v>211</v>
       </c>
@@ -14908,7 +15071,7 @@
         <v>43.35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="122" t="s">
         <v>212</v>
       </c>
@@ -14919,7 +15082,7 @@
         <v>6378.16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="122" t="s">
         <v>213</v>
       </c>
@@ -14930,7 +15093,7 @@
         <v>35786.300000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="122" t="s">
         <v>214</v>
       </c>
@@ -14941,7 +15104,7 @@
         <v>37780.794999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="122" t="s">
         <v>215</v>
       </c>
@@ -14952,7 +15115,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="122" t="s">
         <v>216</v>
       </c>
@@ -14963,12 +15126,12 @@
         <v>150.81</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="124"/>
       <c r="B13" s="124"/>
       <c r="C13" s="124"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="119" t="s">
         <v>217</v>
       </c>
@@ -14979,7 +15142,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="119" t="s">
         <v>218</v>
       </c>
@@ -14992,12 +15155,12 @@
         <v>-18.147397727373288</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="125"/>
       <c r="B16" s="126"/>
       <c r="C16" s="126"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="119" t="s">
         <v>219</v>
       </c>
@@ -15010,7 +15173,7 @@
         <v>14.22414374543391</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="119" t="s">
         <v>220</v>
       </c>
@@ -15023,7 +15186,7 @@
         <v>20.852602272626712</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="119" t="s">
         <v>221</v>
       </c>
@@ -15034,7 +15197,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="119" t="s">
         <v>222</v>
       </c>
@@ -15045,7 +15208,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="119" t="s">
         <v>223</v>
       </c>
@@ -15058,7 +15221,7 @@
         <v>54.665645956735368</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="119" t="s">
         <v>224</v>
       </c>
@@ -15071,7 +15234,7 @@
         <v>4.8763553571844795</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="119" t="s">
         <v>225</v>
       </c>
@@ -15084,7 +15247,7 @@
         <v>15.976246915442232</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="119" t="s">
         <v>226</v>
       </c>
@@ -15097,12 +15260,12 @@
         <v>27000000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="127"/>
       <c r="B25" s="124"/>
       <c r="C25" s="124"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="119" t="s">
         <v>227</v>
       </c>
@@ -15113,7 +15276,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="130" t="s">
         <v>228</v>
       </c>
@@ -15124,7 +15287,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="130" t="s">
         <v>229</v>
       </c>
@@ -15135,7 +15298,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="130" t="s">
         <v>230</v>
       </c>
@@ -15148,7 +15311,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="130" t="s">
         <v>231</v>
       </c>
@@ -15161,7 +15324,7 @@
         <v>115.96798498424216</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="130" t="s">
         <v>232</v>
       </c>
@@ -15172,7 +15335,7 @@
         <v>118.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="128" t="s">
         <v>240</v>
       </c>
@@ -15183,7 +15346,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="128" t="s">
         <v>233</v>
       </c>
@@ -15194,7 +15357,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="128" t="s">
         <v>239</v>
       </c>
@@ -15205,7 +15368,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="128" t="s">
         <v>238</v>
       </c>
@@ -15216,7 +15379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="128" t="s">
         <v>234</v>
       </c>
@@ -15227,7 +15390,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="128" t="s">
         <v>235</v>
       </c>
@@ -15238,7 +15401,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="128" t="s">
         <v>236</v>
       </c>
@@ -15249,7 +15412,7 @@
         <v>12.75</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="128" t="s">
         <v>241</v>
       </c>
@@ -15262,7 +15425,7 @@
         <v>206.09562554132461</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="128" t="s">
         <v>242</v>
       </c>
@@ -15273,7 +15436,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="128" t="s">
         <v>249</v>
       </c>
@@ -15284,7 +15447,7 @@
         <v>1.3800000000000001E-23</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="128" t="s">
         <v>243</v>
       </c>
@@ -15297,7 +15460,7 @@
         <v>100.72029093246357</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="128" t="s">
         <v>244</v>
       </c>
@@ -15310,7 +15473,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="128" t="s">
         <v>237</v>
       </c>
@@ -15323,7 +15486,7 @@
         <v>-134.25640177870341</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="128" t="s">
         <v>245</v>
       </c>
@@ -15336,7 +15499,7 @@
         <v>39.939223762621197</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="128" t="s">
         <v>246</v>
       </c>
@@ -15349,7 +15512,7 @@
         <v>2.3529411764705882E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="128"/>
       <c r="B50" s="133">
         <f>B48*POWER(10,(B47/20))</f>
@@ -15360,7 +15523,7 @@
         <v>2.3365348234310672</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="128" t="s">
         <v>247</v>
       </c>
@@ -15373,7 +15536,7 @@
         <v>0.8889418761785618</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="128" t="s">
         <v>248</v>
       </c>

</xml_diff>

<commit_message>
Cálculos Mástil + Cambios Satelite
</commit_message>
<xml_diff>
--- a/3C/ITSIT/CTI3.xlsx
+++ b/3C/ITSIT/CTI3.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upvedues-my.sharepoint.com/personal/cribella_upv_edu_es/Documents/6-1/ITSIT/Trabajo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="859" documentId="11_AA5C2796D14A585BA2449CEF5E30AD8D88D2DDCB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52BF5A66-8E80-4E21-8951-A3AA84092000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9576" windowHeight="2760" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Network" sheetId="1" r:id="rId1"/>
     <sheet name="Antenna + Headend" sheetId="2" r:id="rId2"/>
     <sheet name="Satellite" sheetId="3" r:id="rId3"/>
+    <sheet name="Mast + Tower" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="345">
   <si>
     <t>TECHNICAL CHARACTERISTICS OF ELEMENTS FROM CATALOGUE</t>
   </si>
@@ -670,75 +670,6 @@
     <t>Longitud</t>
   </si>
   <si>
-    <t>phi</t>
-  </si>
-  <si>
-    <t>beta</t>
-  </si>
-  <si>
-    <t>Radio Tierra (km)</t>
-  </si>
-  <si>
-    <t>Altura satélite (km)</t>
-  </si>
-  <si>
-    <t>d(km)</t>
-  </si>
-  <si>
-    <t>Elevación</t>
-  </si>
-  <si>
-    <t>Azimut</t>
-  </si>
-  <si>
-    <t>PIRE</t>
-  </si>
-  <si>
-    <t>Vrec_0dBi</t>
-  </si>
-  <si>
-    <t>C/Nout</t>
-  </si>
-  <si>
-    <t>Cin</t>
-  </si>
-  <si>
-    <t>Gpar</t>
-  </si>
-  <si>
-    <t>Ts</t>
-  </si>
-  <si>
-    <t>Te,sis</t>
-  </si>
-  <si>
-    <t>Nin</t>
-  </si>
-  <si>
-    <t>C/Nin</t>
-  </si>
-  <si>
-    <t>Beq</t>
-  </si>
-  <si>
-    <t>C/I(Samp)</t>
-  </si>
-  <si>
-    <t>C/I(Smax)</t>
-  </si>
-  <si>
-    <t>Samp</t>
-  </si>
-  <si>
-    <t>Smax30ch</t>
-  </si>
-  <si>
-    <t>Smax2ch</t>
-  </si>
-  <si>
-    <t>Amp</t>
-  </si>
-  <si>
     <t xml:space="preserve">Offset </t>
   </si>
   <si>
@@ -985,17 +916,175 @@
     <t xml:space="preserve">C28-C29 (MPE4) </t>
   </si>
   <si>
-    <t>D (cm)</t>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>RadioTierra</t>
+  </si>
+  <si>
+    <t>DistGeosta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elevacion </t>
+  </si>
+  <si>
+    <t>Azimuth</t>
+  </si>
+  <si>
+    <t>dist sat-ant</t>
+  </si>
+  <si>
+    <t>Phi</t>
+  </si>
+  <si>
+    <t>Velocidad viento (m/s)</t>
+  </si>
+  <si>
+    <t>Gravedad (m/s2)</t>
+  </si>
+  <si>
+    <t>Area efectiva incidente (m2)</t>
+  </si>
+  <si>
+    <t>Presion Viento (N/m2)</t>
+  </si>
+  <si>
+    <t>Carga Viento (N)</t>
+  </si>
+  <si>
+    <t>altura_mastil (m)</t>
+  </si>
+  <si>
+    <t>coeficiente_viento</t>
+  </si>
+  <si>
+    <t>area_efectiva_viento (m2)</t>
+  </si>
+  <si>
+    <t>AREA EFECTIVA VIENTO EN MASTIL</t>
+  </si>
+  <si>
+    <t>MOMENTO FLECTOR INSTALACION</t>
+  </si>
+  <si>
+    <t>Carga_viento_TDT (N)</t>
+  </si>
+  <si>
+    <t>Distancia_suelo_TDT (m)</t>
+  </si>
+  <si>
+    <t>Carga_viento_DAB (N)</t>
+  </si>
+  <si>
+    <t>Distancia_suelo_DAB (m)</t>
+  </si>
+  <si>
+    <t>Distancia_suelo_FM (m)</t>
+  </si>
+  <si>
+    <t>Carga_viento_SAT1 (N)</t>
+  </si>
+  <si>
+    <t>Distancia_suelo_SAT1 (m)</t>
+  </si>
+  <si>
+    <t>Carga_viento_FM (N)</t>
+  </si>
+  <si>
+    <t>Momento_antenas (N*m)</t>
+  </si>
+  <si>
+    <t>Momento_mastil</t>
+  </si>
+  <si>
+    <t>Momento_total</t>
+  </si>
+  <si>
+    <t>Inecuacion</t>
+  </si>
+  <si>
+    <t>Torre Serie 180</t>
+  </si>
+  <si>
+    <t>Tramo superior</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Es mayor la de antenas, no sirve</t>
+  </si>
+  <si>
+    <t>Mástil</t>
+  </si>
+  <si>
+    <t>EJEMPLO PDF</t>
+  </si>
+  <si>
+    <t>grosor_mastil (m)</t>
+  </si>
+  <si>
+    <t>Area efectiva viento(m2)</t>
+  </si>
+  <si>
+    <t>Momento antena (Nm)</t>
+  </si>
+  <si>
+    <t>carga_viento (N)</t>
+  </si>
+  <si>
+    <t>https://www.televes.com/es/g-041-base-fija-de-atornillar-empotrar.html</t>
+  </si>
+  <si>
+    <t>https://www.televes.com/es/3032-tramo-superior-zinc-rpr.html</t>
+  </si>
+  <si>
+    <t>https://www.televes.com/es/3010-mastil-3m-x-o-45mm-x-espesor-2mm.html</t>
+  </si>
+  <si>
+    <t>Fuerzas laterales (igual a carga_viento)</t>
+  </si>
+  <si>
+    <t>Fuerza total (en sentido opuesto)</t>
+  </si>
+  <si>
+    <t>Carga viento al propio mastil tambien suma</t>
+  </si>
+  <si>
+    <t>Fuerzas verticales (según diapositivas he aproximado los pesos de cada antena)</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Pin (dBW)</t>
+  </si>
+  <si>
+    <t>Vin (uV)</t>
+  </si>
+  <si>
+    <t>Vin_log (dBuV)</t>
+  </si>
+  <si>
+    <t>G_IF</t>
+  </si>
+  <si>
+    <t>D (m)</t>
+  </si>
+  <si>
+    <t>C/N</t>
+  </si>
+  <si>
+    <t>Prx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="179" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1185,12 +1274,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCFE2F3"/>
-        <bgColor rgb="FFCFE2F3"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="58">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1575,46 +1664,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -2223,46 +2272,10 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2292,40 +2305,40 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2336,32 +2349,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2374,8 +2387,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="9" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="9" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2391,24 +2422,32 @@
     <xf numFmtId="0" fontId="3" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -2734,10 +2773,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O308"/>
   <sheetViews>
-    <sheetView topLeftCell="A290" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G308" sqref="G308"/>
     </sheetView>
   </sheetViews>
@@ -12461,10 +12500,10 @@
     <row r="286" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="287" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C287" s="114" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="D287" s="114" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
     </row>
     <row r="288" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12491,33 +12530,33 @@
     <row r="290" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="291" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A291" s="114" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
     </row>
     <row r="292" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A292" s="78" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
     </row>
     <row r="293" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C293" s="140" t="s">
+      <c r="C293" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D293" s="141" t="s">
+      <c r="D293" s="129" t="s">
         <v>50</v>
       </c>
-      <c r="E293" s="141" t="s">
-        <v>254</v>
-      </c>
-      <c r="F293" s="142" t="s">
+      <c r="E293" s="129" t="s">
+        <v>231</v>
+      </c>
+      <c r="F293" s="130" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A294" s="137" t="s">
-        <v>255</v>
-      </c>
-      <c r="C294" s="143">
+      <c r="A294" s="125" t="s">
+        <v>232</v>
+      </c>
+      <c r="C294" s="131">
         <v>40</v>
       </c>
       <c r="D294" s="115">
@@ -12526,71 +12565,71 @@
       <c r="E294" s="115">
         <v>47</v>
       </c>
-      <c r="F294" s="144">
+      <c r="F294" s="132">
         <v>47</v>
       </c>
     </row>
     <row r="295" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A295" s="138" t="s">
-        <v>256</v>
-      </c>
-      <c r="C295" s="145">
+      <c r="A295" s="126" t="s">
+        <v>233</v>
+      </c>
+      <c r="C295" s="133">
         <v>70</v>
       </c>
-      <c r="D295" s="146">
+      <c r="D295" s="134">
         <v>70</v>
       </c>
-      <c r="E295" s="146">
+      <c r="E295" s="134">
         <v>70</v>
       </c>
-      <c r="F295" s="147">
+      <c r="F295" s="135">
         <v>70</v>
       </c>
     </row>
     <row r="296" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="297" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A297" s="139" t="s">
-        <v>257</v>
+      <c r="A297" s="127" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A298" s="137" t="s">
-        <v>258</v>
-      </c>
-      <c r="C298" s="148">
+      <c r="A298" s="125" t="s">
+        <v>235</v>
+      </c>
+      <c r="C298" s="136">
         <f>MAX(H167:H273)+C294</f>
         <v>84.808999999999997</v>
       </c>
-      <c r="D298" s="149">
+      <c r="D298" s="137">
         <f>MAX(I167:I273)+D294</f>
         <v>75.03</v>
       </c>
-      <c r="E298" s="149">
+      <c r="E298" s="137">
         <f>MAX(K167:K273)+E294</f>
         <v>96.51</v>
       </c>
-      <c r="F298" s="150">
+      <c r="F298" s="138">
         <f>MAX(M167:M273)+F294</f>
         <v>104.52500000000001</v>
       </c>
     </row>
     <row r="299" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A299" s="138" t="s">
-        <v>259</v>
-      </c>
-      <c r="C299" s="151">
+      <c r="A299" s="126" t="s">
+        <v>236</v>
+      </c>
+      <c r="C299" s="139">
         <f>MIN(H167:H273)+C295</f>
         <v>104.16200000000001</v>
       </c>
-      <c r="D299" s="152">
+      <c r="D299" s="140">
         <f>MIN(I167:I273)+D295</f>
         <v>104.675</v>
       </c>
-      <c r="E299" s="152">
+      <c r="E299" s="140">
         <f>MIN(K167:K273)+E295</f>
         <v>106.358</v>
       </c>
-      <c r="F299" s="153">
+      <c r="F299" s="141">
         <f>MIN(M167:M273)+F295</f>
         <v>105.26300000000001</v>
       </c>
@@ -12598,30 +12637,30 @@
     <row r="300" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="301" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A301" s="78" t="s">
-        <v>260</v>
-      </c>
-      <c r="C301" s="154">
+        <v>237</v>
+      </c>
+      <c r="C301" s="142">
         <f>0.25*C298+0.75*C299</f>
         <v>99.32374999999999</v>
       </c>
-      <c r="D301" s="155">
+      <c r="D301" s="143">
         <f>0.25*D298+0.75*D299</f>
         <v>97.263749999999987</v>
       </c>
-      <c r="E301" s="149">
+      <c r="E301" s="137">
         <f>0.25*E298+0.75*E299</f>
         <v>103.896</v>
       </c>
-      <c r="F301" s="150">
+      <c r="F301" s="138">
         <f>0.25*F298+0.75*F299</f>
         <v>105.07849999999999</v>
       </c>
     </row>
     <row r="302" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A302" s="78" t="s">
-        <v>261</v>
-      </c>
-      <c r="C302" s="159">
+        <v>238</v>
+      </c>
+      <c r="C302" s="147">
         <v>100</v>
       </c>
       <c r="D302" s="21">
@@ -12630,44 +12669,44 @@
       <c r="E302" s="21">
         <v>104</v>
       </c>
-      <c r="F302" s="160">
+      <c r="F302" s="148">
         <v>105</v>
       </c>
     </row>
     <row r="303" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A303" s="78" t="s">
-        <v>262</v>
-      </c>
-      <c r="C303" s="194" t="s">
-        <v>264</v>
-      </c>
-      <c r="D303" s="195" t="s">
-        <v>265</v>
-      </c>
-      <c r="E303" s="195" t="s">
-        <v>266</v>
-      </c>
-      <c r="F303" s="196" t="s">
-        <v>267</v>
+        <v>239</v>
+      </c>
+      <c r="C303" s="177" t="s">
+        <v>241</v>
+      </c>
+      <c r="D303" s="178" t="s">
+        <v>242</v>
+      </c>
+      <c r="E303" s="178" t="s">
+        <v>243</v>
+      </c>
+      <c r="F303" s="179" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="306" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A306" s="139" t="s">
-        <v>313</v>
+      <c r="A306" s="127" t="s">
+        <v>290</v>
       </c>
       <c r="C306" s="114" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="D306" s="104" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A307" s="137" t="s">
-        <v>311</v>
-      </c>
-      <c r="C307" s="197">
+      <c r="A307" s="125" t="s">
+        <v>288</v>
+      </c>
+      <c r="C307" s="180">
         <f>E302-MAX(G277:K277)</f>
         <v>54.489999999999995</v>
       </c>
@@ -12677,8 +12716,8 @@
       </c>
     </row>
     <row r="308" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A308" s="138" t="s">
-        <v>312</v>
+      <c r="A308" s="126" t="s">
+        <v>289</v>
       </c>
       <c r="C308" s="60">
         <f>E302-MIN(G276:K276)</f>
@@ -12704,11 +12743,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12736,10 +12775,10 @@
         <v>54</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="K1" s="42" t="s">
         <v>66</v>
@@ -12750,7 +12789,7 @@
       <c r="M1" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="135" t="s">
+      <c r="N1" s="123" t="s">
         <v>69</v>
       </c>
       <c r="O1" s="45" t="s">
@@ -12789,7 +12828,7 @@
       <c r="M2" s="44">
         <v>650</v>
       </c>
-      <c r="N2" s="136">
+      <c r="N2" s="124">
         <v>674</v>
       </c>
       <c r="O2" s="46">
@@ -12841,7 +12880,7 @@
         <v>0.23</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12954,7 +12993,7 @@
         <v>50</v>
       </c>
       <c r="Q16" t="s">
-        <v>249</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -13302,8 +13341,8 @@
       <c r="N33" s="106">
         <v>15</v>
       </c>
-      <c r="O33" s="199"/>
-      <c r="P33" s="205"/>
+      <c r="O33" s="182"/>
+      <c r="P33" s="188"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="107" t="s">
@@ -13412,71 +13451,71 @@
     </row>
     <row r="38" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="140" t="s">
-        <v>272</v>
-      </c>
-      <c r="D39" s="142" t="s">
-        <v>273</v>
+      <c r="C39" s="128" t="s">
+        <v>249</v>
+      </c>
+      <c r="D39" s="130" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="139" t="s">
-        <v>250</v>
+      <c r="A40" s="127" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A41" s="137" t="s">
-        <v>269</v>
-      </c>
-      <c r="F41" s="172">
+      <c r="A41" s="125" t="s">
+        <v>246</v>
+      </c>
+      <c r="F41" s="160">
         <f>Network!C302</f>
         <v>100</v>
       </c>
-      <c r="G41" s="173">
+      <c r="G41" s="161">
         <f>Network!D302</f>
         <v>98</v>
       </c>
-      <c r="H41" s="174">
+      <c r="H41" s="162">
         <f>Network!E302</f>
         <v>104</v>
       </c>
-      <c r="I41" s="174">
+      <c r="I41" s="162">
         <f>Network!E302</f>
         <v>104</v>
       </c>
-      <c r="J41" s="174">
+      <c r="J41" s="162">
         <f>Network!E302</f>
         <v>104</v>
       </c>
-      <c r="K41" s="174">
+      <c r="K41" s="162">
         <f>Network!E302</f>
         <v>104</v>
       </c>
-      <c r="L41" s="174">
+      <c r="L41" s="162">
         <f>Network!E302</f>
         <v>104</v>
       </c>
-      <c r="M41" s="174">
+      <c r="M41" s="162">
         <f>Network!E302</f>
         <v>104</v>
       </c>
-      <c r="N41" s="174">
+      <c r="N41" s="162">
         <f>Network!E302</f>
         <v>104</v>
       </c>
-      <c r="O41" s="175">
+      <c r="O41" s="163">
         <f>Network!F302</f>
         <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="162" t="s">
-        <v>270</v>
-      </c>
-      <c r="F42" s="159">
+      <c r="A42" s="150" t="s">
+        <v>247</v>
+      </c>
+      <c r="F42" s="147">
         <v>8</v>
       </c>
-      <c r="G42" s="170">
+      <c r="G42" s="158">
         <v>7</v>
       </c>
       <c r="H42" s="21">
@@ -13500,25 +13539,25 @@
       <c r="N42" s="21">
         <v>0</v>
       </c>
-      <c r="O42" s="160">
+      <c r="O42" s="148">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="162" t="s">
-        <v>271</v>
-      </c>
-      <c r="C43" s="157">
+      <c r="A43" s="150" t="s">
+        <v>248</v>
+      </c>
+      <c r="C43" s="145">
         <v>0.3</v>
       </c>
-      <c r="D43" s="158">
+      <c r="D43" s="146">
         <v>0.5</v>
       </c>
-      <c r="F43" s="159">
+      <c r="F43" s="147">
         <f>F42*C43</f>
         <v>2.4</v>
       </c>
-      <c r="G43" s="170">
+      <c r="G43" s="158">
         <f>G42*C43</f>
         <v>2.1</v>
       </c>
@@ -13550,20 +13589,20 @@
         <f>N42*D43</f>
         <v>0</v>
       </c>
-      <c r="O43" s="160">
+      <c r="O43" s="148">
         <f>O42*D43</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A44" s="168" t="s">
-        <v>274</v>
-      </c>
-      <c r="F44" s="179">
+      <c r="A44" s="156" t="s">
+        <v>251</v>
+      </c>
+      <c r="F44" s="167">
         <f t="shared" ref="F44:O44" si="1">F41+F43</f>
         <v>102.4</v>
       </c>
-      <c r="G44" s="180">
+      <c r="G44" s="168">
         <f t="shared" si="1"/>
         <v>100.1</v>
       </c>
@@ -13595,147 +13634,147 @@
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="O44" s="181">
+      <c r="O44" s="169">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A45" s="162" t="s">
-        <v>275</v>
-      </c>
-      <c r="F45" s="169">
+      <c r="A45" s="150" t="s">
+        <v>252</v>
+      </c>
+      <c r="F45" s="157">
         <f>F19-F87</f>
         <v>99.032015015757835</v>
       </c>
-      <c r="G45" s="171">
+      <c r="G45" s="159">
         <f t="shared" ref="G45:O45" si="2">G19-G87</f>
         <v>101.17931555708239</v>
       </c>
-      <c r="H45" s="164">
+      <c r="H45" s="152">
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="I45" s="164">
+      <c r="I45" s="152">
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="J45" s="164">
+      <c r="J45" s="152">
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="K45" s="164">
+      <c r="K45" s="152">
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="L45" s="164">
+      <c r="L45" s="152">
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="M45" s="164">
+      <c r="M45" s="152">
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="N45" s="164">
+      <c r="N45" s="152">
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="O45" s="167">
+      <c r="O45" s="155">
         <f t="shared" si="2"/>
         <v>113.03201501575784</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="138" t="s">
-        <v>276</v>
-      </c>
-      <c r="F46" s="176" t="str">
+      <c r="A46" s="126" t="s">
+        <v>253</v>
+      </c>
+      <c r="F46" s="164" t="str">
         <f t="shared" ref="F46:O46" si="3">IF(F44&lt;=(F19-F87),"OK","NO")</f>
         <v>NO</v>
       </c>
-      <c r="G46" s="177" t="str">
+      <c r="G46" s="165" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="H46" s="177" t="str">
+      <c r="H46" s="165" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="I46" s="177" t="str">
+      <c r="I46" s="165" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="J46" s="177" t="str">
+      <c r="J46" s="165" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="K46" s="177" t="str">
+      <c r="K46" s="165" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="L46" s="177" t="str">
+      <c r="L46" s="165" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="M46" s="177" t="str">
+      <c r="M46" s="165" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="N46" s="182" t="str">
+      <c r="N46" s="170" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
-      <c r="O46" s="178" t="str">
+      <c r="O46" s="166" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="48" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="139" t="s">
-        <v>281</v>
+      <c r="A48" s="127" t="s">
+        <v>258</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A49" s="161" t="s">
-        <v>282</v>
-      </c>
-      <c r="F49" s="148">
+      <c r="A49" s="149" t="s">
+        <v>259</v>
+      </c>
+      <c r="F49" s="136">
         <v>6</v>
       </c>
-      <c r="G49" s="149">
+      <c r="G49" s="137">
         <v>8</v>
       </c>
-      <c r="H49" s="149">
+      <c r="H49" s="137">
         <v>8</v>
       </c>
-      <c r="I49" s="149">
+      <c r="I49" s="137">
         <v>8</v>
       </c>
-      <c r="J49" s="149">
+      <c r="J49" s="137">
         <v>8</v>
       </c>
-      <c r="K49" s="149">
+      <c r="K49" s="137">
         <v>8</v>
       </c>
-      <c r="L49" s="149">
+      <c r="L49" s="137">
         <v>8</v>
       </c>
-      <c r="M49" s="149">
+      <c r="M49" s="137">
         <v>8</v>
       </c>
-      <c r="N49" s="150">
+      <c r="N49" s="138">
         <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A50" s="162" t="s">
-        <v>283</v>
-      </c>
-      <c r="F50" s="159">
+      <c r="A50" s="150" t="s">
+        <v>260</v>
+      </c>
+      <c r="F50" s="147">
         <f>F5*F49</f>
         <v>0.30000000000000004</v>
       </c>
@@ -13767,16 +13806,16 @@
         <f t="shared" si="4"/>
         <v>0.88</v>
       </c>
-      <c r="N50" s="160">
+      <c r="N50" s="148">
         <f>N5*N49</f>
         <v>0.88</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="162" t="s">
-        <v>270</v>
-      </c>
-      <c r="F51" s="159">
+      <c r="A51" s="150" t="s">
+        <v>247</v>
+      </c>
+      <c r="F51" s="147">
         <v>8</v>
       </c>
       <c r="G51" s="21">
@@ -13800,21 +13839,21 @@
       <c r="M51" s="21">
         <v>1</v>
       </c>
-      <c r="N51" s="160">
+      <c r="N51" s="148">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="162" t="s">
-        <v>271</v>
-      </c>
-      <c r="C52" s="157">
+      <c r="A52" s="150" t="s">
+        <v>248</v>
+      </c>
+      <c r="C52" s="145">
         <v>0.3</v>
       </c>
-      <c r="D52" s="158">
+      <c r="D52" s="146">
         <v>0.5</v>
       </c>
-      <c r="F52" s="159">
+      <c r="F52" s="147">
         <f>C52*F51</f>
         <v>2.4</v>
       </c>
@@ -13846,16 +13885,16 @@
         <f>D52*M51</f>
         <v>0.5</v>
       </c>
-      <c r="N52" s="160">
+      <c r="N52" s="148">
         <f>D52*N51</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A53" s="162" t="s">
-        <v>284</v>
-      </c>
-      <c r="F53" s="159">
+      <c r="A53" s="150" t="s">
+        <v>261</v>
+      </c>
+      <c r="F53" s="147">
         <f t="shared" ref="F53:N53" si="5">F52+F50</f>
         <v>2.7</v>
       </c>
@@ -13887,48 +13926,48 @@
         <f t="shared" si="5"/>
         <v>1.38</v>
       </c>
-      <c r="N53" s="160">
+      <c r="N53" s="148">
         <f t="shared" si="5"/>
         <v>0.88</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="163" t="s">
-        <v>285</v>
-      </c>
-      <c r="F54" s="151">
+      <c r="A54" s="151" t="s">
+        <v>262</v>
+      </c>
+      <c r="F54" s="139">
         <f t="shared" ref="F54:N54" si="6">F32-F53</f>
         <v>67.3</v>
       </c>
-      <c r="G54" s="152">
+      <c r="G54" s="140">
         <f t="shared" si="6"/>
         <v>55.42</v>
       </c>
-      <c r="H54" s="152">
+      <c r="H54" s="140">
         <f t="shared" si="6"/>
         <v>46.2</v>
       </c>
-      <c r="I54" s="152">
+      <c r="I54" s="140">
         <f t="shared" si="6"/>
         <v>46.7</v>
       </c>
-      <c r="J54" s="152">
+      <c r="J54" s="140">
         <f t="shared" si="6"/>
         <v>47.2</v>
       </c>
-      <c r="K54" s="152">
+      <c r="K54" s="140">
         <f t="shared" si="6"/>
         <v>47.62</v>
       </c>
-      <c r="L54" s="152">
+      <c r="L54" s="140">
         <f t="shared" si="6"/>
         <v>48.12</v>
       </c>
-      <c r="M54" s="152">
+      <c r="M54" s="140">
         <f t="shared" si="6"/>
         <v>48.62</v>
       </c>
-      <c r="N54" s="153">
+      <c r="N54" s="141">
         <f t="shared" si="6"/>
         <v>49.12</v>
       </c>
@@ -13936,148 +13975,148 @@
     <row r="55" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="56" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="8" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="139" t="s">
-        <v>289</v>
+      <c r="A57" s="127" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A58" s="161" t="s">
-        <v>290</v>
-      </c>
-      <c r="F58" s="148">
+      <c r="A58" s="149" t="s">
+        <v>267</v>
+      </c>
+      <c r="F58" s="136">
         <f>F44-(F32-F53)</f>
         <v>35.100000000000009</v>
       </c>
-      <c r="G58" s="149">
+      <c r="G58" s="137">
         <f>G44-(G32-G53)</f>
         <v>44.679999999999993</v>
       </c>
-      <c r="H58" s="149">
+      <c r="H58" s="137">
         <f>H44-(H32-H53)</f>
         <v>60.8</v>
       </c>
-      <c r="I58" s="149">
+      <c r="I58" s="137">
         <f>I44-(I32-I53)</f>
         <v>59.8</v>
       </c>
-      <c r="J58" s="149">
+      <c r="J58" s="137">
         <f t="shared" ref="J58:N58" si="7">J44-(J32-J53)</f>
         <v>58.8</v>
       </c>
-      <c r="K58" s="149">
+      <c r="K58" s="137">
         <f t="shared" si="7"/>
         <v>57.88</v>
       </c>
-      <c r="L58" s="149">
+      <c r="L58" s="137">
         <f t="shared" si="7"/>
         <v>56.88</v>
       </c>
-      <c r="M58" s="149">
+      <c r="M58" s="137">
         <f t="shared" si="7"/>
         <v>55.88</v>
       </c>
-      <c r="N58" s="150">
+      <c r="N58" s="138">
         <f t="shared" si="7"/>
         <v>54.88</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="163" t="s">
-        <v>291</v>
-      </c>
-      <c r="F59" s="176" t="str">
+      <c r="A59" s="151" t="s">
+        <v>268</v>
+      </c>
+      <c r="F59" s="164" t="str">
         <f>IF(AND(F16&gt;F58,(F16-F17)&lt;F58),"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="G59" s="177" t="str">
+      <c r="G59" s="165" t="str">
         <f t="shared" ref="G59:N59" si="8">IF(AND(G16&gt;G58,(G16-G17)&lt;G58),"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="H59" s="177" t="str">
+      <c r="H59" s="165" t="str">
         <f t="shared" si="8"/>
         <v>NO</v>
       </c>
-      <c r="I59" s="177" t="str">
+      <c r="I59" s="165" t="str">
         <f t="shared" si="8"/>
         <v>NO</v>
       </c>
-      <c r="J59" s="177" t="str">
+      <c r="J59" s="165" t="str">
         <f t="shared" si="8"/>
         <v>NO</v>
       </c>
-      <c r="K59" s="177" t="str">
+      <c r="K59" s="165" t="str">
         <f t="shared" si="8"/>
         <v>NO</v>
       </c>
-      <c r="L59" s="177" t="str">
+      <c r="L59" s="165" t="str">
         <f t="shared" si="8"/>
         <v>NO</v>
       </c>
-      <c r="M59" s="177" t="str">
+      <c r="M59" s="165" t="str">
         <f t="shared" si="8"/>
         <v>NO</v>
       </c>
-      <c r="N59" s="178" t="str">
+      <c r="N59" s="166" t="str">
         <f t="shared" si="8"/>
         <v>NO</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="61" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="139" t="s">
-        <v>292</v>
+      <c r="A61" s="127" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A62" s="161" t="s">
-        <v>293</v>
-      </c>
-      <c r="F62" s="148">
+      <c r="A62" s="149" t="s">
+        <v>270</v>
+      </c>
+      <c r="F62" s="136">
         <f>IF(F58-F24&gt;F16-F17,F58-F24,F16-F17)</f>
         <v>35.100000000000009</v>
       </c>
-      <c r="G62" s="149">
+      <c r="G62" s="137">
         <f t="shared" ref="G62:N62" si="9">IF(G58-G24&gt;G16-G17,G58-G24,G16-G17)</f>
         <v>44.679999999999993</v>
       </c>
-      <c r="H62" s="149">
+      <c r="H62" s="137">
         <f t="shared" si="9"/>
         <v>32.799999999999997</v>
       </c>
-      <c r="I62" s="149">
+      <c r="I62" s="137">
         <f>IF(I58-I24&gt;I16-I17,I58-I24,I16-I17)</f>
         <v>31.799999999999997</v>
       </c>
-      <c r="J62" s="149">
+      <c r="J62" s="137">
         <f t="shared" si="9"/>
         <v>30.799999999999997</v>
       </c>
-      <c r="K62" s="149">
+      <c r="K62" s="137">
         <f t="shared" si="9"/>
         <v>29.880000000000003</v>
       </c>
-      <c r="L62" s="149">
+      <c r="L62" s="137">
         <f t="shared" si="9"/>
         <v>28.880000000000003</v>
       </c>
-      <c r="M62" s="149">
+      <c r="M62" s="137">
         <f t="shared" si="9"/>
         <v>27.880000000000003</v>
       </c>
-      <c r="N62" s="150">
+      <c r="N62" s="138">
         <f t="shared" si="9"/>
         <v>26.880000000000003</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A63" s="162" t="s">
-        <v>294</v>
-      </c>
-      <c r="F63" s="159">
+      <c r="A63" s="150" t="s">
+        <v>271</v>
+      </c>
+      <c r="F63" s="147">
         <f>F58-F62</f>
         <v>0</v>
       </c>
@@ -14109,96 +14148,96 @@
         <f t="shared" si="10"/>
         <v>28</v>
       </c>
-      <c r="N63" s="160">
+      <c r="N63" s="148">
         <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="O63" s="1"/>
     </row>
     <row r="64" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="163" t="s">
-        <v>295</v>
-      </c>
-      <c r="F64" s="176" t="str">
+      <c r="A64" s="151" t="s">
+        <v>272</v>
+      </c>
+      <c r="F64" s="164" t="str">
         <f>IF(AND(F16&gt;F62,(F16-F17)&lt;F62),"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="G64" s="177" t="str">
+      <c r="G64" s="165" t="str">
         <f t="shared" ref="G64:N64" si="11">IF(AND(G16&gt;G62,(G16-G17)&lt;G62),"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="H64" s="177" t="str">
+      <c r="H64" s="165" t="str">
         <f t="shared" si="11"/>
         <v>OK</v>
       </c>
-      <c r="I64" s="177" t="str">
+      <c r="I64" s="165" t="str">
         <f t="shared" si="11"/>
         <v>OK</v>
       </c>
-      <c r="J64" s="177" t="str">
+      <c r="J64" s="165" t="str">
         <f t="shared" si="11"/>
         <v>OK</v>
       </c>
-      <c r="K64" s="177" t="str">
+      <c r="K64" s="165" t="str">
         <f t="shared" si="11"/>
         <v>OK</v>
       </c>
-      <c r="L64" s="177" t="str">
+      <c r="L64" s="165" t="str">
         <f t="shared" si="11"/>
         <v>OK</v>
       </c>
-      <c r="M64" s="177" t="str">
+      <c r="M64" s="165" t="str">
         <f t="shared" si="11"/>
         <v>OK</v>
       </c>
-      <c r="N64" s="178" t="str">
+      <c r="N64" s="166" t="str">
         <f t="shared" si="11"/>
         <v>OK</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="66" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="183" t="s">
-        <v>296</v>
+      <c r="A66" s="171" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A67" s="162" t="s">
-        <v>297</v>
-      </c>
-      <c r="F67" s="148">
+      <c r="A67" s="150" t="s">
+        <v>274</v>
+      </c>
+      <c r="F67" s="136">
         <v>0.15</v>
       </c>
-      <c r="G67" s="149">
+      <c r="G67" s="137">
         <v>1.536</v>
       </c>
-      <c r="H67" s="149">
+      <c r="H67" s="137">
         <v>8</v>
       </c>
-      <c r="I67" s="149">
+      <c r="I67" s="137">
         <v>8</v>
       </c>
-      <c r="J67" s="149">
+      <c r="J67" s="137">
         <v>8</v>
       </c>
-      <c r="K67" s="149">
+      <c r="K67" s="137">
         <v>8</v>
       </c>
-      <c r="L67" s="149">
+      <c r="L67" s="137">
         <v>8</v>
       </c>
-      <c r="M67" s="149">
+      <c r="M67" s="137">
         <v>8</v>
       </c>
-      <c r="N67" s="150">
+      <c r="N67" s="138">
         <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A68" s="162" t="s">
-        <v>298</v>
-      </c>
-      <c r="F68" s="159">
+      <c r="A68" s="150" t="s">
+        <v>275</v>
+      </c>
+      <c r="F68" s="147">
         <v>290</v>
       </c>
       <c r="G68" s="21">
@@ -14222,15 +14261,15 @@
       <c r="M68" s="21">
         <v>290</v>
       </c>
-      <c r="N68" s="160">
+      <c r="N68" s="148">
         <v>290</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A69" s="162" t="s">
-        <v>299</v>
-      </c>
-      <c r="F69" s="159">
+      <c r="A69" s="150" t="s">
+        <v>276</v>
+      </c>
+      <c r="F69" s="147">
         <v>-13</v>
       </c>
       <c r="G69" s="21">
@@ -14254,100 +14293,100 @@
       <c r="M69" s="21">
         <v>4</v>
       </c>
-      <c r="N69" s="160">
+      <c r="N69" s="148">
         <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="163" t="s">
-        <v>300</v>
-      </c>
-      <c r="F70" s="151">
+      <c r="A70" s="151" t="s">
+        <v>277</v>
+      </c>
+      <c r="F70" s="139">
         <v>38</v>
       </c>
-      <c r="G70" s="152">
+      <c r="G70" s="140">
         <v>18</v>
       </c>
-      <c r="H70" s="152">
+      <c r="H70" s="140">
         <v>25</v>
       </c>
-      <c r="I70" s="152">
+      <c r="I70" s="140">
         <v>25</v>
       </c>
-      <c r="J70" s="152">
+      <c r="J70" s="140">
         <v>25</v>
       </c>
-      <c r="K70" s="152">
+      <c r="K70" s="140">
         <v>25</v>
       </c>
-      <c r="L70" s="152">
+      <c r="L70" s="140">
         <v>25</v>
       </c>
-      <c r="M70" s="152">
+      <c r="M70" s="140">
         <v>25</v>
       </c>
-      <c r="N70" s="153">
+      <c r="N70" s="141">
         <v>25</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A72" s="184" t="s">
-        <v>301</v>
+      <c r="A72" s="172" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="185" t="s">
-        <v>289</v>
+      <c r="A73" s="173" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A74" s="162" t="s">
-        <v>302</v>
+      <c r="A74" s="150" t="s">
+        <v>279</v>
       </c>
       <c r="B74" s="1"/>
-      <c r="F74" s="148">
+      <c r="F74" s="136">
         <f>10*LOG10(10^((F18+F53)/10)+10^((F53-F58)/10)*(10^((F43+Network!H277)/10)-1))</f>
         <v>16.537205707170102</v>
       </c>
-      <c r="G74" s="149">
+      <c r="G74" s="137">
         <f>10*LOG10(10^((G18+G53)/10)+10^((G53-G58)/10)*(10^((G43+Network!I277)/10)-1))</f>
         <v>12.448242010510427</v>
       </c>
-      <c r="H74" s="149">
+      <c r="H74" s="137">
         <f>10*LOG10(10^((H18+H53)/10)+10^((H53-H58)/10)*(10^((H43+Network!J277)/10)-1))</f>
         <v>12.837121168044634</v>
       </c>
-      <c r="I74" s="149">
+      <c r="I74" s="137">
         <f>10*LOG10(10^((I18+I53)/10)+10^((I53-I58)/10)*(10^((I43+Network!J277)/10)-1))</f>
         <v>12.341628930936814</v>
       </c>
-      <c r="J74" s="149">
+      <c r="J74" s="137">
         <f>10*LOG10(10^((J18+J53)/10)+10^((J53-J58)/10)*(10^((J43+Network!J277)/10)-1))</f>
         <v>11.846681144362297</v>
       </c>
-      <c r="K74" s="149">
+      <c r="K74" s="137">
         <f>10*LOG10(10^((K18+K53)/10)+10^((K53-K58)/10)*(10^((K43+Network!J277)/10)-1))</f>
         <v>11.431393079318745</v>
       </c>
-      <c r="L74" s="149">
+      <c r="L74" s="137">
         <f>10*LOG10(10^((L18+L53)/10)+10^((L53-L58)/10)*(10^((L43+Network!K277)/10)-1))</f>
         <v>11.004322432591573</v>
       </c>
-      <c r="M74" s="149">
+      <c r="M74" s="137">
         <f>10*LOG10(10^((M18+M53)/10)+10^((M53-M58)/10)*(10^((M43+Network!K277)/10)-1))</f>
         <v>10.51925115842595</v>
       </c>
-      <c r="N74" s="150">
+      <c r="N74" s="138">
         <f>10*LOG10(10^((N18+N53)/10)+10^((N53-N58)/10)*(10^((N43+Network!K277)/10)-1))</f>
         <v>10.035940560689802</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A75" s="162" t="s">
-        <v>303</v>
-      </c>
-      <c r="F75" s="179">
+      <c r="A75" s="150" t="s">
+        <v>280</v>
+      </c>
+      <c r="F75" s="167">
         <f>F32-F69-10*LOG10(10^((F18+F53)/10)+10^((F53-F58)/10)*(10^((F43+Network!H277)/10)-1))</f>
         <v>66.462794292829898</v>
       </c>
@@ -14379,105 +14418,105 @@
         <f>M32-M69-10*LOG10(10^((M18+M53)/10)+10^((M53-M58)/10)*(10^((J43+Network!P277)/10)-1))</f>
         <v>35.619999174226699</v>
       </c>
-      <c r="N75" s="181">
+      <c r="N75" s="169">
         <f>N32-N69-10*LOG10(10^((N18+N53)/10)+10^((N53-N58)/10)*(10^((J43+Network!Q277)/10)-1))</f>
         <v>36.119998960413028</v>
       </c>
     </row>
     <row r="76" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="163" t="s">
-        <v>304</v>
-      </c>
-      <c r="F76" s="176" t="str">
+      <c r="A76" s="151" t="s">
+        <v>281</v>
+      </c>
+      <c r="F76" s="164" t="str">
         <f>IF(F75&gt;=F70,"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="G76" s="177" t="str">
+      <c r="G76" s="165" t="str">
         <f t="shared" ref="G76:N76" si="12">IF(G75&gt;=G70,"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="H76" s="177" t="str">
+      <c r="H76" s="165" t="str">
         <f t="shared" si="12"/>
         <v>OK</v>
       </c>
-      <c r="I76" s="177" t="str">
+      <c r="I76" s="165" t="str">
         <f t="shared" si="12"/>
         <v>OK</v>
       </c>
-      <c r="J76" s="177" t="str">
+      <c r="J76" s="165" t="str">
         <f t="shared" si="12"/>
         <v>OK</v>
       </c>
-      <c r="K76" s="177" t="str">
+      <c r="K76" s="165" t="str">
         <f t="shared" si="12"/>
         <v>OK</v>
       </c>
-      <c r="L76" s="177" t="str">
+      <c r="L76" s="165" t="str">
         <f t="shared" si="12"/>
         <v>OK</v>
       </c>
-      <c r="M76" s="177" t="str">
+      <c r="M76" s="165" t="str">
         <f t="shared" si="12"/>
         <v>OK</v>
       </c>
-      <c r="N76" s="178" t="str">
+      <c r="N76" s="166" t="str">
         <f t="shared" si="12"/>
         <v>OK</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="78" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="183" t="s">
-        <v>292</v>
+      <c r="A78" s="171" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A79" s="162" t="s">
-        <v>302</v>
-      </c>
-      <c r="F79" s="148">
+      <c r="A79" s="150" t="s">
+        <v>279</v>
+      </c>
+      <c r="F79" s="136">
         <f>10*LOG10(10^(F26/10)+(10^(F53/10)-1)/10^(F63/10)+(10^(F18/10)-1)*10^(F53/10)/10^(F63/10)+10^((F53-F62-F63)/10)*(10^((F43+Network!H277)/10)-1))</f>
         <v>16.537205707170102</v>
       </c>
-      <c r="G79" s="149">
+      <c r="G79" s="137">
         <f>10*LOG10(10^(G26/10)+(10^(G53/10)-1)/10^(G63/10)+(10^(G18/10)-1)*10^(G53/10)/10^(G63/10)+10^((G53-G62-G63)/10)*(10^((G43+Network!I277)/10)-1))</f>
         <v>12.448242010510429</v>
       </c>
-      <c r="H79" s="149">
+      <c r="H79" s="137">
         <f>10*LOG10(10^(H26/10)+(10^(H53/10)-1)/10^(H63/10)+(10^(H18/10)-1)*10^(H53/10)/10^(H63/10)+10^((H53-H62-H63)/10)*(10^((H43+Network!J277)/10)-1))</f>
         <v>6.6829431135643471</v>
       </c>
-      <c r="I79" s="149">
+      <c r="I79" s="137">
         <f>10*LOG10(10^(I26/10)+(10^(I53/10)-1)/10^(I63/10)+(10^(I18/10)-1)*10^(I53/10)/10^(I63/10)+10^((I53-I62-I63)/10)*(10^((I43+Network!J277)/10)-1))</f>
         <v>6.6798804391014315</v>
       </c>
-      <c r="J79" s="149">
+      <c r="J79" s="137">
         <f>10*LOG10(10^(J26/10)+(10^(J53/10)-1)/10^(J63/10)+(10^(J18/10)-1)*10^(J53/10)/10^(J63/10)+10^((J53-J62-J63)/10)*(10^((J43+Network!J277)/10)-1))</f>
         <v>6.6771489537078939</v>
       </c>
-      <c r="K79" s="149">
+      <c r="K79" s="137">
         <f>10*LOG10(10^(K26/10)+(10^(K53/10)-1)/10^(K63/10)+(10^(K18/10)-1)*10^(K53/10)/10^(K63/10)+10^((K53-K62-K63)/10)*(10^((K43+Network!J277)/10)-1))</f>
         <v>6.6750842057365247</v>
       </c>
-      <c r="L79" s="149">
+      <c r="L79" s="137">
         <f>10*LOG10(10^(L26/10)+(10^(L53/10)-1)/10^(L63/10)+(10^(L18/10)-1)*10^(L53/10)/10^(L63/10)+10^((L53-L62-L63)/10)*(10^((L43+Network!K277)/10)-1))</f>
         <v>6.8487120708452345</v>
       </c>
-      <c r="M79" s="149">
+      <c r="M79" s="137">
         <f>10*LOG10(10^(M26/10)+(10^(M53/10)-1)/10^(M63/10)+(10^(M18/10)-1)*10^(M53/10)/10^(M63/10)+10^((M53-M62-M63)/10)*(10^((M43+Network!K277)/10)-1))</f>
         <v>6.8468174917760871</v>
       </c>
-      <c r="N79" s="150">
+      <c r="N79" s="138">
         <f>10*LOG10(10^(N26/10)+(10^(N53/10)-1)/10^(N63/10)+(10^(N18/10)-1)*10^(N53/10)/10^(N63/10)+10^((N53-N62-N63)/10)*(10^((N43+Network!K277)/10)-1))</f>
         <v>6.8451281695987118</v>
       </c>
       <c r="O79" s="1"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A80" s="162" t="s">
-        <v>303</v>
-      </c>
-      <c r="F80" s="179">
+      <c r="A80" s="150" t="s">
+        <v>280</v>
+      </c>
+      <c r="F80" s="167">
         <f>F32-F69-10*LOG10(10^(F26/10)+(10^(F53/10)-1)/10^(F63/10)+(10^(F18/10)-1)*10^(F53/10)/10^(F63/10)+10^((F53-F62-F63)/10)*(10^((F43+Network!H277)/10)-1))</f>
         <v>66.462794292829898</v>
       </c>
@@ -14509,347 +14548,347 @@
         <f>M32-M69-10*LOG10(10^(M26/10)+(10^(M53/10)-1)/10^(M63/10)+(10^(M18/10)-1)*10^(M53/10)/10^(M63/10)+10^((M53-M62-M63)/10)*(10^((M43+Network!K277)/10)-1))</f>
         <v>39.153182508223914</v>
       </c>
-      <c r="N80" s="181">
+      <c r="N80" s="169">
         <f>N32-N69-10*LOG10(10^(N26/10)+(10^(N53/10)-1)/10^(N63/10)+(10^(N18/10)-1)*10^(N53/10)/10^(N63/10)+10^((N53-N62-N63)/10)*(10^((N43+Network!K277)/10)-1))</f>
         <v>39.154871830401291</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="163" t="s">
-        <v>305</v>
-      </c>
-      <c r="F81" s="176" t="str">
+      <c r="A81" s="151" t="s">
+        <v>282</v>
+      </c>
+      <c r="F81" s="164" t="str">
         <f>IF(F80&gt;=F70,"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="G81" s="177" t="str">
+      <c r="G81" s="165" t="str">
         <f t="shared" ref="G81:N81" si="13">IF(G80&gt;=G70,"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="H81" s="177" t="str">
+      <c r="H81" s="165" t="str">
         <f t="shared" si="13"/>
         <v>OK</v>
       </c>
-      <c r="I81" s="177" t="str">
+      <c r="I81" s="165" t="str">
         <f t="shared" si="13"/>
         <v>OK</v>
       </c>
-      <c r="J81" s="177" t="str">
+      <c r="J81" s="165" t="str">
         <f t="shared" si="13"/>
         <v>OK</v>
       </c>
-      <c r="K81" s="177" t="str">
+      <c r="K81" s="165" t="str">
         <f t="shared" si="13"/>
         <v>OK</v>
       </c>
-      <c r="L81" s="177" t="str">
+      <c r="L81" s="165" t="str">
         <f t="shared" si="13"/>
         <v>OK</v>
       </c>
-      <c r="M81" s="177" t="str">
+      <c r="M81" s="165" t="str">
         <f t="shared" si="13"/>
         <v>OK</v>
       </c>
-      <c r="N81" s="178" t="str">
+      <c r="N81" s="166" t="str">
         <f t="shared" si="13"/>
         <v>OK</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="85" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="139" t="s">
-        <v>277</v>
+      <c r="A85" s="127" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A86" s="161" t="s">
-        <v>278</v>
-      </c>
-      <c r="F86" s="148">
+      <c r="A86" s="149" t="s">
+        <v>255</v>
+      </c>
+      <c r="F86" s="136">
         <v>30</v>
       </c>
-      <c r="G86" s="149">
+      <c r="G86" s="137">
         <v>16</v>
       </c>
-      <c r="H86" s="149">
+      <c r="H86" s="137">
         <v>1</v>
       </c>
-      <c r="I86" s="149">
+      <c r="I86" s="137">
         <v>2</v>
       </c>
-      <c r="J86" s="149">
+      <c r="J86" s="137">
         <v>1</v>
       </c>
-      <c r="K86" s="149">
+      <c r="K86" s="137">
         <v>1</v>
       </c>
-      <c r="L86" s="149">
+      <c r="L86" s="137">
         <v>1</v>
       </c>
-      <c r="M86" s="149">
+      <c r="M86" s="137">
         <v>1</v>
       </c>
-      <c r="N86" s="149">
+      <c r="N86" s="137">
         <v>1</v>
       </c>
-      <c r="O86" s="150">
+      <c r="O86" s="138">
         <v>30</v>
       </c>
     </row>
     <row r="87" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="162" t="s">
-        <v>279</v>
-      </c>
-      <c r="F87" s="165">
+      <c r="A87" s="150" t="s">
+        <v>256</v>
+      </c>
+      <c r="F87" s="153">
         <f>7.5*LOG10((F86-1))</f>
         <v>10.96798498424217</v>
       </c>
-      <c r="G87" s="166">
+      <c r="G87" s="154">
         <f>7.5*LOG10(G86-1)</f>
         <v>8.8206844429176101</v>
       </c>
-      <c r="H87" s="156">
+      <c r="H87" s="144">
         <v>0</v>
       </c>
-      <c r="I87" s="156">
+      <c r="I87" s="144">
         <f>7.5*LOG10(I86-1)</f>
         <v>0</v>
       </c>
-      <c r="J87" s="156">
+      <c r="J87" s="144">
         <v>0</v>
       </c>
-      <c r="K87" s="156">
+      <c r="K87" s="144">
         <v>0</v>
       </c>
-      <c r="L87" s="156">
+      <c r="L87" s="144">
         <v>0</v>
       </c>
-      <c r="M87" s="156">
+      <c r="M87" s="144">
         <v>0</v>
       </c>
-      <c r="N87" s="156">
+      <c r="N87" s="144">
         <v>0</v>
       </c>
-      <c r="O87" s="167">
+      <c r="O87" s="155">
         <f>7.5*LOG10(O86-1)</f>
         <v>10.96798498424217</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="163" t="s">
-        <v>280</v>
-      </c>
-      <c r="H88" s="151">
+      <c r="A88" s="151" t="s">
+        <v>257</v>
+      </c>
+      <c r="H88" s="139">
         <v>30</v>
       </c>
-      <c r="I88" s="152">
+      <c r="I88" s="140">
         <v>30</v>
       </c>
-      <c r="J88" s="152">
+      <c r="J88" s="140">
         <v>30</v>
       </c>
-      <c r="K88" s="152">
+      <c r="K88" s="140">
         <v>30</v>
       </c>
-      <c r="L88" s="152">
+      <c r="L88" s="140">
         <v>30</v>
       </c>
-      <c r="M88" s="152">
+      <c r="M88" s="140">
         <v>30</v>
       </c>
-      <c r="N88" s="152">
+      <c r="N88" s="140">
         <v>30</v>
       </c>
-      <c r="O88" s="153">
+      <c r="O88" s="141">
         <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="90" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="183" t="s">
-        <v>289</v>
+      <c r="A90" s="171" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A91" s="168" t="s">
-        <v>306</v>
-      </c>
-      <c r="H91" s="172">
+      <c r="A91" s="156" t="s">
+        <v>283</v>
+      </c>
+      <c r="H91" s="160">
         <f>H28+2*(H27-H87-H44)</f>
         <v>33</v>
       </c>
-      <c r="I91" s="174">
-        <f t="shared" ref="I91:L91" si="14">I28+2*(I27-H87-I44)</f>
+      <c r="I91" s="162">
+        <f t="shared" ref="I91" si="14">I28+2*(I27-H87-I44)</f>
         <v>34</v>
       </c>
-      <c r="J91" s="174">
+      <c r="J91" s="162">
         <f>J28+2*(J27-J87-J44)</f>
         <v>35</v>
       </c>
-      <c r="K91" s="174">
+      <c r="K91" s="162">
         <f>K28+2*(K27-K87-K44)</f>
         <v>36</v>
       </c>
-      <c r="L91" s="174">
+      <c r="L91" s="162">
         <f>L28+2*(L27-L87-L44)</f>
         <v>37</v>
       </c>
-      <c r="M91" s="174">
+      <c r="M91" s="162">
         <f>M28+2*(M27-M87-M44)</f>
         <v>38</v>
       </c>
-      <c r="N91" s="198">
+      <c r="N91" s="181">
         <f>N28+2*(N27-N87-N44)</f>
         <v>39</v>
       </c>
-      <c r="O91" s="175">
+      <c r="O91" s="163">
         <f>O20+2*(O19-O87-O44)</f>
         <v>51.064030031515671</v>
       </c>
     </row>
     <row r="92" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="138" t="s">
-        <v>307</v>
-      </c>
-      <c r="H92" s="176" t="str">
+      <c r="A92" s="126" t="s">
+        <v>284</v>
+      </c>
+      <c r="H92" s="164" t="str">
         <f>IF(H91&gt;=H88,"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="I92" s="177" t="str">
-        <f t="shared" ref="I92:O92" si="15">IF(I91&gt;=I88,"OK","NO")</f>
+      <c r="I92" s="165" t="str">
+        <f t="shared" ref="I92:N92" si="15">IF(I91&gt;=I88,"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="J92" s="177" t="str">
+      <c r="J92" s="165" t="str">
         <f t="shared" si="15"/>
         <v>OK</v>
       </c>
-      <c r="K92" s="177" t="str">
+      <c r="K92" s="165" t="str">
         <f t="shared" si="15"/>
         <v>OK</v>
       </c>
-      <c r="L92" s="177" t="str">
+      <c r="L92" s="165" t="str">
         <f t="shared" si="15"/>
         <v>OK</v>
       </c>
-      <c r="M92" s="177" t="str">
+      <c r="M92" s="165" t="str">
         <f t="shared" si="15"/>
         <v>OK</v>
       </c>
-      <c r="N92" s="182" t="str">
+      <c r="N92" s="170" t="str">
         <f t="shared" si="15"/>
         <v>OK</v>
       </c>
-      <c r="O92" s="178" t="str">
+      <c r="O92" s="166" t="str">
         <f>IF(O91&gt;=O88,"OK","NO")</f>
         <v>OK</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="O93" s="200"/>
+      <c r="O93" s="183"/>
     </row>
     <row r="94" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="183" t="s">
-        <v>292</v>
-      </c>
-      <c r="O94" s="200"/>
+      <c r="A94" s="171" t="s">
+        <v>269</v>
+      </c>
+      <c r="O94" s="183"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A95" s="162" t="s">
-        <v>308</v>
-      </c>
-      <c r="H95" s="148">
+      <c r="A95" s="150" t="s">
+        <v>285</v>
+      </c>
+      <c r="H95" s="136">
         <f>H32+H63</f>
         <v>78</v>
       </c>
-      <c r="I95" s="149">
-        <f t="shared" ref="I95:O95" si="16">I32+I63</f>
+      <c r="I95" s="137">
+        <f t="shared" ref="I95:L95" si="16">I32+I63</f>
         <v>78</v>
       </c>
-      <c r="J95" s="149">
+      <c r="J95" s="137">
         <f t="shared" si="16"/>
         <v>78</v>
       </c>
-      <c r="K95" s="149">
+      <c r="K95" s="137">
         <f t="shared" si="16"/>
         <v>78</v>
       </c>
-      <c r="L95" s="149">
+      <c r="L95" s="137">
         <f t="shared" si="16"/>
         <v>78</v>
       </c>
-      <c r="M95" s="201">
+      <c r="M95" s="184">
         <f>M32+M63</f>
         <v>78</v>
       </c>
-      <c r="N95" s="150">
+      <c r="N95" s="138">
         <f>N32+N63</f>
         <v>78</v>
       </c>
-      <c r="O95" s="203"/>
+      <c r="O95" s="186"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A96" s="168" t="s">
-        <v>309</v>
-      </c>
-      <c r="H96" s="187">
+      <c r="A96" s="156" t="s">
+        <v>286</v>
+      </c>
+      <c r="H96" s="175">
         <f>-20*LOG10(10^(-H91/20)+10^(-(H28+2*(H27-7.5*LOG10(SUM(H86:N86)-1)-H32-H63))/20))</f>
         <v>32.953068544611554</v>
       </c>
-      <c r="I96" s="186">
+      <c r="I96" s="174">
         <f>-20*LOG10(10^(-I91/20)+10^(-(I28+2*(I27-7.5*LOG10(SUM(H86:N86)-1)-I32-I63))/20))</f>
         <v>33.947359360533518</v>
       </c>
-      <c r="J96" s="186">
+      <c r="J96" s="174">
         <f>-20*LOG10(10^(-J91/20)+10^(-(J28+2*(J27-7.5*LOG10(SUM(I86:O86)-1)-J32-J63))/20))</f>
         <v>34.799999274861314</v>
       </c>
-      <c r="K96" s="186">
+      <c r="K96" s="174">
         <f>-20*LOG10(10^(-K91/20)+10^(-(K28+2*(K27-7.5*LOG10(SUM(H86:N86)-1)-K32-K63))/20))</f>
         <v>35.933781198644489</v>
       </c>
-      <c r="L96" s="186">
+      <c r="L96" s="174">
         <f>-20*LOG10(10^(-L91/20)+10^(-(L28+2*(L27-7.5*LOG10(SUM(H86:N86)-1)-L32-L63))/20))</f>
         <v>36.925735731532804</v>
       </c>
-      <c r="M96" s="202">
+      <c r="M96" s="185">
         <f>-20*LOG10(10^(-M91/20)+10^(-(M28+2*(M27-7.5*LOG10(SUM(H86:N86)-1)-M32-M63))/20))</f>
         <v>37.916717431794545</v>
       </c>
-      <c r="N96" s="188">
+      <c r="N96" s="176">
         <f>-20*LOG10(10^(-N91/20)+10^(-(N28+2*(N27-7.5*LOG10(SUM(H86:N86)-1)-N32-N63))/20))</f>
         <v>38.906609867464191</v>
       </c>
-      <c r="O96" s="204"/>
+      <c r="O96" s="187"/>
     </row>
     <row r="97" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="138" t="s">
-        <v>310</v>
-      </c>
-      <c r="H97" s="176" t="str">
+      <c r="A97" s="126" t="s">
+        <v>287</v>
+      </c>
+      <c r="H97" s="164" t="str">
         <f>IF(H96&gt;=H88,"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="I97" s="177" t="str">
+      <c r="I97" s="165" t="str">
         <f t="shared" ref="I97:N97" si="17">IF(I96&gt;=I88,"OK","NO")</f>
         <v>OK</v>
       </c>
-      <c r="J97" s="177" t="str">
+      <c r="J97" s="165" t="str">
         <f t="shared" si="17"/>
         <v>OK</v>
       </c>
-      <c r="K97" s="177" t="str">
+      <c r="K97" s="165" t="str">
         <f t="shared" si="17"/>
         <v>OK</v>
       </c>
-      <c r="L97" s="177" t="str">
+      <c r="L97" s="165" t="str">
         <f t="shared" si="17"/>
         <v>OK</v>
       </c>
-      <c r="M97" s="182" t="str">
+      <c r="M97" s="170" t="str">
         <f t="shared" si="17"/>
         <v>OK</v>
       </c>
-      <c r="N97" s="178" t="str">
+      <c r="N97" s="166" t="str">
         <f t="shared" si="17"/>
         <v>OK</v>
       </c>
@@ -14861,11 +14900,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="97" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="97" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14875,544 +14914,441 @@
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="32"/>
       <c r="B2" s="192" t="s">
         <v>205</v>
       </c>
       <c r="C2" s="193"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="118"/>
-      <c r="B3" s="119" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="197"/>
+      <c r="B3" s="198" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="198" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="120" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="119" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="121">
+      <c r="B4" s="199">
         <v>39.49</v>
       </c>
-      <c r="C4" s="121">
+      <c r="C4" s="199">
         <v>39.49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="122" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="119" t="s">
         <v>209</v>
       </c>
-      <c r="B5" s="123">
+      <c r="B5" s="199">
         <v>30</v>
       </c>
-      <c r="C5" s="123">
+      <c r="C5" s="199">
         <v>19.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="122" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="119" t="s">
+        <v>298</v>
+      </c>
+      <c r="B6" s="199">
+        <f>30-0.36</f>
+        <v>29.64</v>
+      </c>
+      <c r="C6" s="199">
+        <f>-C5-0.36</f>
+        <v>-19.559999999999999</v>
+      </c>
+      <c r="F6" s="194"/>
+      <c r="G6" s="194"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="119" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="200">
+        <f>DEGREES(ACOS(COS(RADIANS(B6))*COS(RADIANS(B4))))</f>
+        <v>47.874722541842957</v>
+      </c>
+      <c r="C7" s="200">
+        <f>DEGREES(ACOS(COS(RADIANS(C6))*COS(RADIANS(C4))))</f>
+        <v>43.347844323707463</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="119" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" s="199">
+        <v>6378.16</v>
+      </c>
+      <c r="C8" s="199">
+        <v>6378.16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="119" t="s">
+        <v>294</v>
+      </c>
+      <c r="B9" s="199">
+        <v>35786.300000000003</v>
+      </c>
+      <c r="C9" s="199">
+        <v>35786.300000000003</v>
+      </c>
+      <c r="F9" s="196"/>
+      <c r="G9" s="196"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="119" t="s">
+        <v>295</v>
+      </c>
+      <c r="B10" s="201">
+        <f>DEGREES(ATAN((COS(RADIANS(B7))-B8/(B9+B8))/SIN(RADIANS(B7))))</f>
+        <v>35.008051729265496</v>
+      </c>
+      <c r="C10" s="201">
+        <f>DEGREES(ATAN((COS(RADIANS(C7))-B8/(B9+B8))/SIN(RADIANS(C7))))</f>
+        <v>39.997625557419383</v>
+      </c>
+      <c r="F10" s="194"/>
+      <c r="G10" s="194"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="119" t="s">
+        <v>296</v>
+      </c>
+      <c r="B11" s="200">
+        <f>180 + DEGREES(ATAN(TAN(RADIANS(B6))/SIN(RADIANS(B4))))</f>
+        <v>221.82020731856079</v>
+      </c>
+      <c r="C11" s="200">
+        <f>180 + DEGREES(ATAN(TAN(RADIANS(C6))/SIN(RADIANS(C4))))</f>
+        <v>150.80819109153012</v>
+      </c>
+      <c r="F11" s="194"/>
+      <c r="G11" s="195"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="119" t="s">
+        <v>297</v>
+      </c>
+      <c r="B12" s="200">
+        <f>B9*SQRT(1+((2*B8*(B8+B9))/POWER(B9,2)*(1-COS(RADIANS(B7)))))</f>
+        <v>38180.475101277909</v>
+      </c>
+      <c r="C12" s="202">
+        <f>C9*SQRT(1+((2*C8*(C8+C9))/POWER(C9,2)*(1-COS(RADIANS(C7)))))</f>
+        <v>37780.795202936883</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="118"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="118"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="119" t="s">
+        <v>217</v>
+      </c>
+      <c r="B15" s="120">
+        <v>54</v>
+      </c>
+      <c r="C15" s="120">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="119" t="s">
         <v>210</v>
       </c>
-      <c r="B6" s="123">
-        <f>B5-0.36</f>
-        <v>29.64</v>
-      </c>
-      <c r="C6" s="123">
-        <f>-0.36-19.2</f>
-        <v>-19.559999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="122" t="s">
-        <v>211</v>
-      </c>
-      <c r="B7" s="121">
-        <v>47.88</v>
-      </c>
-      <c r="C7" s="121">
-        <v>43.35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="122" t="s">
-        <v>212</v>
-      </c>
-      <c r="B8" s="121">
-        <v>6378.16</v>
-      </c>
-      <c r="C8" s="121">
-        <v>6378.16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="122" t="s">
-        <v>213</v>
-      </c>
-      <c r="B9" s="121">
-        <v>35786.300000000003</v>
-      </c>
-      <c r="C9" s="121">
-        <v>35786.300000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="122" t="s">
-        <v>214</v>
-      </c>
-      <c r="B10" s="121">
-        <v>38180.474999999999</v>
-      </c>
-      <c r="C10" s="121">
-        <v>37780.794999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="122" t="s">
-        <v>215</v>
-      </c>
-      <c r="B11" s="121">
-        <v>35</v>
-      </c>
-      <c r="C11" s="121">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="122" t="s">
-        <v>216</v>
-      </c>
-      <c r="B12" s="121">
-        <v>221.82</v>
-      </c>
-      <c r="C12" s="121">
-        <v>150.81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="124"/>
-      <c r="B13" s="124"/>
-      <c r="C13" s="124"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="119" t="s">
-        <v>217</v>
-      </c>
-      <c r="B14" s="121">
-        <v>54</v>
-      </c>
-      <c r="C14" s="121">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="119" t="s">
-        <v>218</v>
-      </c>
-      <c r="B15" s="121">
-        <f>B14-20*LOG10((4*PI()*B10*10^3)/((3*10^8)/(12.75*10^9)))-1.8+138.75</f>
-        <v>-15.238802423677953</v>
-      </c>
-      <c r="C15" s="121">
-        <f>C14-20*LOG10((4*PI()*C10*10^3)/((3*10^8)/(12.75*10^9)))-1.8+138.75</f>
-        <v>-18.147397727373288</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="125"/>
-      <c r="B16" s="126"/>
-      <c r="C16" s="126"/>
+      <c r="B16" s="120">
+        <v>0.7</v>
+      </c>
+      <c r="C16" s="120">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="119" t="s">
-        <v>219</v>
-      </c>
-      <c r="B17" s="121">
-        <f>B23-10*LOG10(1+(B21/B20))</f>
-        <v>17.132739049129246</v>
-      </c>
-      <c r="C17" s="121">
-        <f>C23-10*LOG10(1+(C21/C20))</f>
-        <v>14.22414374543391</v>
+        <v>216</v>
+      </c>
+      <c r="B17" s="120">
+        <v>50</v>
+      </c>
+      <c r="C17" s="120">
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="119" t="s">
-        <v>220</v>
-      </c>
-      <c r="B18" s="121">
-        <f>B15+B19</f>
-        <v>23.761197576322047</v>
-      </c>
-      <c r="C18" s="121">
-        <f>C15+C19</f>
-        <v>20.852602272626712</v>
+        <v>215</v>
+      </c>
+      <c r="B18" s="120">
+        <v>3</v>
+      </c>
+      <c r="C18" s="120">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="119" t="s">
-        <v>221</v>
-      </c>
-      <c r="B19" s="121">
-        <v>39</v>
-      </c>
-      <c r="C19" s="121">
-        <v>39</v>
+        <v>211</v>
+      </c>
+      <c r="B19" s="120">
+        <v>27</v>
+      </c>
+      <c r="C19" s="120">
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="119" t="s">
-        <v>222</v>
-      </c>
-      <c r="B20" s="121">
-        <v>110</v>
-      </c>
-      <c r="C20" s="121">
-        <v>110</v>
+        <v>212</v>
+      </c>
+      <c r="B20" s="120">
+        <v>0.7</v>
+      </c>
+      <c r="C20" s="120">
+        <v>0.7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="119" t="s">
-        <v>223</v>
-      </c>
-      <c r="B21" s="121">
-        <f>290*(10^(0.75/10)-1)</f>
-        <v>54.665645956735368</v>
-      </c>
-      <c r="C21" s="121">
-        <f>290*(10^(0.75/10)-1)</f>
-        <v>54.665645956735368</v>
+        <v>213</v>
+      </c>
+      <c r="B21" s="120">
+        <v>12.75</v>
+      </c>
+      <c r="C21" s="120">
+        <v>12.75</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="119" t="s">
-        <v>224</v>
-      </c>
-      <c r="B22" s="121">
-        <f>10*LOG10((1.38*10^(-23))*B20*B24)+138.75</f>
-        <v>4.8763553571844795</v>
-      </c>
-      <c r="C22" s="121">
-        <f>10*LOG10((1.38*10^(-23))*C20*C24)+138.75</f>
-        <v>4.8763553571844795</v>
+        <v>218</v>
+      </c>
+      <c r="B22" s="120">
+        <f>92.44+20*LOG10(B21)+20*LOG10(B12)</f>
+        <v>206.18703026066953</v>
+      </c>
+      <c r="C22" s="120">
+        <f>92.44+20*LOG10(C21)+20*LOG10(C12)</f>
+        <v>206.09562558798024</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="119" t="s">
-        <v>225</v>
-      </c>
-      <c r="B23" s="121">
-        <f>B18-B22</f>
-        <v>18.884842219137568</v>
-      </c>
-      <c r="C23" s="121">
-        <f>C18-C22</f>
-        <v>15.976246915442232</v>
+        <v>219</v>
+      </c>
+      <c r="B23" s="120">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C23" s="120">
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="119" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B24" s="121">
-        <f>27*1000000</f>
-        <v>27000000</v>
+        <v>1.3800000000000001E-23</v>
       </c>
       <c r="C24" s="121">
-        <f>27*1000000</f>
-        <v>27000000</v>
+        <v>1.3800000000000001E-23</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="127"/>
-      <c r="B25" s="124"/>
-      <c r="C25" s="124"/>
+      <c r="A25" s="119" t="s">
+        <v>220</v>
+      </c>
+      <c r="B25" s="120">
+        <f>B17+290*(POWER(10,B20/10)-1)</f>
+        <v>100.72029093246357</v>
+      </c>
+      <c r="C25" s="120">
+        <f>C17+290*(POWER(10,C20/10)-1)</f>
+        <v>100.72029093246357</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="119" t="s">
-        <v>227</v>
-      </c>
-      <c r="B26" s="129">
-        <v>25</v>
-      </c>
-      <c r="C26" s="129">
-        <v>25</v>
+        <v>221</v>
+      </c>
+      <c r="B26" s="122">
+        <f>11+B18</f>
+        <v>14</v>
+      </c>
+      <c r="C26" s="120">
+        <f>11+C18</f>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="130" t="s">
-        <v>228</v>
-      </c>
-      <c r="B27" s="131">
-        <v>35</v>
-      </c>
-      <c r="C27" s="131">
-        <v>35</v>
+      <c r="A27" s="119" t="s">
+        <v>214</v>
+      </c>
+      <c r="B27" s="121">
+        <f>10*LOG10(B24*B25*B19*1000000)</f>
+        <v>-134.25640177870341</v>
+      </c>
+      <c r="C27" s="121">
+        <f>10*LOG10(C24*C25*C19*1000000)</f>
+        <v>-134.25640177870341</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="130" t="s">
-        <v>229</v>
-      </c>
-      <c r="B28" s="131">
-        <v>110</v>
-      </c>
-      <c r="C28" s="131">
-        <v>110</v>
+      <c r="A28" s="119" t="s">
+        <v>222</v>
+      </c>
+      <c r="B28" s="121">
+        <f>B26-B15+B22+B23+B27</f>
+        <v>37.030628481966119</v>
+      </c>
+      <c r="C28" s="121">
+        <f>C26-C15+C22+C23+C27</f>
+        <v>39.939223809276825</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="130" t="s">
-        <v>230</v>
-      </c>
-      <c r="B29" s="131">
-        <f>B28+(B26-B27)/2</f>
-        <v>105</v>
-      </c>
-      <c r="C29" s="131">
-        <f>C28+(C26-C27)/2</f>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="130" t="s">
-        <v>231</v>
-      </c>
-      <c r="B30" s="131">
-        <f>B29+7.5*LOG10(30-1)</f>
-        <v>115.96798498424216</v>
-      </c>
-      <c r="C30" s="131">
-        <f>C29+7.5*LOG10(30-1)</f>
-        <v>115.96798498424216</v>
+      <c r="A29" s="119" t="s">
+        <v>223</v>
+      </c>
+      <c r="B29" s="120">
+        <f>300000000/(B21*1000000000)</f>
+        <v>2.3529411764705882E-2</v>
+      </c>
+      <c r="C29" s="120">
+        <f>300000000/(C21*1000000000)</f>
+        <v>2.3529411764705882E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="130" t="s">
-        <v>232</v>
-      </c>
-      <c r="B31" s="131">
-        <v>118.5</v>
-      </c>
-      <c r="C31" s="131">
-        <v>118.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="128" t="s">
-        <v>240</v>
-      </c>
-      <c r="B34" s="132">
-        <v>54</v>
-      </c>
-      <c r="C34" s="132">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="128" t="s">
-        <v>233</v>
-      </c>
-      <c r="B35" s="132">
-        <v>0.7</v>
-      </c>
-      <c r="C35" s="132">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="128" t="s">
-        <v>239</v>
-      </c>
-      <c r="B36" s="132">
-        <v>50</v>
-      </c>
-      <c r="C36" s="132">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="128" t="s">
-        <v>238</v>
-      </c>
-      <c r="B37" s="132">
-        <v>3</v>
-      </c>
-      <c r="C37" s="132">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="128" t="s">
-        <v>234</v>
-      </c>
-      <c r="B38" s="132">
-        <v>27</v>
-      </c>
-      <c r="C38" s="132">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="128" t="s">
-        <v>235</v>
-      </c>
-      <c r="B39" s="132">
-        <v>0.7</v>
-      </c>
-      <c r="C39" s="132">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="128" t="s">
-        <v>236</v>
-      </c>
-      <c r="B40" s="132">
-        <v>12.75</v>
-      </c>
-      <c r="C40" s="132">
-        <v>12.75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="128" t="s">
-        <v>241</v>
-      </c>
-      <c r="B41" s="132">
-        <f>92.44+20*LOG10(B40)+20*LOG10(B10)</f>
-        <v>206.18703023762927</v>
-      </c>
-      <c r="C41" s="132">
-        <f>92.44+20*LOG10(C40)+20*LOG10(C10)</f>
-        <v>206.09562554132461</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="128" t="s">
-        <v>242</v>
-      </c>
-      <c r="B42" s="132">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="C42" s="132">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="128" t="s">
-        <v>248</v>
-      </c>
-      <c r="B43" s="133">
-        <v>1.3800000000000001E-23</v>
-      </c>
-      <c r="C43" s="133">
-        <v>1.3800000000000001E-23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="128" t="s">
-        <v>243</v>
-      </c>
-      <c r="B44" s="132">
-        <f>B36+290*(POWER(10,B39/10)-1)</f>
-        <v>100.72029093246357</v>
-      </c>
-      <c r="C44" s="132">
-        <f>C36+290*(POWER(10,C39/10)-1)</f>
-        <v>100.72029093246357</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="128" t="s">
-        <v>244</v>
-      </c>
-      <c r="B45" s="134">
-        <f>11+B37</f>
+      <c r="A31" s="119"/>
+      <c r="B31" s="121">
+        <f>B29*POWER(10,(B28/20))</f>
+        <v>1.6716389969050396</v>
+      </c>
+      <c r="C31" s="121">
+        <f>C29*POWER(10,(C28/20))</f>
+        <v>2.3365348359815972</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="119" t="s">
+        <v>342</v>
+      </c>
+      <c r="B32" s="121">
+        <f>B31/(PI()*SQRT(B16))</f>
+        <v>0.63598020936830035</v>
+      </c>
+      <c r="C32" s="121">
+        <f>C31/(PI()*SQRT(C16))</f>
+        <v>0.88894188095344961</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="119" t="s">
+        <v>224</v>
+      </c>
+      <c r="B33" s="121">
+        <f>B28-10*LOG10(B25)</f>
+        <v>16.999458766271765</v>
+      </c>
+      <c r="C33" s="121">
+        <f>C28-10*LOG10(C25)</f>
+        <v>19.908054093582471</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="204" t="s">
+        <v>344</v>
+      </c>
+      <c r="B34" s="205">
+        <f>B15-B23-B22+B28</f>
+        <v>-120.25640177870341</v>
+      </c>
+      <c r="C34" s="205">
+        <f>C15-C23-C22+C28</f>
+        <v>-120.25640177870341</v>
+      </c>
+      <c r="D34" s="203"/>
+      <c r="E34" s="203"/>
+      <c r="F34" s="203"/>
+      <c r="G34" s="203">
+        <f>(G13-G21-G22+G30)-G29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>343</v>
+      </c>
+      <c r="B35" s="203">
+        <f>(B15-B23-B22+B28)-B27</f>
         <v>14</v>
       </c>
-      <c r="C45" s="132">
-        <f>11+C37</f>
+      <c r="C35" s="203">
+        <f>(C15-C23-C22+C28)-C27</f>
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="128" t="s">
-        <v>237</v>
-      </c>
-      <c r="B46" s="133">
-        <f>10*LOG10(B43*B44*B38*1000000)</f>
-        <v>-134.25640177870341</v>
-      </c>
-      <c r="C46" s="133">
-        <f>10*LOG10(C43*C44*C38*1000000)</f>
-        <v>-134.25640177870341</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="128" t="s">
-        <v>245</v>
-      </c>
-      <c r="B47" s="133">
-        <f>B45-B34+B41+B42+B46</f>
-        <v>37.030628458925861</v>
-      </c>
-      <c r="C47" s="133">
-        <f>C45-C34+C41+C42+C46</f>
-        <v>39.939223762621197</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="128" t="s">
-        <v>246</v>
-      </c>
-      <c r="B48" s="132">
-        <f>300000000/(B40*1000000000)</f>
-        <v>2.3529411764705882E-2</v>
-      </c>
-      <c r="C48" s="132">
-        <f>300000000/(C40*1000000000)</f>
-        <v>2.3529411764705882E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="128"/>
-      <c r="B50" s="133">
-        <f>B48*POWER(10,(B47/20))</f>
-        <v>1.671638992470837</v>
-      </c>
-      <c r="C50" s="133">
-        <f>C48*POWER(10,(C47/20))</f>
-        <v>2.3365348234310672</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="128" t="s">
-        <v>315</v>
-      </c>
-      <c r="B51" s="133">
-        <f>B50/(PI()*SQRT(B35))</f>
-        <v>0.63598020768129437</v>
-      </c>
-      <c r="C51" s="133">
-        <f>C50/(PI()*SQRT(C35))</f>
-        <v>0.8889418761785618</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="128" t="s">
-        <v>247</v>
-      </c>
-      <c r="B52" s="133">
-        <f>B47-10*LOG10(B44)</f>
-        <v>16.999458743231507</v>
-      </c>
-      <c r="C52" s="133">
-        <f>C47-10*LOG10(C44)</f>
-        <v>19.908054046926843</v>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>338</v>
+      </c>
+      <c r="B36">
+        <f>B34+60-(29.6*0.2)</f>
+        <v>-66.176401778703408</v>
+      </c>
+      <c r="C36">
+        <f>C34+60-(29.6*0.2)</f>
+        <v>-66.176401778703408</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>339</v>
+      </c>
+      <c r="B37">
+        <f>SQRT(POWER(10,(B36/10))*75)*1000000</f>
+        <v>4253.1484633272221</v>
+      </c>
+      <c r="C37">
+        <f>SQRT(POWER(10,(C36/10))*75)*1000000</f>
+        <v>4253.1484633272221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>340</v>
+      </c>
+      <c r="B38">
+        <f>20*LOG10(B37)</f>
+        <v>72.574210855213593</v>
+      </c>
+      <c r="C38">
+        <f>20*LOG10(C37)</f>
+        <v>72.574210855213593</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>341</v>
+      </c>
+      <c r="B40">
+        <f>123-B38</f>
+        <v>50.425789144786407</v>
+      </c>
+      <c r="C40">
+        <f>123-C38</f>
+        <v>50.425789144786407</v>
       </c>
     </row>
   </sheetData>
@@ -15420,5 +15356,428 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2">
+        <f>B3*B6</f>
+        <v>523.20000000000005</v>
+      </c>
+      <c r="E2" t="s">
+        <v>322</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B3">
+        <f>((B4)^2/16)*B5</f>
+        <v>799.52256944444457</v>
+      </c>
+      <c r="E3" t="s">
+        <v>324</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4">
+        <f>130*(1000/3600)</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="E4" t="s">
+        <v>327</v>
+      </c>
+      <c r="F4">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B5">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B6">
+        <f>523.2/B3</f>
+        <v>0.65439053254437862</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>326</v>
+      </c>
+      <c r="B9">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E9">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>305</v>
+      </c>
+      <c r="B11">
+        <v>0.7</v>
+      </c>
+      <c r="E11">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>306</v>
+      </c>
+      <c r="B12">
+        <f>B9*B10*B11</f>
+        <v>0.189</v>
+      </c>
+      <c r="E12">
+        <f>E9*E10*E11</f>
+        <v>9.4500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13">
+        <f>800*B12</f>
+        <v>151.19999999999999</v>
+      </c>
+      <c r="E13">
+        <f>800*E12</f>
+        <v>75.599999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>308</v>
+      </c>
+      <c r="C16" t="s">
+        <v>328</v>
+      </c>
+      <c r="E16" t="s">
+        <v>308</v>
+      </c>
+      <c r="F16" t="s">
+        <v>328</v>
+      </c>
+      <c r="H16" t="s">
+        <v>333</v>
+      </c>
+      <c r="K16" t="s">
+        <v>336</v>
+      </c>
+      <c r="L16" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>309</v>
+      </c>
+      <c r="B17">
+        <v>93</v>
+      </c>
+      <c r="C17">
+        <f>B17*B18</f>
+        <v>558</v>
+      </c>
+      <c r="E17">
+        <v>93</v>
+      </c>
+      <c r="F17">
+        <f>E17*E18</f>
+        <v>558</v>
+      </c>
+      <c r="H17">
+        <v>93</v>
+      </c>
+      <c r="K17">
+        <f>2*B5</f>
+        <v>19.62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>310</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>311</v>
+      </c>
+      <c r="B19">
+        <v>36.5</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:C23" si="0">B19*B20</f>
+        <v>146</v>
+      </c>
+      <c r="E19">
+        <v>36.5</v>
+      </c>
+      <c r="F19">
+        <f>E19*E20</f>
+        <v>146</v>
+      </c>
+      <c r="H19">
+        <v>36.5</v>
+      </c>
+      <c r="K19">
+        <f>1.5*B5</f>
+        <v>14.715</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>312</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>316</v>
+      </c>
+      <c r="B21">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <f>B21*B22</f>
+        <v>54</v>
+      </c>
+      <c r="E21">
+        <v>27</v>
+      </c>
+      <c r="F21">
+        <f>E21*E22</f>
+        <v>54</v>
+      </c>
+      <c r="H21">
+        <v>27</v>
+      </c>
+      <c r="K21">
+        <f>1.2*B5</f>
+        <v>11.772</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>313</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>314</v>
+      </c>
+      <c r="B23">
+        <v>523.20000000000005</v>
+      </c>
+      <c r="C23">
+        <f>B23*B24</f>
+        <v>261.60000000000002</v>
+      </c>
+      <c r="E23">
+        <v>523.20000000000005</v>
+      </c>
+      <c r="F23">
+        <f>E23*E24</f>
+        <v>261.60000000000002</v>
+      </c>
+      <c r="H23">
+        <v>523.20000000000005</v>
+      </c>
+      <c r="K23">
+        <f>5*9.81</f>
+        <v>49.050000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>315</v>
+      </c>
+      <c r="B24">
+        <v>0.5</v>
+      </c>
+      <c r="E24">
+        <v>0.5</v>
+      </c>
+      <c r="H24">
+        <f>E13</f>
+        <v>75.599999999999994</v>
+      </c>
+      <c r="I24" t="s">
+        <v>335</v>
+      </c>
+      <c r="K24">
+        <f>2*B5</f>
+        <v>19.62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <f>2.5*B5</f>
+        <v>24.525000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>317</v>
+      </c>
+      <c r="B26">
+        <f>SUM(C17,C19,C21,C23)</f>
+        <v>1019.6</v>
+      </c>
+      <c r="E26">
+        <f>SUM(F17,F21,F19,F23)</f>
+        <v>1019.6</v>
+      </c>
+      <c r="H26" t="s">
+        <v>334</v>
+      </c>
+      <c r="I26">
+        <f>-SUM(H17,H19,H21,H23,H24)</f>
+        <v>-755.30000000000007</v>
+      </c>
+      <c r="K26">
+        <f>-SUM(K24,K25,K23,K21,K19,K17)</f>
+        <v>-139.30200000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>318</v>
+      </c>
+      <c r="B27">
+        <f>0.045*280*((B10)^2-(3)^2)</f>
+        <v>340.2</v>
+      </c>
+      <c r="E27">
+        <f>(0.045*280*((E10)^2))*6</f>
+        <v>680.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>319</v>
+      </c>
+      <c r="B28">
+        <f>B26+B27</f>
+        <v>1359.8</v>
+      </c>
+      <c r="E28">
+        <f>E26+E27</f>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>320</v>
+      </c>
+      <c r="B29">
+        <f>B28-355</f>
+        <v>1004.8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>323</v>
+      </c>
+      <c r="E29">
+        <f>E28-355</f>
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>332</v>
+      </c>
+      <c r="E33" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>331</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificación de los cálculos con altura antena
</commit_message>
<xml_diff>
--- a/3C/ITSIT/CTI3.xlsx
+++ b/3C/ITSIT/CTI3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upvedues-my.sharepoint.com/personal/cribella_upv_edu_es/Documents/6-1/ITSIT/Trabajo/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_9F969C7D01730002509DB1C2D8DF9BE1D3ADC0FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33D6F5FC-D604-4C69-81D5-FDBAEFC00409}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9576" windowHeight="2760" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Network" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Satellite" sheetId="3" r:id="rId3"/>
     <sheet name="Mast + Tower" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="342">
   <si>
     <t>TECHNICAL CHARACTERISTICS OF ELEMENTS FROM CATALOGUE</t>
   </si>
@@ -829,12 +830,6 @@
     <t>Amplificador input level, Sin (dBuV)</t>
   </si>
   <si>
-    <t>Preguntar que tipo de cable es este para buscar los valores que corresponden</t>
-  </si>
-  <si>
-    <t>Preguntar si los valores de Outdoor cable length son estos (Me tienen que decir Josepe estos valores a que altura estan las antenas estas)</t>
-  </si>
-  <si>
     <t>AMPLIFIER GAIN</t>
   </si>
   <si>
@@ -1049,9 +1044,6 @@
   </si>
   <si>
     <t>Fuerzas verticales (según diapositivas he aproximado los pesos de cada antena)</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
   <si>
     <t>Pin (dBW)</t>
@@ -1078,13 +1070,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
-    <numFmt numFmtId="179" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1995,7 +1987,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2400,13 +2392,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2422,32 +2435,6 @@
     <xf numFmtId="0" fontId="3" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="19" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -2773,10 +2760,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O308"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G308" sqref="G308"/>
     </sheetView>
   </sheetViews>
@@ -12376,16 +12363,16 @@
       <c r="A280" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="C280" s="189" t="s">
+      <c r="C280" s="198" t="s">
         <v>198</v>
       </c>
-      <c r="D280" s="190"/>
-      <c r="E280" s="191"/>
-      <c r="G280" s="189" t="s">
+      <c r="D280" s="199"/>
+      <c r="E280" s="200"/>
+      <c r="G280" s="198" t="s">
         <v>199</v>
       </c>
-      <c r="H280" s="190"/>
-      <c r="I280" s="191"/>
+      <c r="H280" s="199"/>
+      <c r="I280" s="200"/>
     </row>
     <row r="281" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A281" s="81" t="s">
@@ -12693,7 +12680,7 @@
     <row r="305" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="306" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A306" s="127" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C306" s="114" t="s">
         <v>231</v>
@@ -12704,7 +12691,7 @@
     </row>
     <row r="307" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A307" s="125" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C307" s="180">
         <f>E302-MAX(G277:K277)</f>
@@ -12717,7 +12704,7 @@
     </row>
     <row r="308" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A308" s="126" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C308" s="60">
         <f>E302-MIN(G276:K276)</f>
@@ -12743,11 +12730,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="76" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12775,7 +12762,7 @@
         <v>54</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J1" s="42" t="s">
         <v>240</v>
@@ -12879,9 +12866,7 @@
       <c r="O5" s="2">
         <v>0.23</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>263</v>
-      </c>
+      <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="32"/>
@@ -13342,7 +13327,7 @@
         <v>15</v>
       </c>
       <c r="O33" s="182"/>
-      <c r="P33" s="188"/>
+      <c r="P33" s="186"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="107" t="s">
@@ -13734,40 +13719,46 @@
       <c r="A48" s="127" t="s">
         <v>258</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>264</v>
-      </c>
+      <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="149" t="s">
         <v>259</v>
       </c>
       <c r="F49" s="136">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="G49" s="137">
-        <v>8</v>
+        <f>18+'Mast + Tower'!B20</f>
+        <v>22</v>
       </c>
       <c r="H49" s="137">
-        <v>8</v>
+        <f>18+'Mast + Tower'!B18</f>
+        <v>24</v>
       </c>
       <c r="I49" s="137">
-        <v>8</v>
+        <f>18+'Mast + Tower'!B18</f>
+        <v>24</v>
       </c>
       <c r="J49" s="137">
-        <v>8</v>
+        <f>18+'Mast + Tower'!B18</f>
+        <v>24</v>
       </c>
       <c r="K49" s="137">
-        <v>8</v>
+        <f>18+'Mast + Tower'!B18</f>
+        <v>24</v>
       </c>
       <c r="L49" s="137">
-        <v>8</v>
+        <f>18+'Mast + Tower'!B18</f>
+        <v>24</v>
       </c>
       <c r="M49" s="137">
-        <v>8</v>
+        <f>18+'Mast + Tower'!B18</f>
+        <v>24</v>
       </c>
       <c r="N49" s="138">
-        <v>8</v>
+        <f>18+'Mast + Tower'!B18</f>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
@@ -13776,39 +13767,39 @@
       </c>
       <c r="F50" s="147">
         <f>F5*F49</f>
-        <v>0.30000000000000004</v>
+        <v>1</v>
       </c>
       <c r="G50" s="21">
         <f>G5*G49</f>
-        <v>0.48</v>
+        <v>1.3199999999999998</v>
       </c>
       <c r="H50" s="21">
         <f>H5*H49</f>
-        <v>0.8</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="I50" s="21">
         <f t="shared" ref="I50:M50" si="4">I5*I49</f>
-        <v>0.8</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="J50" s="21">
         <f t="shared" si="4"/>
-        <v>0.8</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="K50" s="21">
         <f t="shared" si="4"/>
-        <v>0.88</v>
+        <v>2.64</v>
       </c>
       <c r="L50" s="21">
         <f t="shared" si="4"/>
-        <v>0.88</v>
+        <v>2.64</v>
       </c>
       <c r="M50" s="21">
         <f t="shared" si="4"/>
-        <v>0.88</v>
+        <v>2.64</v>
       </c>
       <c r="N50" s="148">
         <f>N5*N49</f>
-        <v>0.88</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13896,39 +13887,39 @@
       </c>
       <c r="F53" s="147">
         <f t="shared" ref="F53:N53" si="5">F52+F50</f>
-        <v>2.7</v>
+        <v>3.4</v>
       </c>
       <c r="G53" s="21">
         <f t="shared" si="5"/>
-        <v>2.58</v>
+        <v>3.42</v>
       </c>
       <c r="H53" s="21">
         <f t="shared" si="5"/>
-        <v>3.8</v>
+        <v>5.4</v>
       </c>
       <c r="I53" s="21">
         <f t="shared" si="5"/>
-        <v>3.3</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="J53" s="21">
         <f t="shared" si="5"/>
-        <v>2.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K53" s="21">
         <f t="shared" si="5"/>
-        <v>2.38</v>
+        <v>4.1400000000000006</v>
       </c>
       <c r="L53" s="21">
         <f t="shared" si="5"/>
-        <v>1.88</v>
+        <v>3.64</v>
       </c>
       <c r="M53" s="21">
         <f t="shared" si="5"/>
-        <v>1.38</v>
+        <v>3.14</v>
       </c>
       <c r="N53" s="148">
         <f t="shared" si="5"/>
-        <v>0.88</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13937,96 +13928,96 @@
       </c>
       <c r="F54" s="139">
         <f t="shared" ref="F54:N54" si="6">F32-F53</f>
-        <v>67.3</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="G54" s="140">
         <f t="shared" si="6"/>
-        <v>55.42</v>
+        <v>54.58</v>
       </c>
       <c r="H54" s="140">
         <f t="shared" si="6"/>
-        <v>46.2</v>
+        <v>44.6</v>
       </c>
       <c r="I54" s="140">
         <f t="shared" si="6"/>
-        <v>46.7</v>
+        <v>45.1</v>
       </c>
       <c r="J54" s="140">
         <f t="shared" si="6"/>
-        <v>47.2</v>
+        <v>45.6</v>
       </c>
       <c r="K54" s="140">
         <f t="shared" si="6"/>
-        <v>47.62</v>
+        <v>45.86</v>
       </c>
       <c r="L54" s="140">
         <f t="shared" si="6"/>
-        <v>48.12</v>
+        <v>46.36</v>
       </c>
       <c r="M54" s="140">
         <f t="shared" si="6"/>
-        <v>48.62</v>
+        <v>46.86</v>
       </c>
       <c r="N54" s="141">
         <f t="shared" si="6"/>
-        <v>49.12</v>
+        <v>47.36</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="56" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="127" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="149" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F58" s="136">
         <f>F44-(F32-F53)</f>
-        <v>35.100000000000009</v>
+        <v>35.800000000000011</v>
       </c>
       <c r="G58" s="137">
         <f>G44-(G32-G53)</f>
-        <v>44.679999999999993</v>
+        <v>45.519999999999996</v>
       </c>
       <c r="H58" s="137">
         <f>H44-(H32-H53)</f>
-        <v>60.8</v>
+        <v>62.4</v>
       </c>
       <c r="I58" s="137">
         <f>I44-(I32-I53)</f>
-        <v>59.8</v>
+        <v>61.4</v>
       </c>
       <c r="J58" s="137">
         <f t="shared" ref="J58:N58" si="7">J44-(J32-J53)</f>
-        <v>58.8</v>
+        <v>60.4</v>
       </c>
       <c r="K58" s="137">
         <f t="shared" si="7"/>
-        <v>57.88</v>
+        <v>59.64</v>
       </c>
       <c r="L58" s="137">
         <f t="shared" si="7"/>
-        <v>56.88</v>
+        <v>58.64</v>
       </c>
       <c r="M58" s="137">
         <f t="shared" si="7"/>
-        <v>55.88</v>
+        <v>57.64</v>
       </c>
       <c r="N58" s="138">
         <f t="shared" si="7"/>
-        <v>54.88</v>
+        <v>56.64</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="151" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F59" s="164" t="str">
         <f>IF(AND(F16&gt;F58,(F16-F17)&lt;F58),"OK","NO")</f>
@@ -14068,53 +14059,53 @@
     <row r="60" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="61" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="127" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="149" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F62" s="136">
         <f>IF(F58-F24&gt;F16-F17,F58-F24,F16-F17)</f>
-        <v>35.100000000000009</v>
+        <v>35.800000000000011</v>
       </c>
       <c r="G62" s="137">
         <f t="shared" ref="G62:N62" si="9">IF(G58-G24&gt;G16-G17,G58-G24,G16-G17)</f>
-        <v>44.679999999999993</v>
+        <v>45.519999999999996</v>
       </c>
       <c r="H62" s="137">
         <f t="shared" si="9"/>
-        <v>32.799999999999997</v>
+        <v>34.4</v>
       </c>
       <c r="I62" s="137">
         <f>IF(I58-I24&gt;I16-I17,I58-I24,I16-I17)</f>
-        <v>31.799999999999997</v>
+        <v>33.4</v>
       </c>
       <c r="J62" s="137">
         <f t="shared" si="9"/>
-        <v>30.799999999999997</v>
+        <v>32.4</v>
       </c>
       <c r="K62" s="137">
         <f t="shared" si="9"/>
-        <v>29.880000000000003</v>
+        <v>31.64</v>
       </c>
       <c r="L62" s="137">
         <f t="shared" si="9"/>
-        <v>28.880000000000003</v>
+        <v>30.64</v>
       </c>
       <c r="M62" s="137">
         <f t="shared" si="9"/>
-        <v>27.880000000000003</v>
+        <v>29.64</v>
       </c>
       <c r="N62" s="138">
         <f t="shared" si="9"/>
-        <v>26.880000000000003</v>
+        <v>28.64</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="150" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F63" s="147">
         <f>F58-F62</f>
@@ -14156,7 +14147,7 @@
     </row>
     <row r="64" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="151" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F64" s="164" t="str">
         <f>IF(AND(F16&gt;F62,(F16-F17)&lt;F62),"OK","NO")</f>
@@ -14198,12 +14189,12 @@
     <row r="65" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="66" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="171" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="150" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F67" s="136">
         <v>0.15</v>
@@ -14235,7 +14226,7 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="150" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F68" s="147">
         <v>290</v>
@@ -14267,7 +14258,7 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="150" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F69" s="147">
         <v>-13</v>
@@ -14299,7 +14290,7 @@
     </row>
     <row r="70" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="151" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F70" s="139">
         <v>38</v>
@@ -14332,100 +14323,100 @@
     <row r="71" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="172" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="173" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="150" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B74" s="1"/>
       <c r="F74" s="136">
         <f>10*LOG10(10^((F18+F53)/10)+10^((F53-F58)/10)*(10^((F43+Network!H277)/10)-1))</f>
-        <v>16.537205707170102</v>
+        <v>16.779680899642923</v>
       </c>
       <c r="G74" s="137">
         <f>10*LOG10(10^((G18+G53)/10)+10^((G53-G58)/10)*(10^((G43+Network!I277)/10)-1))</f>
-        <v>12.448242010510427</v>
+        <v>13.147592929371502</v>
       </c>
       <c r="H74" s="137">
         <f>10*LOG10(10^((H18+H53)/10)+10^((H53-H58)/10)*(10^((H43+Network!J277)/10)-1))</f>
-        <v>12.837121168044634</v>
+        <v>14.425715360153408</v>
       </c>
       <c r="I74" s="137">
         <f>10*LOG10(10^((I18+I53)/10)+10^((I53-I58)/10)*(10^((I43+Network!J277)/10)-1))</f>
-        <v>12.341628930936814</v>
+        <v>13.928842668311461</v>
       </c>
       <c r="J74" s="137">
         <f>10*LOG10(10^((J18+J53)/10)+10^((J53-J58)/10)*(10^((J43+Network!J277)/10)-1))</f>
-        <v>11.846681144362297</v>
+        <v>13.432348875919986</v>
       </c>
       <c r="K74" s="137">
         <f>10*LOG10(10^((K18+K53)/10)+10^((K53-K58)/10)*(10^((K43+Network!J277)/10)-1))</f>
-        <v>11.431393079318745</v>
+        <v>13.174336724245999</v>
       </c>
       <c r="L74" s="137">
         <f>10*LOG10(10^((L18+L53)/10)+10^((L53-L58)/10)*(10^((L43+Network!K277)/10)-1))</f>
-        <v>11.004322432591573</v>
+        <v>12.723293121364554</v>
       </c>
       <c r="M74" s="137">
         <f>10*LOG10(10^((M18+M53)/10)+10^((M53-M58)/10)*(10^((M43+Network!K277)/10)-1))</f>
-        <v>10.51925115842595</v>
+        <v>12.233347830022003</v>
       </c>
       <c r="N74" s="138">
         <f>10*LOG10(10^((N18+N53)/10)+10^((N53-N58)/10)*(10^((N43+Network!K277)/10)-1))</f>
-        <v>10.035940560689802</v>
+        <v>11.744601729619896</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="150" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F75" s="167">
         <f>F32-F69-10*LOG10(10^((F18+F53)/10)+10^((F53-F58)/10)*(10^((F43+Network!H277)/10)-1))</f>
-        <v>66.462794292829898</v>
+        <v>66.220319100357074</v>
       </c>
       <c r="G75" s="90">
         <f>G32-G69-10*LOG10(10^((G18+G53)/10)+10^((G53-G58)/10)*(10^((G43+Network!I277)/10)-1))</f>
-        <v>48.551757989489573</v>
+        <v>47.852407070628502</v>
       </c>
       <c r="H75" s="90">
         <f>H32-H69-10*LOG10(10^((H18+H53)/10)+10^((H53-H58)/10)*(10^((H43+Network!J277)/10)-1))</f>
-        <v>33.162878831955368</v>
+        <v>31.574284639846592</v>
       </c>
       <c r="I75" s="90">
         <f>I32-I69-10*LOG10(10^((I18+I53)/10)+10^((I53-I58)/10)*(10^((I43+Network!J277)/10)-1))</f>
-        <v>33.658371069063186</v>
+        <v>32.071157331688539</v>
       </c>
       <c r="J75" s="90">
         <f>J32-J69-10*LOG10(10^((J18+J53)/10)+10^((J53-J58)/10)*(10^((J43+Network!J277)/10)-1))</f>
-        <v>34.153318855637707</v>
+        <v>32.567651124080015</v>
       </c>
       <c r="K75" s="90">
         <f>K32-K69-10*LOG10(10^((K18+K53)/10)+10^((K53-K58)/10)*(10^((K43+Network!J277)/10)-1))</f>
-        <v>34.568606920681255</v>
+        <v>32.825663275754003</v>
       </c>
       <c r="L75" s="90">
         <f>L32-L69-10*LOG10(10^((L18+L53)/10)+10^((L53-L58)/10)*(10^((J43+Network!O277)/10)-1))</f>
-        <v>35.119979752503028</v>
+        <v>33.35998649882147</v>
       </c>
       <c r="M75" s="90">
         <f>M32-M69-10*LOG10(10^((M18+M53)/10)+10^((M53-M58)/10)*(10^((J43+Network!P277)/10)-1))</f>
-        <v>35.619999174226699</v>
+        <v>33.859999449368757</v>
       </c>
       <c r="N75" s="169">
         <f>N32-N69-10*LOG10(10^((N18+N53)/10)+10^((N53-N58)/10)*(10^((J43+Network!Q277)/10)-1))</f>
-        <v>36.119998960413028</v>
+        <v>34.35999930679634</v>
       </c>
     </row>
     <row r="76" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="151" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F76" s="164" t="str">
         <f>IF(F75&gt;=F70,"OK","NO")</f>
@@ -14467,95 +14458,95 @@
     <row r="77" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="78" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="171" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="150" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F79" s="136">
         <f>10*LOG10(10^(F26/10)+(10^(F53/10)-1)/10^(F63/10)+(10^(F18/10)-1)*10^(F53/10)/10^(F63/10)+10^((F53-F62-F63)/10)*(10^((F43+Network!H277)/10)-1))</f>
-        <v>16.537205707170102</v>
+        <v>16.779680899642923</v>
       </c>
       <c r="G79" s="137">
         <f>10*LOG10(10^(G26/10)+(10^(G53/10)-1)/10^(G63/10)+(10^(G18/10)-1)*10^(G53/10)/10^(G63/10)+10^((G53-G62-G63)/10)*(10^((G43+Network!I277)/10)-1))</f>
-        <v>12.448242010510429</v>
+        <v>13.147592929371502</v>
       </c>
       <c r="H79" s="137">
         <f>10*LOG10(10^(H26/10)+(10^(H53/10)-1)/10^(H63/10)+(10^(H18/10)-1)*10^(H53/10)/10^(H63/10)+10^((H53-H62-H63)/10)*(10^((H43+Network!J277)/10)-1))</f>
-        <v>6.6829431135643471</v>
+        <v>6.6954645101141157</v>
       </c>
       <c r="I79" s="137">
         <f>10*LOG10(10^(I26/10)+(10^(I53/10)-1)/10^(I63/10)+(10^(I18/10)-1)*10^(I53/10)/10^(I63/10)+10^((I53-I62-I63)/10)*(10^((I43+Network!J277)/10)-1))</f>
-        <v>6.6798804391014315</v>
+        <v>6.6910497575131398</v>
       </c>
       <c r="J79" s="137">
         <f>10*LOG10(10^(J26/10)+(10^(J53/10)-1)/10^(J63/10)+(10^(J18/10)-1)*10^(J53/10)/10^(J63/10)+10^((J53-J62-J63)/10)*(10^((J43+Network!J277)/10)-1))</f>
-        <v>6.6771489537078939</v>
+        <v>6.6871112669985608</v>
       </c>
       <c r="K79" s="137">
         <f>10*LOG10(10^(K26/10)+(10^(K53/10)-1)/10^(K63/10)+(10^(K18/10)-1)*10^(K53/10)/10^(K63/10)+10^((K53-K62-K63)/10)*(10^((K43+Network!J277)/10)-1))</f>
-        <v>6.6750842057365247</v>
+        <v>6.6852341688357919</v>
       </c>
       <c r="L79" s="137">
         <f>10*LOG10(10^(L26/10)+(10^(L53/10)-1)/10^(L63/10)+(10^(L18/10)-1)*10^(L53/10)/10^(L63/10)+10^((L53-L62-L63)/10)*(10^((L43+Network!K277)/10)-1))</f>
-        <v>6.8487120708452345</v>
+        <v>6.8574051682622006</v>
       </c>
       <c r="M79" s="137">
         <f>10*LOG10(10^(M26/10)+(10^(M53/10)-1)/10^(M63/10)+(10^(M18/10)-1)*10^(M53/10)/10^(M63/10)+10^((M53-M62-M63)/10)*(10^((M43+Network!K277)/10)-1))</f>
-        <v>6.8468174917760871</v>
+        <v>6.8545694438043423</v>
       </c>
       <c r="N79" s="138">
         <f>10*LOG10(10^(N26/10)+(10^(N53/10)-1)/10^(N63/10)+(10^(N18/10)-1)*10^(N53/10)/10^(N63/10)+10^((N53-N62-N63)/10)*(10^((N43+Network!K277)/10)-1))</f>
-        <v>6.8451281695987118</v>
+        <v>6.8520404604457941</v>
       </c>
       <c r="O79" s="1"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="150" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F80" s="167">
         <f>F32-F69-10*LOG10(10^(F26/10)+(10^(F53/10)-1)/10^(F63/10)+(10^(F18/10)-1)*10^(F53/10)/10^(F63/10)+10^((F53-F62-F63)/10)*(10^((F43+Network!H277)/10)-1))</f>
-        <v>66.462794292829898</v>
+        <v>66.220319100357074</v>
       </c>
       <c r="G80" s="90">
         <f>G32-G69-10*LOG10(10^(G26/10)+(10^(G53/10)-1)/10^(G63/10)+(10^(G18/10)-1)*10^(G53/10)/10^(G63/10)+10^((G53-G62-G63)/10)*(10^((G43+Network!I277)/10)-1))</f>
-        <v>48.551757989489573</v>
+        <v>47.852407070628502</v>
       </c>
       <c r="H80" s="90">
         <f>H32-H69-10*LOG10(10^(H26/10)+(10^(H53/10)-1)/10^(H63/10)+(10^(H18/10)-1)*10^(H53/10)/10^(H63/10)+10^((H53-H62-H63)/10)*(10^((H43+Network!J277)/10)-1))</f>
-        <v>39.317056886435651</v>
+        <v>39.304535489885886</v>
       </c>
       <c r="I80" s="90">
         <f>I32-I69-10*LOG10(10^(I26/10)+(10^(I53/10)-1)/10^(I63/10)+(10^(I18/10)-1)*10^(I53/10)/10^(I63/10)+10^((I53-I62-I63)/10)*(10^((I43+Network!J277)/10)-1))</f>
-        <v>39.320119560898569</v>
+        <v>39.308950242486858</v>
       </c>
       <c r="J80" s="90">
         <f>J32-J69-10*LOG10(10^(J26/10)+(10^(J53/10)-1)/10^(J63/10)+(10^(J18/10)-1)*10^(J53/10)/10^(J63/10)+10^((J53-J62-J63)/10)*(10^((J43+Network!J277)/10)-1))</f>
-        <v>39.322851046292108</v>
+        <v>39.312888733001436</v>
       </c>
       <c r="K80" s="90">
         <f>K32-K69-10*LOG10(10^(K26/10)+(10^(K53/10)-1)/10^(K63/10)+(10^(K18/10)-1)*10^(K53/10)/10^(K63/10)+10^((K53-K62-K63)/10)*(10^((K43+Network!J277)/10)-1))</f>
-        <v>39.324915794263475</v>
+        <v>39.314765831164209</v>
       </c>
       <c r="L80" s="90">
         <f>L32-L69-10*LOG10(10^(L26/10)+(10^(L53/10)-1)/10^(L63/10)+(10^(L18/10)-1)*10^(L53/10)/10^(L63/10)+10^((L53-L62-L63)/10)*(10^((L43+Network!K277)/10)-1))</f>
-        <v>39.151287929154762</v>
+        <v>39.142594831737796</v>
       </c>
       <c r="M80" s="90">
         <f>M32-M69-10*LOG10(10^(M26/10)+(10^(M53/10)-1)/10^(M63/10)+(10^(M18/10)-1)*10^(M53/10)/10^(M63/10)+10^((M53-M62-M63)/10)*(10^((M43+Network!K277)/10)-1))</f>
-        <v>39.153182508223914</v>
+        <v>39.145430556195656</v>
       </c>
       <c r="N80" s="169">
         <f>N32-N69-10*LOG10(10^(N26/10)+(10^(N53/10)-1)/10^(N63/10)+(10^(N18/10)-1)*10^(N53/10)/10^(N63/10)+10^((N53-N62-N63)/10)*(10^((N43+Network!K277)/10)-1))</f>
-        <v>39.154871830401291</v>
+        <v>39.147959539554208</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="151" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F81" s="164" t="str">
         <f>IF(F80&gt;=F70,"OK","NO")</f>
@@ -14706,12 +14697,12 @@
     <row r="89" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="90" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="171" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="156" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H91" s="160">
         <f>H28+2*(H27-H87-H44)</f>
@@ -14748,7 +14739,7 @@
     </row>
     <row r="92" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="126" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H92" s="164" t="str">
         <f>IF(H91&gt;=H88,"OK","NO")</f>
@@ -14783,18 +14774,15 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="O93" s="183"/>
-    </row>
+    <row r="93" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="94" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="171" t="s">
-        <v>269</v>
-      </c>
-      <c r="O94" s="183"/>
+        <v>267</v>
+      </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" s="150" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H95" s="136">
         <f>H32+H63</f>
@@ -14816,7 +14804,7 @@
         <f t="shared" si="16"/>
         <v>78</v>
       </c>
-      <c r="M95" s="184">
+      <c r="M95" s="183">
         <f>M32+M63</f>
         <v>78</v>
       </c>
@@ -14824,11 +14812,10 @@
         <f>N32+N63</f>
         <v>78</v>
       </c>
-      <c r="O95" s="186"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="156" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H96" s="175">
         <f>-20*LOG10(10^(-H91/20)+10^(-(H28+2*(H27-7.5*LOG10(SUM(H86:N86)-1)-H32-H63))/20))</f>
@@ -14839,8 +14826,8 @@
         <v>33.947359360533518</v>
       </c>
       <c r="J96" s="174">
-        <f>-20*LOG10(10^(-J91/20)+10^(-(J28+2*(J27-7.5*LOG10(SUM(I86:O86)-1)-J32-J63))/20))</f>
-        <v>34.799999274861314</v>
+        <f>-20*LOG10(10^(-J91/20)+10^(-(J28+2*(J27-7.5*LOG10(SUM(H86:N86)-1)-J32-J63))/20))</f>
+        <v>34.940958014846672</v>
       </c>
       <c r="K96" s="174">
         <f>-20*LOG10(10^(-K91/20)+10^(-(K28+2*(K27-7.5*LOG10(SUM(H86:N86)-1)-K32-K63))/20))</f>
@@ -14850,7 +14837,7 @@
         <f>-20*LOG10(10^(-L91/20)+10^(-(L28+2*(L27-7.5*LOG10(SUM(H86:N86)-1)-L32-L63))/20))</f>
         <v>36.925735731532804</v>
       </c>
-      <c r="M96" s="185">
+      <c r="M96" s="184">
         <f>-20*LOG10(10^(-M91/20)+10^(-(M28+2*(M27-7.5*LOG10(SUM(H86:N86)-1)-M32-M63))/20))</f>
         <v>37.916717431794545</v>
       </c>
@@ -14858,11 +14845,11 @@
         <f>-20*LOG10(10^(-N91/20)+10^(-(N28+2*(N27-7.5*LOG10(SUM(H86:N86)-1)-N32-N63))/20))</f>
         <v>38.906609867464191</v>
       </c>
-      <c r="O96" s="187"/>
+      <c r="O96" s="185"/>
     </row>
     <row r="97" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="126" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H97" s="164" t="str">
         <f>IF(H96&gt;=H88,"OK","NO")</f>
@@ -14900,10 +14887,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="97" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="97" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -14916,17 +14903,17 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="32"/>
-      <c r="B2" s="192" t="s">
+      <c r="B2" s="201" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="193"/>
+      <c r="C2" s="202"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="197"/>
-      <c r="B3" s="198" t="s">
+      <c r="A3" s="118"/>
+      <c r="B3" s="190" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="198" t="s">
+      <c r="C3" s="190" t="s">
         <v>207</v>
       </c>
     </row>
@@ -14934,10 +14921,10 @@
       <c r="A4" s="119" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="199">
+      <c r="B4" s="191">
         <v>39.49</v>
       </c>
-      <c r="C4" s="199">
+      <c r="C4" s="191">
         <v>39.49</v>
       </c>
     </row>
@@ -14945,104 +14932,104 @@
       <c r="A5" s="119" t="s">
         <v>209</v>
       </c>
-      <c r="B5" s="199">
+      <c r="B5" s="191">
         <v>30</v>
       </c>
-      <c r="C5" s="199">
+      <c r="C5" s="191">
         <v>19.2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="119" t="s">
-        <v>298</v>
-      </c>
-      <c r="B6" s="199">
+        <v>296</v>
+      </c>
+      <c r="B6" s="191">
         <f>30-0.36</f>
         <v>29.64</v>
       </c>
-      <c r="C6" s="199">
+      <c r="C6" s="191">
         <f>-C5-0.36</f>
         <v>-19.559999999999999</v>
       </c>
-      <c r="F6" s="194"/>
-      <c r="G6" s="194"/>
+      <c r="F6" s="187"/>
+      <c r="G6" s="187"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="119" t="s">
-        <v>292</v>
-      </c>
-      <c r="B7" s="200">
+        <v>290</v>
+      </c>
+      <c r="B7" s="192">
         <f>DEGREES(ACOS(COS(RADIANS(B6))*COS(RADIANS(B4))))</f>
         <v>47.874722541842957</v>
       </c>
-      <c r="C7" s="200">
+      <c r="C7" s="192">
         <f>DEGREES(ACOS(COS(RADIANS(C6))*COS(RADIANS(C4))))</f>
         <v>43.347844323707463</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="119" t="s">
-        <v>293</v>
-      </c>
-      <c r="B8" s="199">
+        <v>291</v>
+      </c>
+      <c r="B8" s="191">
         <v>6378.16</v>
       </c>
-      <c r="C8" s="199">
+      <c r="C8" s="191">
         <v>6378.16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="119" t="s">
-        <v>294</v>
-      </c>
-      <c r="B9" s="199">
+        <v>292</v>
+      </c>
+      <c r="B9" s="191">
         <v>35786.300000000003</v>
       </c>
-      <c r="C9" s="199">
+      <c r="C9" s="191">
         <v>35786.300000000003</v>
       </c>
-      <c r="F9" s="196"/>
-      <c r="G9" s="196"/>
+      <c r="F9" s="189"/>
+      <c r="G9" s="189"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="119" t="s">
-        <v>295</v>
-      </c>
-      <c r="B10" s="201">
+        <v>293</v>
+      </c>
+      <c r="B10" s="193">
         <f>DEGREES(ATAN((COS(RADIANS(B7))-B8/(B9+B8))/SIN(RADIANS(B7))))</f>
         <v>35.008051729265496</v>
       </c>
-      <c r="C10" s="201">
+      <c r="C10" s="193">
         <f>DEGREES(ATAN((COS(RADIANS(C7))-B8/(B9+B8))/SIN(RADIANS(C7))))</f>
         <v>39.997625557419383</v>
       </c>
-      <c r="F10" s="194"/>
-      <c r="G10" s="194"/>
+      <c r="F10" s="187"/>
+      <c r="G10" s="187"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="119" t="s">
-        <v>296</v>
-      </c>
-      <c r="B11" s="200">
+        <v>294</v>
+      </c>
+      <c r="B11" s="192">
         <f>180 + DEGREES(ATAN(TAN(RADIANS(B6))/SIN(RADIANS(B4))))</f>
         <v>221.82020731856079</v>
       </c>
-      <c r="C11" s="200">
+      <c r="C11" s="192">
         <f>180 + DEGREES(ATAN(TAN(RADIANS(C6))/SIN(RADIANS(C4))))</f>
         <v>150.80819109153012</v>
       </c>
-      <c r="F11" s="194"/>
-      <c r="G11" s="195"/>
+      <c r="F11" s="187"/>
+      <c r="G11" s="188"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="119" t="s">
-        <v>297</v>
-      </c>
-      <c r="B12" s="200">
+        <v>295</v>
+      </c>
+      <c r="B12" s="192">
         <f>B9*SQRT(1+((2*B8*(B8+B9))/POWER(B9,2)*(1-COS(RADIANS(B7)))))</f>
         <v>38180.475101277909</v>
       </c>
-      <c r="C12" s="202">
+      <c r="C12" s="194">
         <f>C9*SQRT(1+((2*C8*(C8+C9))/POWER(C9,2)*(1-COS(RADIANS(C7)))))</f>
         <v>37780.795202936883</v>
       </c>
@@ -15242,7 +15229,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="119" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B32" s="121">
         <f>B31/(PI()*SQRT(B16))</f>
@@ -15267,41 +15254,41 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="204" t="s">
-        <v>344</v>
-      </c>
-      <c r="B34" s="205">
+      <c r="A34" s="196" t="s">
+        <v>341</v>
+      </c>
+      <c r="B34" s="197">
         <f>B15-B23-B22+B28</f>
         <v>-120.25640177870341</v>
       </c>
-      <c r="C34" s="205">
+      <c r="C34" s="197">
         <f>C15-C23-C22+C28</f>
         <v>-120.25640177870341</v>
       </c>
-      <c r="D34" s="203"/>
-      <c r="E34" s="203"/>
-      <c r="F34" s="203"/>
-      <c r="G34" s="203">
+      <c r="D34" s="195"/>
+      <c r="E34" s="195"/>
+      <c r="F34" s="195"/>
+      <c r="G34" s="195">
         <f>(G13-G21-G22+G30)-G29</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>343</v>
-      </c>
-      <c r="B35" s="203">
+        <v>340</v>
+      </c>
+      <c r="B35" s="195">
         <f>(B15-B23-B22+B28)-B27</f>
         <v>14</v>
       </c>
-      <c r="C35" s="203">
+      <c r="C35" s="195">
         <f>(C15-C23-C22+C28)-C27</f>
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B36">
         <f>B34+60-(29.6*0.2)</f>
@@ -15314,7 +15301,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B37">
         <f>SQRT(POWER(10,(B36/10))*75)*1000000</f>
@@ -15327,7 +15314,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B38">
         <f>20*LOG10(B37)</f>
@@ -15340,7 +15327,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B40">
         <f>123-B38</f>
@@ -15361,99 +15348,101 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView topLeftCell="A6" zoomScale="126" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="38.21875" customWidth="1"/>
     <col min="7" max="7" width="17.44140625" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B2">
         <f>B3*B6</f>
         <v>523.20000000000005</v>
       </c>
       <c r="E2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B3">
         <f>((B4)^2/16)*B5</f>
         <v>799.52256944444457</v>
       </c>
       <c r="E3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B4">
         <f>130*(1000/3600)</f>
         <v>36.111111111111114</v>
       </c>
       <c r="E4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F4">
         <v>0.27200000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B5">
         <v>9.81</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B6">
         <f>523.2/B3</f>
         <v>0.65439053254437862</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B9">
         <v>4.4999999999999998E-2</v>
@@ -15462,9 +15451,9 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -15473,9 +15462,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B11">
         <v>0.7</v>
@@ -15484,9 +15473,9 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B12">
         <f>B9*B10*B11</f>
@@ -15497,9 +15486,9 @@
         <v>9.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B13">
         <f>800*B12</f>
@@ -15510,32 +15499,29 @@
         <v>75.599999999999994</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E16" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="K16" t="s">
-        <v>336</v>
-      </c>
-      <c r="L16" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B17">
         <v>93</v>
@@ -15561,7 +15547,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -15572,13 +15558,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B19">
         <v>36.5</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:C23" si="0">B19*B20</f>
+        <f t="shared" ref="C19" si="0">B19*B20</f>
         <v>146</v>
       </c>
       <c r="E19">
@@ -15598,7 +15584,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -15609,7 +15595,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B21">
         <v>27</v>
@@ -15635,7 +15621,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -15646,7 +15632,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B23">
         <v>523.20000000000005</v>
@@ -15672,7 +15658,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B24">
         <v>0.5</v>
@@ -15685,7 +15671,7 @@
         <v>75.599999999999994</v>
       </c>
       <c r="I24" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="K24">
         <f>2*B5</f>
@@ -15700,7 +15686,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B26">
         <f>SUM(C17,C19,C21,C23)</f>
@@ -15711,7 +15697,7 @@
         <v>1019.6</v>
       </c>
       <c r="H26" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I26">
         <f>-SUM(H17,H19,H21,H23,H24)</f>
@@ -15724,7 +15710,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B27">
         <f>0.045*280*((B10)^2-(3)^2)</f>
@@ -15737,7 +15723,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B28">
         <f>B26+B27</f>
@@ -15750,14 +15736,14 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B29">
         <f>B28-355</f>
         <v>1004.8</v>
       </c>
       <c r="C29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E29">
         <f>E28-355</f>
@@ -15766,15 +15752,15 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E33" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E34" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios despues de exponer
</commit_message>
<xml_diff>
--- a/3C/ITSIT/CTI3.xlsx
+++ b/3C/ITSIT/CTI3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\Máster UPV\2º curso\ITSIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Network" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="343">
   <si>
     <t>TECHNICAL CHARACTERISTICS OF ELEMENTS FROM CATALOGUE</t>
   </si>
@@ -622,9 +622,6 @@
     <t>k (J/K)</t>
   </si>
   <si>
-    <t>Usaremos el amplificador TECATEL 40dB 13/18v</t>
-  </si>
-  <si>
     <t>HEADEND ADJUSTING</t>
   </si>
   <si>
@@ -904,9 +901,6 @@
     <t>Area efectiva viento(m2)</t>
   </si>
   <si>
-    <t>Momento antena (Nm)</t>
-  </si>
-  <si>
     <t>carga_viento (N)</t>
   </si>
   <si>
@@ -937,9 +931,6 @@
     <t>Ma&gt;Mtotal-Mmastil</t>
   </si>
   <si>
-    <t>Ma&lt;Mtotal-Mmastil</t>
-  </si>
-  <si>
     <t>MOMENTO FLECTOR  MASTIL</t>
   </si>
   <si>
@@ -958,9 +949,6 @@
     <t>EIRP (dBW)</t>
   </si>
   <si>
-    <t>MOMENTO FLECTOR TORRETA-MASTIL*</t>
-  </si>
-  <si>
     <t>F_horizontal</t>
   </si>
   <si>
@@ -1064,6 +1052,21 @@
   </si>
   <si>
     <t>ATTENUATION OF DISPERSION+INTERIOR. BEST AND WORST OUTLET ON EACH FLOOR (dB)</t>
+  </si>
+  <si>
+    <t>MOMENTO FLECTOR BASE MASTIL</t>
+  </si>
+  <si>
+    <t>MOMENTO FLECTOR BASE TORRE</t>
+  </si>
+  <si>
+    <t>Es menor que 5108 Nm, cumple</t>
+  </si>
+  <si>
+    <t>SE PODRIA COGER UN MASTIL DE 1,5M DE LONGITUD Y CUMPLIRIA</t>
+  </si>
+  <si>
+    <t>NO CUMPLE HABRIA QUE REDUCIR DISTANCIA ENTRE ANTENAS (4,5 3 y 1,5)</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1077,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1143,15 +1146,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="23">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1263,18 +1259,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2015,26 +1999,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -2045,11 +2009,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2491,31 +2477,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2524,7 +2495,6 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2532,6 +2502,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2555,19 +2534,44 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2897,7 +2901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="M294" activeCellId="1" sqref="A326 M294"/>
     </sheetView>
   </sheetViews>
@@ -3246,7 +3250,7 @@
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="28" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="30"/>
@@ -3330,8 +3334,8 @@
         <f>($D19*O$6)+D$11+(E$19*O$5)+D$13</f>
         <v>5.335</v>
       </c>
-      <c r="P19" s="215" t="s">
-        <v>339</v>
+      <c r="P19" s="209" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3377,7 +3381,7 @@
         <f>($D20*O$6)+D$11+(E$19*O$5)+D$13</f>
         <v>4.99</v>
       </c>
-      <c r="P20" s="215"/>
+      <c r="P20" s="209"/>
     </row>
     <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="55" t="s">
@@ -3422,7 +3426,7 @@
         <f>($D21*O$6)+D$11+(E$19*O$5)+D$13</f>
         <v>4.53</v>
       </c>
-      <c r="P21" s="215"/>
+      <c r="P21" s="209"/>
     </row>
     <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="55" t="s">
@@ -3467,8 +3471,8 @@
         <f t="shared" ref="O22:O23" si="4">($D22*O$6)+D$11+(E$19*O$5)+D$13</f>
         <v>3.0350000000000001</v>
       </c>
-      <c r="P22" s="215" t="s">
-        <v>338</v>
+      <c r="P22" s="209" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3514,13 +3518,13 @@
         <f t="shared" si="4"/>
         <v>4.76</v>
       </c>
-      <c r="P23" s="215"/>
+      <c r="P23" s="209"/>
     </row>
     <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="52"/>
       <c r="N24" s="91"/>
       <c r="O24" s="91"/>
-      <c r="P24" s="215"/>
+      <c r="P24" s="209"/>
     </row>
     <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="54" t="s">
@@ -3568,8 +3572,8 @@
         <f>($D25*O$6)+D$11+(E$25*O$5)+D$13</f>
         <v>5.335</v>
       </c>
-      <c r="P25" s="215" t="s">
-        <v>339</v>
+      <c r="P25" s="209" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3615,7 +3619,7 @@
         <f t="shared" ref="O26:O29" si="9">($D26*O$6)+D$11+(E$25*O$5)+D$13</f>
         <v>4.53</v>
       </c>
-      <c r="P26" s="215"/>
+      <c r="P26" s="209"/>
     </row>
     <row r="27" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="55" t="s">
@@ -3660,11 +3664,11 @@
         <f t="shared" si="9"/>
         <v>4.53</v>
       </c>
-      <c r="P27" s="215"/>
+      <c r="P27" s="209"/>
     </row>
     <row r="28" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="55" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D28" s="59">
         <v>2</v>
@@ -3705,8 +3709,8 @@
         <f t="shared" si="9"/>
         <v>3.0350000000000001</v>
       </c>
-      <c r="P28" s="215" t="s">
-        <v>338</v>
+      <c r="P28" s="209" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3752,13 +3756,13 @@
         <f t="shared" si="9"/>
         <v>4.76</v>
       </c>
-      <c r="P29" s="215"/>
+      <c r="P29" s="209"/>
     </row>
     <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="52"/>
       <c r="N30" s="91"/>
       <c r="O30" s="91"/>
-      <c r="P30" s="215"/>
+      <c r="P30" s="209"/>
     </row>
     <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="54" t="s">
@@ -3806,7 +3810,7 @@
         <f>($D31*O$6)+D$12+(E$31*O$5)+D$13</f>
         <v>4.3000000000000007</v>
       </c>
-      <c r="P31" s="215"/>
+      <c r="P31" s="209"/>
     </row>
     <row r="32" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="55" t="s">
@@ -3851,7 +3855,7 @@
         <f>($D32*O$6)+D$12+(E$31*O$5)+D$13</f>
         <v>6.37</v>
       </c>
-      <c r="P32" s="215"/>
+      <c r="P32" s="209"/>
     </row>
     <row r="33" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="55" t="s">
@@ -3897,7 +3901,7 @@
         <f t="shared" ref="O33:O36" si="18">($D33*O$6)+D$12+(E$31*O$5)+D$13</f>
         <v>4.1850000000000005</v>
       </c>
-      <c r="P33" s="215"/>
+      <c r="P33" s="209"/>
     </row>
     <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="55" t="s">
@@ -3942,13 +3946,13 @@
         <f t="shared" si="18"/>
         <v>6.6000000000000005</v>
       </c>
-      <c r="P34" s="215" t="s">
-        <v>339</v>
+      <c r="P34" s="209" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="55" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D35" s="61">
         <v>13</v>
@@ -3989,7 +3993,7 @@
         <f t="shared" si="18"/>
         <v>4.1850000000000005</v>
       </c>
-      <c r="P35" s="215"/>
+      <c r="P35" s="209"/>
     </row>
     <row r="36" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="56" t="s">
@@ -4034,15 +4038,15 @@
         <f t="shared" si="18"/>
         <v>3.15</v>
       </c>
-      <c r="P36" s="215" t="s">
-        <v>338</v>
+      <c r="P36" s="209" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="52"/>
       <c r="N37" s="91"/>
       <c r="O37" s="91"/>
-      <c r="P37" s="215"/>
+      <c r="P37" s="209"/>
     </row>
     <row r="38" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="54" t="s">
@@ -4090,7 +4094,7 @@
         <f>($D38*O$6)+D$12+(E$38*O$5)+D$13</f>
         <v>4.3000000000000007</v>
       </c>
-      <c r="P38" s="215"/>
+      <c r="P38" s="209"/>
     </row>
     <row r="39" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="55" t="s">
@@ -4135,7 +4139,7 @@
         <f t="shared" ref="O39:O43" si="26">($D39*O$6)+D$12+(E$38*O$5)+D$13</f>
         <v>6.37</v>
       </c>
-      <c r="P39" s="215"/>
+      <c r="P39" s="209"/>
     </row>
     <row r="40" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="55" t="s">
@@ -4180,7 +4184,7 @@
         <f t="shared" si="26"/>
         <v>4.1850000000000005</v>
       </c>
-      <c r="P40" s="215"/>
+      <c r="P40" s="209"/>
     </row>
     <row r="41" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="55" t="s">
@@ -4225,13 +4229,13 @@
         <f t="shared" si="26"/>
         <v>6.6000000000000005</v>
       </c>
-      <c r="P41" s="215" t="s">
-        <v>339</v>
+      <c r="P41" s="209" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="55" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D42" s="61">
         <v>13</v>
@@ -4272,7 +4276,7 @@
         <f t="shared" si="26"/>
         <v>4.1850000000000005</v>
       </c>
-      <c r="P42" s="215"/>
+      <c r="P42" s="209"/>
     </row>
     <row r="43" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="56" t="s">
@@ -4317,15 +4321,15 @@
         <f t="shared" si="26"/>
         <v>3.15</v>
       </c>
-      <c r="P43" s="215" t="s">
-        <v>338</v>
+      <c r="P43" s="209" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="52"/>
       <c r="N44" s="91"/>
       <c r="O44" s="91"/>
-      <c r="P44" s="215"/>
+      <c r="P44" s="209"/>
     </row>
     <row r="45" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="54" t="s">
@@ -4373,8 +4377,8 @@
         <f>($D45*O$6)+D$11+(E$45*O$5)+D$13</f>
         <v>5.335</v>
       </c>
-      <c r="P45" s="215" t="s">
-        <v>339</v>
+      <c r="P45" s="209" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4420,7 +4424,7 @@
         <f t="shared" ref="O46:O49" si="35">($D46*O$6)+D$11+(E$45*O$5)+D$13</f>
         <v>4.99</v>
       </c>
-      <c r="P46" s="215"/>
+      <c r="P46" s="209"/>
     </row>
     <row r="47" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="55" t="s">
@@ -4465,7 +4469,7 @@
         <f t="shared" si="35"/>
         <v>4.53</v>
       </c>
-      <c r="P47" s="215"/>
+      <c r="P47" s="209"/>
     </row>
     <row r="48" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="55" t="s">
@@ -4510,8 +4514,8 @@
         <f t="shared" si="35"/>
         <v>3.0350000000000001</v>
       </c>
-      <c r="P48" s="215" t="s">
-        <v>338</v>
+      <c r="P48" s="209" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4557,13 +4561,13 @@
         <f t="shared" si="35"/>
         <v>4.76</v>
       </c>
-      <c r="P49" s="215"/>
+      <c r="P49" s="209"/>
     </row>
     <row r="50" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="52"/>
       <c r="N50" s="91"/>
       <c r="O50" s="91"/>
-      <c r="P50" s="215"/>
+      <c r="P50" s="209"/>
     </row>
     <row r="51" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="54" t="s">
@@ -4611,8 +4615,8 @@
         <f>($D51*O$6)+D$11+(E$51*O$5)+D$13</f>
         <v>5.335</v>
       </c>
-      <c r="P51" s="215" t="s">
-        <v>339</v>
+      <c r="P51" s="209" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4658,7 +4662,7 @@
         <f t="shared" ref="O52:O55" si="42">($D52*O$6)+D$11+(E$51*O$5)+D$13</f>
         <v>4.53</v>
       </c>
-      <c r="P52" s="215"/>
+      <c r="P52" s="209"/>
     </row>
     <row r="53" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="55" t="s">
@@ -4703,9 +4707,9 @@
         <f t="shared" si="42"/>
         <v>4.53</v>
       </c>
-      <c r="P53" s="215"/>
-      <c r="Q53" s="215" t="s">
-        <v>340</v>
+      <c r="P53" s="209"/>
+      <c r="Q53" s="209" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4751,8 +4755,8 @@
         <f t="shared" si="42"/>
         <v>3.0350000000000001</v>
       </c>
-      <c r="P54" s="215" t="s">
-        <v>338</v>
+      <c r="P54" s="209" t="s">
+        <v>334</v>
       </c>
       <c r="Q54">
         <f>(D54*N6)+(E51*N5)</f>
@@ -4802,13 +4806,13 @@
         <f t="shared" si="42"/>
         <v>4.76</v>
       </c>
-      <c r="P55" s="215"/>
+      <c r="P55" s="209"/>
     </row>
     <row r="56" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="52"/>
       <c r="N56" s="91"/>
       <c r="O56" s="91"/>
-      <c r="P56" s="215"/>
+      <c r="P56" s="209"/>
     </row>
     <row r="57" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="54" t="s">
@@ -4856,7 +4860,7 @@
         <f>($D57*O$6)+D$12+(E$57*O$5)+D$13</f>
         <v>4.3000000000000007</v>
       </c>
-      <c r="P57" s="215"/>
+      <c r="P57" s="209"/>
     </row>
     <row r="58" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="55" t="s">
@@ -4901,7 +4905,7 @@
         <f t="shared" ref="O58:O62" si="51">($D58*O$6)+D$12+(E$57*O$5)+D$13</f>
         <v>6.37</v>
       </c>
-      <c r="P58" s="215"/>
+      <c r="P58" s="209"/>
     </row>
     <row r="59" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="55" t="s">
@@ -4946,9 +4950,9 @@
         <f t="shared" si="51"/>
         <v>4.1850000000000005</v>
       </c>
-      <c r="P59" s="215"/>
-      <c r="Q59" s="215" t="s">
-        <v>340</v>
+      <c r="P59" s="209"/>
+      <c r="Q59" s="209" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4994,8 +4998,8 @@
         <f>($D60*O$6)+D$12+(E$57*O$5)+D$13</f>
         <v>6.6000000000000005</v>
       </c>
-      <c r="P60" s="215" t="s">
-        <v>339</v>
+      <c r="P60" s="209" t="s">
+        <v>335</v>
       </c>
       <c r="Q60">
         <f>(D60*N5)+(E57*N6)</f>
@@ -5045,7 +5049,7 @@
         <f t="shared" si="51"/>
         <v>4.1850000000000005</v>
       </c>
-      <c r="P61" s="215"/>
+      <c r="P61" s="209"/>
     </row>
     <row r="62" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="56" t="s">
@@ -5090,15 +5094,15 @@
         <f t="shared" si="51"/>
         <v>3.15</v>
       </c>
-      <c r="P62" s="215" t="s">
-        <v>338</v>
+      <c r="P62" s="209" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="52"/>
       <c r="N63" s="91"/>
       <c r="O63" s="91"/>
-      <c r="P63" s="215"/>
+      <c r="P63" s="209"/>
     </row>
     <row r="64" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="54" t="s">
@@ -5146,7 +5150,7 @@
         <f>($D64*O$6)+D$12+(E$64*O$5)+D$13</f>
         <v>4.3000000000000007</v>
       </c>
-      <c r="P64" s="215"/>
+      <c r="P64" s="209"/>
     </row>
     <row r="65" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="55" t="s">
@@ -5191,7 +5195,7 @@
         <f t="shared" ref="O65:O69" si="60">($D65*O$6)+D$12+(E$64*O$5)+D$13</f>
         <v>6.37</v>
       </c>
-      <c r="P65" s="215"/>
+      <c r="P65" s="209"/>
     </row>
     <row r="66" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="55" t="s">
@@ -5236,7 +5240,7 @@
         <f t="shared" si="60"/>
         <v>4.1850000000000005</v>
       </c>
-      <c r="P66" s="215"/>
+      <c r="P66" s="209"/>
     </row>
     <row r="67" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="55" t="s">
@@ -5281,13 +5285,13 @@
         <f t="shared" si="60"/>
         <v>6.37</v>
       </c>
-      <c r="P67" s="215" t="s">
-        <v>339</v>
+      <c r="P67" s="209" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="68" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="55" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D68" s="61">
         <v>13</v>
@@ -5328,7 +5332,7 @@
         <f t="shared" si="60"/>
         <v>4.1850000000000005</v>
       </c>
-      <c r="P68" s="215"/>
+      <c r="P68" s="209"/>
     </row>
     <row r="69" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="56" t="s">
@@ -5373,15 +5377,15 @@
         <f t="shared" si="60"/>
         <v>3.15</v>
       </c>
-      <c r="P69" s="215" t="s">
-        <v>338</v>
+      <c r="P69" s="209" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="52"/>
       <c r="N70" s="91"/>
       <c r="O70" s="91"/>
-      <c r="P70" s="215"/>
+      <c r="P70" s="209"/>
     </row>
     <row r="71" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="54" t="s">
@@ -5429,8 +5433,8 @@
         <f>($D71*O$6)+D$11+(E$71*O$5)+D$13</f>
         <v>5.335</v>
       </c>
-      <c r="P71" s="215" t="s">
-        <v>339</v>
+      <c r="P71" s="209" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5476,11 +5480,11 @@
         <f t="shared" ref="O72:O75" si="67">($D72*O$6)+D$11+(E$71*O$5)+D$13</f>
         <v>4.99</v>
       </c>
-      <c r="P72" s="215"/>
+      <c r="P72" s="209"/>
     </row>
     <row r="73" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="55" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D73" s="59">
         <v>15</v>
@@ -5521,11 +5525,11 @@
         <f t="shared" si="67"/>
         <v>4.53</v>
       </c>
-      <c r="P73" s="215"/>
+      <c r="P73" s="209"/>
     </row>
     <row r="74" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="55" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D74" s="59">
         <v>2</v>
@@ -5566,8 +5570,8 @@
         <f t="shared" si="67"/>
         <v>3.0350000000000001</v>
       </c>
-      <c r="P74" s="215" t="s">
-        <v>338</v>
+      <c r="P74" s="209" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="75" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5613,13 +5617,13 @@
         <f t="shared" si="67"/>
         <v>4.76</v>
       </c>
-      <c r="P75" s="215"/>
+      <c r="P75" s="209"/>
     </row>
     <row r="76" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="52"/>
       <c r="N76" s="91"/>
       <c r="O76" s="91"/>
-      <c r="P76" s="215"/>
+      <c r="P76" s="209"/>
     </row>
     <row r="77" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="54" t="s">
@@ -5667,8 +5671,8 @@
         <f>($D77*O$6)+D$11+(E$77*O$5)+D$13</f>
         <v>5.335</v>
       </c>
-      <c r="P77" s="215" t="s">
-        <v>339</v>
+      <c r="P77" s="209" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="78" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5714,11 +5718,11 @@
         <f t="shared" ref="O78:O81" si="74">($D78*O$6)+D$11+(E$77*O$5)+D$13</f>
         <v>4.53</v>
       </c>
-      <c r="P78" s="215"/>
+      <c r="P78" s="209"/>
     </row>
     <row r="79" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="55" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D79" s="59">
         <v>15</v>
@@ -5759,7 +5763,7 @@
         <f t="shared" si="74"/>
         <v>4.53</v>
       </c>
-      <c r="P79" s="215"/>
+      <c r="P79" s="209"/>
     </row>
     <row r="80" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="55" t="s">
@@ -5804,8 +5808,8 @@
         <f t="shared" si="74"/>
         <v>3.0350000000000001</v>
       </c>
-      <c r="P80" s="215" t="s">
-        <v>338</v>
+      <c r="P80" s="209" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="81" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5851,13 +5855,13 @@
         <f t="shared" si="74"/>
         <v>4.76</v>
       </c>
-      <c r="P81" s="215"/>
+      <c r="P81" s="209"/>
     </row>
     <row r="82" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="52"/>
       <c r="N82" s="91"/>
       <c r="O82" s="91"/>
-      <c r="P82" s="215"/>
+      <c r="P82" s="209"/>
     </row>
     <row r="83" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="54" t="s">
@@ -5905,7 +5909,7 @@
         <f>($D83*O$6)+D$12+(E$83*O$5)+D$13</f>
         <v>4.3000000000000007</v>
       </c>
-      <c r="P83" s="215"/>
+      <c r="P83" s="209"/>
     </row>
     <row r="84" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="55" t="s">
@@ -5950,11 +5954,11 @@
         <f t="shared" ref="O84:O87" si="83">($D84*O$6)+D$12+(E$83*O$5)+D$13</f>
         <v>6.37</v>
       </c>
-      <c r="P84" s="215"/>
+      <c r="P84" s="209"/>
     </row>
     <row r="85" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="55" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B85" s="52"/>
       <c r="C85" s="52"/>
@@ -5999,11 +6003,11 @@
         <f t="shared" si="83"/>
         <v>4.1850000000000005</v>
       </c>
-      <c r="P85" s="215"/>
+      <c r="P85" s="209"/>
     </row>
     <row r="86" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="55" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B86" s="52"/>
       <c r="C86" s="52"/>
@@ -6048,8 +6052,8 @@
         <f t="shared" si="83"/>
         <v>6.6000000000000005</v>
       </c>
-      <c r="P86" s="215" t="s">
-        <v>339</v>
+      <c r="P86" s="209" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="87" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6099,7 +6103,7 @@
         <f t="shared" si="83"/>
         <v>4.1850000000000005</v>
       </c>
-      <c r="P87" s="215"/>
+      <c r="P87" s="209"/>
     </row>
     <row r="88" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="56" t="s">
@@ -6148,8 +6152,8 @@
         <f>($D88*O$6)+D$12+(E$83*O$5)+D$13</f>
         <v>3.15</v>
       </c>
-      <c r="P88" s="215" t="s">
-        <v>338</v>
+      <c r="P88" s="209" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6268,7 +6272,7 @@
     </row>
     <row r="92" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="55" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D92" s="59">
         <v>13</v>
@@ -6312,7 +6316,7 @@
     </row>
     <row r="93" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="55" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D93" s="59">
         <v>32</v>
@@ -6354,7 +6358,7 @@
         <v>6.37</v>
       </c>
       <c r="P93" s="52" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="94" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6445,7 +6449,7 @@
         <v>3.15</v>
       </c>
       <c r="P95" s="52" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="96" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6499,7 +6503,7 @@
         <v>5.335</v>
       </c>
       <c r="P97" s="52" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="98" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6548,7 +6552,7 @@
     </row>
     <row r="99" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="55" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D99" s="59">
         <v>15</v>
@@ -6634,7 +6638,7 @@
         <v>3.0350000000000001</v>
       </c>
       <c r="P100" s="52" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="101" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6732,7 +6736,7 @@
         <v>5.335</v>
       </c>
       <c r="P103" s="52" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="104" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6781,7 +6785,7 @@
     </row>
     <row r="105" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="55" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D105" s="59">
         <v>15</v>
@@ -6867,7 +6871,7 @@
         <v>3.0350000000000001</v>
       </c>
       <c r="P106" s="52" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="107" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7011,7 +7015,7 @@
     </row>
     <row r="111" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="55" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D111" s="59">
         <v>13</v>
@@ -7055,7 +7059,7 @@
     </row>
     <row r="112" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="55" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D112" s="59">
         <v>34</v>
@@ -7097,7 +7101,7 @@
         <v>6.6000000000000005</v>
       </c>
       <c r="P112" s="52" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="113" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7188,7 +7192,7 @@
         <v>3.15</v>
       </c>
       <c r="P114" s="52" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="115" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7288,7 +7292,7 @@
     </row>
     <row r="118" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A118" s="55" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D118" s="59">
         <v>13</v>
@@ -7332,7 +7336,7 @@
     </row>
     <row r="119" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A119" s="55" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D119" s="59">
         <v>34</v>
@@ -7374,12 +7378,12 @@
         <v>6.6000000000000005</v>
       </c>
       <c r="P119" s="52" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="120" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="55" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D120" s="61">
         <v>13</v>
@@ -7465,7 +7469,7 @@
         <v>3.15</v>
       </c>
       <c r="P121" s="52" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="122" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7519,7 +7523,7 @@
         <v>3.7250000000000001</v>
       </c>
       <c r="P123" s="52" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="124" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7614,7 +7618,7 @@
         <v>4.53</v>
       </c>
       <c r="P125" s="52" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="126" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.35">
@@ -10829,7 +10833,7 @@
     </row>
     <row r="225" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A225" s="55" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G225" s="58">
         <f t="shared" si="190"/>
@@ -10870,7 +10874,7 @@
     </row>
     <row r="226" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A226" s="55" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G226" s="58">
         <f t="shared" si="190"/>
@@ -11037,7 +11041,7 @@
     </row>
     <row r="231" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A231" s="55" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="G231" s="58">
         <f t="shared" si="196"/>
@@ -11245,7 +11249,7 @@
     </row>
     <row r="237" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A237" s="55" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="G237" s="58">
         <f t="shared" si="202"/>
@@ -11286,7 +11290,7 @@
     </row>
     <row r="238" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A238" s="55" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G238" s="58">
         <f t="shared" si="202"/>
@@ -11494,7 +11498,7 @@
     </row>
     <row r="244" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A244" s="55" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="G244" s="58">
         <f t="shared" si="210"/>
@@ -11535,7 +11539,7 @@
     </row>
     <row r="245" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A245" s="55" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="G245" s="58">
         <f t="shared" si="210"/>
@@ -11743,7 +11747,7 @@
     </row>
     <row r="251" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A251" s="55" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="G251" s="58">
         <f t="shared" si="216"/>
@@ -11951,7 +11955,7 @@
     </row>
     <row r="257" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A257" s="55" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="G257" s="58">
         <f t="shared" si="222"/>
@@ -12159,7 +12163,7 @@
     </row>
     <row r="263" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A263" s="55" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G263" s="58">
         <f t="shared" si="232"/>
@@ -12200,7 +12204,7 @@
     </row>
     <row r="264" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A264" s="55" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G264" s="58">
         <f t="shared" si="232"/>
@@ -12408,7 +12412,7 @@
     </row>
     <row r="270" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A270" s="55" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="G270" s="58">
         <f t="shared" si="241"/>
@@ -12449,7 +12453,7 @@
     </row>
     <row r="271" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A271" s="55" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="G271" s="58">
         <f t="shared" si="241"/>
@@ -12490,7 +12494,7 @@
     </row>
     <row r="272" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A272" s="55" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="G272" s="58">
         <f t="shared" si="241"/>
@@ -12661,16 +12665,16 @@
       <c r="A280" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="C280" s="216" t="s">
+      <c r="C280" s="213" t="s">
         <v>170</v>
       </c>
-      <c r="D280" s="217"/>
-      <c r="E280" s="218"/>
-      <c r="G280" s="216" t="s">
+      <c r="D280" s="214"/>
+      <c r="E280" s="215"/>
+      <c r="G280" s="213" t="s">
         <v>171</v>
       </c>
-      <c r="H280" s="217"/>
-      <c r="I280" s="218"/>
+      <c r="H280" s="214"/>
+      <c r="I280" s="215"/>
     </row>
     <row r="281" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A281" s="81" t="s">
@@ -12785,10 +12789,10 @@
     <row r="286" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="287" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C287" s="114" t="s">
+        <v>195</v>
+      </c>
+      <c r="D287" s="114" t="s">
         <v>196</v>
-      </c>
-      <c r="D287" s="114" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="288" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -12815,12 +12819,12 @@
     <row r="290" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="291" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A291" s="114" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="292" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A292" s="78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="293" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -12831,7 +12835,7 @@
         <v>49</v>
       </c>
       <c r="E293" s="128" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F293" s="129" t="s">
         <v>50</v>
@@ -12839,7 +12843,7 @@
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A294" s="124" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C294" s="130">
         <v>40</v>
@@ -12856,7 +12860,7 @@
     </row>
     <row r="295" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A295" s="125" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C295" s="132">
         <v>70</v>
@@ -12874,12 +12878,12 @@
     <row r="296" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="297" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A297" s="126" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A298" s="124" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C298" s="135">
         <f>MAX(H167:H273)+C294</f>
@@ -12900,7 +12904,7 @@
     </row>
     <row r="299" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A299" s="125" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C299" s="138">
         <f>MIN(H167:H273)+C295</f>
@@ -12922,7 +12926,7 @@
     <row r="300" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="301" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A301" s="78" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C301" s="141">
         <f>0.25*C298+0.75*C299</f>
@@ -12943,7 +12947,7 @@
     </row>
     <row r="302" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A302" s="78" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C302" s="146">
         <v>100</v>
@@ -12960,28 +12964,28 @@
     </row>
     <row r="303" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A303" s="78" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C303" s="176" t="s">
+        <v>208</v>
+      </c>
+      <c r="D303" s="177" t="s">
         <v>209</v>
       </c>
-      <c r="D303" s="177" t="s">
+      <c r="E303" s="177" t="s">
         <v>210</v>
       </c>
-      <c r="E303" s="177" t="s">
+      <c r="F303" s="178" t="s">
         <v>211</v>
-      </c>
-      <c r="F303" s="178" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="306" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A306" s="126" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C306" s="114" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D306" s="104" t="s">
         <v>50</v>
@@ -12989,7 +12993,7 @@
     </row>
     <row r="307" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A307" s="124" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C307" s="179">
         <f>E302-MAX(G277:K277)</f>
@@ -13002,7 +13006,7 @@
     </row>
     <row r="308" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A308" s="125" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C308" s="60">
         <f>E302-MIN(G276:K276)</f>
@@ -13016,12 +13020,12 @@
     <row r="310" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="311" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A311" s="126" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A312" s="82" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B312" s="21">
         <f>N161+N158+N155+N152+N149+N146</f>
@@ -13030,7 +13034,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A313" s="82" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B313" s="21">
         <f>Q60</f>
@@ -13039,7 +13043,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A314" s="83" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B314" s="90">
         <f>B312+B313</f>
@@ -13049,12 +13053,12 @@
     <row r="315" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="316" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A316" s="126" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A317" s="82" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B317" s="21">
         <f>N161+N158+N155+N152</f>
@@ -13063,7 +13067,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A318" s="82" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B318" s="21">
         <f>(E45*N6)+(D48*N5)</f>
@@ -13072,7 +13076,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A319" s="83" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B319" s="90">
         <f>B317+B318</f>
@@ -13095,10 +13099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q97"/>
+  <dimension ref="A1:P97"/>
   <sheetViews>
     <sheetView zoomScale="46" zoomScaleNormal="46" workbookViewId="0">
-      <selection activeCell="N97" sqref="N97"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13108,7 +13112,7 @@
     <col min="10" max="15" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="71" t="s">
         <v>46</v>
       </c>
@@ -13126,10 +13130,10 @@
         <v>53</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K1" s="42" t="s">
         <v>62</v>
@@ -13147,7 +13151,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="44" t="s">
         <v>47</v>
       </c>
@@ -13186,17 +13190,17 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="72" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="73" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="70" t="s">
         <v>52</v>
       </c>
@@ -13232,15 +13236,15 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="32"/>
     </row>
-    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="73" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="70" t="s">
         <v>67</v>
       </c>
@@ -13248,7 +13252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>68</v>
       </c>
@@ -13256,7 +13260,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>69</v>
       </c>
@@ -13282,7 +13286,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>175</v>
       </c>
@@ -13290,7 +13294,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>176</v>
       </c>
@@ -13298,16 +13302,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="101" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>157</v>
       </c>
@@ -13340,9 +13344,6 @@
       </c>
       <c r="O16" s="2">
         <v>50</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -13801,20 +13802,20 @@
     <row r="38" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="39" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C39" s="127" t="s">
+        <v>216</v>
+      </c>
+      <c r="D39" s="129" t="s">
         <v>217</v>
-      </c>
-      <c r="D39" s="129" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="126" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="124" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F41" s="159">
         <f>Network!C302</f>
@@ -13859,7 +13860,7 @@
     </row>
     <row r="42" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="149" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F42" s="146">
         <v>8</v>
@@ -13894,7 +13895,7 @@
     </row>
     <row r="43" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="149" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C43" s="144">
         <v>0.3</v>
@@ -13945,7 +13946,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="155" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F44" s="166">
         <f t="shared" ref="F44:O44" si="1">F41+F43</f>
@@ -13990,7 +13991,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="149" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F45" s="156">
         <f>F19-F87</f>
@@ -14035,7 +14036,7 @@
     </row>
     <row r="46" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="125" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F46" s="163" t="str">
         <f t="shared" ref="F46:O46" si="3">IF(F44&lt;=(F19-F87),"OK","NO")</f>
@@ -14081,13 +14082,13 @@
     <row r="47" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="48" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="126" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" s="148" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F49" s="135">
         <f>18+'Mast + Tower'!B22</f>
@@ -14128,7 +14129,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" s="149" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F50" s="146">
         <f>F5*F49</f>
@@ -14169,7 +14170,7 @@
     </row>
     <row r="51" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="149" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F51" s="146">
         <v>8</v>
@@ -14201,7 +14202,7 @@
     </row>
     <row r="52" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="149" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C52" s="144">
         <v>0.3</v>
@@ -14248,7 +14249,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" s="149" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F53" s="146">
         <f t="shared" ref="F53:N53" si="5">F52+F50</f>
@@ -14289,7 +14290,7 @@
     </row>
     <row r="54" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="150" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F54" s="138">
         <f t="shared" ref="F54:N54" si="6">F32-F53</f>
@@ -14331,17 +14332,17 @@
     <row r="55" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="56" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="126" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" s="148" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F58" s="135">
         <f>F44-(F32-F53)</f>
@@ -14382,7 +14383,7 @@
     </row>
     <row r="59" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="150" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F59" s="163" t="str">
         <f>IF(AND(F16&gt;F58,(F16-F17)&lt;F58),"OK","NO")</f>
@@ -14424,12 +14425,12 @@
     <row r="60" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="61" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="126" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" s="148" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F62" s="135">
         <f>IF(F58-F24&gt;F16-F17,F58-F24,F16-F17)</f>
@@ -14470,7 +14471,7 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" s="149" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F63" s="146">
         <f>F58-F62</f>
@@ -14512,7 +14513,7 @@
     </row>
     <row r="64" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="150" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F64" s="163" t="str">
         <f>IF(AND(F16&gt;F62,(F16-F17)&lt;F62),"OK","NO")</f>
@@ -14554,12 +14555,12 @@
     <row r="65" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="66" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="170" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67" s="149" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F67" s="135">
         <v>0.15</v>
@@ -14591,7 +14592,7 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="149" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F68" s="146">
         <v>290</v>
@@ -14623,7 +14624,7 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="149" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F69" s="146">
         <v>-13</v>
@@ -14655,7 +14656,7 @@
     </row>
     <row r="70" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="150" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F70" s="138">
         <v>38</v>
@@ -14688,17 +14689,17 @@
     <row r="71" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" s="171" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="172" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="149" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B74" s="1"/>
       <c r="F74" s="135">
@@ -14740,7 +14741,7 @@
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="149" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F75" s="166">
         <f>F32-F69-10*LOG10(10^((F18+F53)/10)+10^((F53-F58)/10)*(10^((F43+Network!H277)/10)-1))</f>
@@ -14781,7 +14782,7 @@
     </row>
     <row r="76" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="150" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F76" s="163" t="str">
         <f>IF(F75&gt;=F70,"OK","NO")</f>
@@ -14823,12 +14824,12 @@
     <row r="77" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="78" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="170" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" s="149" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F79" s="135">
         <f>10*LOG10(10^(F26/10)+(10^(F53/10)-1)/10^(F63/10)+(10^(F18/10)-1)*10^(F53/10)/10^(F63/10)+10^((F53-F62-F63)/10)*(10^((F43+Network!H277)/10)-1))</f>
@@ -14870,7 +14871,7 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" s="149" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F80" s="166">
         <f>F32-F69-10*LOG10(10^(F26/10)+(10^(F53/10)-1)/10^(F63/10)+(10^(F18/10)-1)*10^(F53/10)/10^(F63/10)+10^((F53-F62-F63)/10)*(10^((F43+Network!H277)/10)-1))</f>
@@ -14911,7 +14912,7 @@
     </row>
     <row r="81" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="150" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F81" s="163" t="str">
         <f>IF(F80&gt;=F70,"OK","NO")</f>
@@ -14953,12 +14954,12 @@
     <row r="84" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="85" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="126" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" s="148" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F86" s="135">
         <v>30</v>
@@ -14993,7 +14994,7 @@
     </row>
     <row r="87" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="149" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F87" s="152">
         <f>7.5*LOG10((F86-1))</f>
@@ -15032,7 +15033,7 @@
     </row>
     <row r="88" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="150" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H88" s="138">
         <v>30</v>
@@ -15062,12 +15063,12 @@
     <row r="89" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="90" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="170" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" s="155" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H91" s="159">
         <f>H28+2*(H27-H87-H44)</f>
@@ -15104,7 +15105,7 @@
     </row>
     <row r="92" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="125" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H92" s="163" t="str">
         <f>IF(H91&gt;=H88,"OK","NO")</f>
@@ -15142,12 +15143,12 @@
     <row r="93" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="94" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="170" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" s="149" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H95" s="135">
         <f>H32+H63</f>
@@ -15180,7 +15181,7 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" s="155" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H96" s="174">
         <f>-20*LOG10(10^(-H91/20)+10^(-(H28+2*(H27-7.5*LOG10(SUM(H86:N86)-1)-H32-H63))/20))</f>
@@ -15214,7 +15215,7 @@
     </row>
     <row r="97" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="125" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H97" s="163" t="str">
         <f>IF(H96&gt;=H88,"OK","NO")</f>
@@ -15268,10 +15269,10 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="32"/>
-      <c r="B2" s="219" t="s">
+      <c r="B2" s="216" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="220"/>
+      <c r="C2" s="217"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="118"/>
@@ -15306,7 +15307,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="119" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B6" s="190">
         <f>30-0.36</f>
@@ -15321,7 +15322,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="119" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B7" s="191">
         <f>DEGREES(ACOS(COS(RADIANS(B6))*COS(RADIANS(B4))))</f>
@@ -15334,7 +15335,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="119" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B8" s="190">
         <v>6378.16</v>
@@ -15345,7 +15346,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="119" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B9" s="190">
         <v>35786.300000000003</v>
@@ -15358,7 +15359,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="119" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B10" s="192">
         <f>DEGREES(ATAN((COS(RADIANS(B7))-B8/(B9+B8))/SIN(RADIANS(B7))))</f>
@@ -15373,7 +15374,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="119" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B11" s="191">
         <f>180 + DEGREES(ATAN(TAN(RADIANS(B6))/SIN(RADIANS(B4))))</f>
@@ -15388,7 +15389,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="119" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B12" s="191">
         <f>B9*SQRT(1+((2*B8*(B8+B9))/POWER(B9,2)*(1-COS(RADIANS(B7)))))</f>
@@ -15406,7 +15407,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="119" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B15" s="120">
         <v>54</v>
@@ -15428,7 +15429,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="119" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B17" s="120">
         <v>50</v>
@@ -15439,7 +15440,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="119" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B18" s="120">
         <v>3</v>
@@ -15557,7 +15558,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="119" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B28" s="196">
         <f>B26-B15+B22+B23+B27</f>
@@ -15583,7 +15584,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="119" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B31" s="196">
         <f>B29*POWER(10,(B28/20))/(PI()*SQRT(B16))</f>
@@ -15609,7 +15610,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="119" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B33" s="196">
         <f>B15-B23-B22+B28</f>
@@ -15626,7 +15627,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="119" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B34" s="196">
         <f>(B15-B23-B22+B28)-B27</f>
@@ -15639,7 +15640,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="119" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B35" s="196">
         <f>B33+60-(29.6*0.2)</f>
@@ -15652,7 +15653,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="119" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B36" s="196">
         <f>SQRT(POWER(10,(B35/10))*75)*1000000</f>
@@ -15665,7 +15666,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="119" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B37" s="196">
         <f>20*LOG10(B36)</f>
@@ -15678,7 +15679,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="119" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B38" s="196">
         <f>123-B37</f>
@@ -15700,49 +15701,50 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.36328125" customWidth="1"/>
-    <col min="2" max="2" width="17.6328125" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" customWidth="1"/>
-    <col min="5" max="5" width="34.90625" customWidth="1"/>
-    <col min="6" max="6" width="21.6328125" customWidth="1"/>
-    <col min="7" max="7" width="17.6328125" customWidth="1"/>
-    <col min="8" max="8" width="18.6328125" customWidth="1"/>
-    <col min="9" max="9" width="5.6328125" customWidth="1"/>
+    <col min="1" max="1" width="32.54296875" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" customWidth="1"/>
+    <col min="3" max="3" width="37.08984375" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="45.1796875" customWidth="1"/>
+    <col min="6" max="6" width="30.26953125" customWidth="1"/>
+    <col min="7" max="7" width="7.81640625" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" customWidth="1"/>
     <col min="10" max="10" width="18.90625" customWidth="1"/>
     <col min="12" max="12" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="209"/>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="204"/>
       <c r="B1" s="119" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D1" s="119" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
       <c r="H1" s="32"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="119" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B2" s="120">
         <f>B3*B6</f>
         <v>523.20000000000005</v>
       </c>
       <c r="C2" s="119" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D2" s="120">
         <v>3</v>
@@ -15752,16 +15754,16 @@
       <c r="G2" s="32"/>
       <c r="H2" s="32"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="119" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B3" s="120">
         <f>((B4)^2/16)*B5</f>
         <v>799.52256944444457</v>
       </c>
       <c r="C3" s="119" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D3" s="120">
         <v>3</v>
@@ -15771,16 +15773,16 @@
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="119" t="s">
-        <v>265</v>
-      </c>
-      <c r="B4" s="223">
+        <v>264</v>
+      </c>
+      <c r="B4" s="210">
         <f>130*(1000/3600)</f>
         <v>36.111111111111114</v>
       </c>
       <c r="C4" s="119" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D4" s="120">
         <v>0.27200000000000002</v>
@@ -15790,9 +15792,9 @@
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="213" t="s">
-        <v>266</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="207" t="s">
+        <v>265</v>
       </c>
       <c r="B5" s="120">
         <v>9.81</v>
@@ -15804,9 +15806,9 @@
       <c r="G5" s="32"/>
       <c r="H5" s="32"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="213" t="s">
-        <v>267</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="207" t="s">
+        <v>266</v>
       </c>
       <c r="B6" s="120">
         <f>523.2/B3</f>
@@ -15819,7 +15821,7 @@
       <c r="G6" s="32"/>
       <c r="H6" s="32"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
@@ -15829,105 +15831,105 @@
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="221" t="s">
-        <v>273</v>
-      </c>
-      <c r="B8" s="222"/>
-      <c r="C8" s="221" t="s">
-        <v>301</v>
-      </c>
-      <c r="D8" s="222"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="218" t="s">
+        <v>272</v>
+      </c>
+      <c r="B8" s="219"/>
+      <c r="C8" s="218" t="s">
+        <v>298</v>
+      </c>
+      <c r="D8" s="219"/>
       <c r="E8" s="32"/>
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
       <c r="H8" s="32"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="119" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B9" s="120">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="C9" s="224">
+      <c r="C9" s="220">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D9" s="225"/>
+      <c r="D9" s="221"/>
       <c r="E9" s="32"/>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="32"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="119" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B10" s="120">
         <v>6</v>
       </c>
-      <c r="C10" s="224">
+      <c r="C10" s="220">
         <v>3</v>
       </c>
-      <c r="D10" s="225"/>
+      <c r="D10" s="221"/>
       <c r="E10" s="32"/>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="119" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B11" s="120">
         <v>0.7</v>
       </c>
-      <c r="C11" s="224">
+      <c r="C11" s="220">
         <v>0.7</v>
       </c>
-      <c r="D11" s="225"/>
+      <c r="D11" s="221"/>
       <c r="E11" s="32"/>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
       <c r="H11" s="32"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="119" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B12" s="120">
         <f>B9*B10*B11</f>
         <v>0.189</v>
       </c>
-      <c r="C12" s="224">
+      <c r="C12" s="220">
         <f>C9*C10*C11</f>
         <v>9.4500000000000001E-2</v>
       </c>
-      <c r="D12" s="225"/>
+      <c r="D12" s="221"/>
       <c r="E12" s="32"/>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
       <c r="H12" s="32"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="119" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B13" s="120">
         <f>800*B12</f>
         <v>151.19999999999999</v>
       </c>
-      <c r="C13" s="224">
+      <c r="C13" s="220">
         <f>800*C12</f>
         <v>75.599999999999994</v>
       </c>
-      <c r="D13" s="225"/>
+      <c r="D13" s="221"/>
       <c r="E13" s="32"/>
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
       <c r="H13" s="32"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -15937,43 +15939,40 @@
       <c r="G14" s="32"/>
       <c r="H14" s="32"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="32"/>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="221" t="s">
-        <v>300</v>
-      </c>
-      <c r="B16" s="222"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="B16" s="219"/>
       <c r="C16" s="119" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D16" s="32"/>
       <c r="E16" s="119" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="F16" s="119" t="s">
-        <v>288</v>
-      </c>
-      <c r="G16" s="32"/>
+        <v>311</v>
+      </c>
       <c r="H16" s="119" t="s">
-        <v>314</v>
-      </c>
-      <c r="I16" s="212"/>
-      <c r="J16" s="119" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+        <v>303</v>
+      </c>
+      <c r="I16" s="120">
+        <f>-SUM(E17,E19,E21,E23,E24)</f>
+        <v>-755.30000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="119" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B17" s="120">
         <v>93</v>
@@ -15987,52 +15986,32 @@
         <v>93</v>
       </c>
       <c r="F17" s="120">
-        <f>E17*E18</f>
-        <v>558</v>
-      </c>
-      <c r="G17" s="32"/>
-      <c r="H17" s="120">
-        <v>93</v>
-      </c>
-      <c r="J17" s="120">
         <f>2*B5</f>
         <v>19.62</v>
       </c>
-      <c r="L17" s="119" t="s">
-        <v>307</v>
-      </c>
-      <c r="M17" s="120">
-        <f>-SUM(H17,H19,H21,H23,H24)</f>
-        <v>-755.30000000000007</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="H17" s="119" t="s">
+        <v>304</v>
+      </c>
+      <c r="I17" s="120">
+        <f>-SUM(F24,F25,F23,F21,F19,F17)</f>
+        <v>-139.30200000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="119" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B18" s="120">
         <v>6</v>
       </c>
       <c r="C18" s="198"/>
       <c r="D18" s="32"/>
-      <c r="E18" s="120">
-        <v>6</v>
-      </c>
+      <c r="E18" s="198"/>
       <c r="F18" s="198"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="198"/>
-      <c r="J18" s="198"/>
-      <c r="L18" s="119" t="s">
-        <v>308</v>
-      </c>
-      <c r="M18" s="120">
-        <f>-SUM(J24,J25,J23,J21,J19,J17)</f>
-        <v>-139.30200000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="119" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B19" s="120">
         <v>36.5</v>
@@ -16046,38 +16025,25 @@
         <v>36.5</v>
       </c>
       <c r="F19" s="120">
-        <f>E19*E20</f>
-        <v>164.25</v>
-      </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="120">
-        <v>36.5</v>
-      </c>
-      <c r="J19" s="120">
         <f>1.5*B5</f>
         <v>14.715</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="119" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B20" s="120">
         <v>4.5</v>
       </c>
       <c r="C20" s="198"/>
       <c r="D20" s="32"/>
-      <c r="E20" s="120">
-        <v>4.5</v>
-      </c>
+      <c r="E20" s="198"/>
       <c r="F20" s="198"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="198"/>
-      <c r="J20" s="198"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="119" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B21" s="120">
         <v>27</v>
@@ -16091,38 +16057,25 @@
         <v>27</v>
       </c>
       <c r="F21" s="120">
-        <f>E21*E22</f>
-        <v>81</v>
-      </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="120">
-        <v>27</v>
-      </c>
-      <c r="J21" s="120">
         <f>1.2*B5</f>
         <v>11.772</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="119" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B22" s="120">
         <v>3</v>
       </c>
       <c r="C22" s="198"/>
       <c r="D22" s="32"/>
-      <c r="E22" s="120">
-        <v>3</v>
-      </c>
+      <c r="E22" s="198"/>
       <c r="F22" s="198"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="198"/>
-      <c r="J22" s="198"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="119" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B23" s="120">
         <v>523.20000000000005</v>
@@ -16136,147 +16089,323 @@
         <v>523.20000000000005</v>
       </c>
       <c r="F23" s="120">
-        <f>E23*E24</f>
-        <v>261.60000000000002</v>
-      </c>
-      <c r="G23" s="32"/>
-      <c r="H23" s="120">
-        <v>523.20000000000005</v>
-      </c>
-      <c r="J23" s="120">
         <f>5*9.81</f>
         <v>49.050000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="210" t="s">
-        <v>280</v>
-      </c>
-      <c r="B24" s="223">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="205" t="s">
+        <v>279</v>
+      </c>
+      <c r="B24" s="210">
         <v>0.5</v>
       </c>
       <c r="C24" s="199"/>
       <c r="D24" s="32"/>
-      <c r="E24" s="223">
-        <v>0.5</v>
-      </c>
-      <c r="F24" s="199"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="223">
+      <c r="E24" s="210">
         <f>C13</f>
         <v>75.599999999999994</v>
       </c>
-      <c r="J24" s="120">
+      <c r="F24" s="120">
         <f>2*B5</f>
         <v>19.62</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="200"/>
       <c r="B25" s="200"/>
       <c r="C25" s="200"/>
       <c r="D25" s="32"/>
       <c r="E25" s="200"/>
-      <c r="F25" s="200"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="200"/>
-      <c r="J25" s="120">
+      <c r="F25" s="120">
         <f>2.5*B5</f>
         <v>24.525000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="214" t="s">
-        <v>309</v>
-      </c>
-      <c r="E26" s="120">
-        <v>2.9</v>
-      </c>
-      <c r="G26" s="32"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="211" t="s">
-        <v>310</v>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="208" t="s">
+        <v>305</v>
+      </c>
+      <c r="E26" s="222"/>
+      <c r="F26" s="222"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="206" t="s">
+        <v>306</v>
       </c>
       <c r="B27" s="120">
         <f>SUM(C17,C19,C21,C23)</f>
         <v>1064.8499999999999</v>
       </c>
       <c r="C27" s="202"/>
-      <c r="D27" s="206"/>
-      <c r="E27" s="226">
-        <f>SUM(F17*(E26-E24),F19*(E26-E22),F21*(E20-E26),F23*(E18-E26))</f>
-        <v>2263.335</v>
-      </c>
-      <c r="F27" s="202"/>
-      <c r="G27" s="32"/>
+      <c r="D27" s="223"/>
+      <c r="E27" s="222"/>
+      <c r="F27" s="222"/>
       <c r="H27" s="32"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="119" t="s">
-        <v>311</v>
-      </c>
-      <c r="B28" s="227">
+        <v>307</v>
+      </c>
+      <c r="B28" s="212">
         <f>0.045*280*((B10)^2-(3)^2)</f>
         <v>340.2</v>
       </c>
       <c r="C28" s="202"/>
       <c r="D28" s="32"/>
-      <c r="E28" s="227">
-        <f>(0.045*280*((C10)^2))*6</f>
-        <v>680.4</v>
-      </c>
-      <c r="F28" s="202"/>
-      <c r="G28" s="32"/>
+      <c r="E28" s="222"/>
+      <c r="F28" s="222"/>
       <c r="H28" s="32"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="119" t="s">
-        <v>312</v>
-      </c>
-      <c r="B29" s="227">
+        <v>308</v>
+      </c>
+      <c r="B29" s="212">
         <f>B27+B28</f>
         <v>1405.05</v>
       </c>
       <c r="C29" s="201"/>
       <c r="D29" s="32"/>
-      <c r="E29" s="227">
-        <f>E27+E28</f>
-        <v>2943.7350000000001</v>
-      </c>
-      <c r="F29" s="201"/>
-      <c r="G29" s="32"/>
+      <c r="E29" s="222"/>
+      <c r="F29" s="222"/>
       <c r="H29" s="32"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="210" t="s">
-        <v>313</v>
-      </c>
-      <c r="B30" s="203">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="205" t="s">
+        <v>309</v>
+      </c>
+      <c r="B30" s="233">
         <f>B29-355</f>
         <v>1050.05</v>
       </c>
-      <c r="C30" s="208" t="s">
-        <v>298</v>
-      </c>
-      <c r="D30" s="204"/>
-      <c r="E30" s="205">
-        <f>E29-355</f>
-        <v>2588.7350000000001</v>
-      </c>
-      <c r="F30" s="207" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C30" s="203" t="s">
+        <v>296</v>
+      </c>
+      <c r="D30" s="202"/>
+      <c r="E30" s="222"/>
+      <c r="F30" s="222"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="197"/>
       <c r="B31" s="197"/>
       <c r="C31" s="197"/>
-      <c r="E31" s="197"/>
-      <c r="F31" s="197"/>
+      <c r="E31" s="222"/>
+      <c r="F31" s="222"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="B33" s="219"/>
+      <c r="C33" s="119" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="119" t="s">
+        <v>273</v>
+      </c>
+      <c r="B34" s="120">
+        <v>93</v>
+      </c>
+      <c r="C34" s="120">
+        <f>B34*B35</f>
+        <v>558</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="119" t="s">
+        <v>274</v>
+      </c>
+      <c r="B35" s="120">
+        <v>6</v>
+      </c>
+      <c r="C35" s="198"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="119" t="s">
+        <v>275</v>
+      </c>
+      <c r="B36" s="120">
+        <v>36.5</v>
+      </c>
+      <c r="C36" s="120">
+        <f t="shared" ref="C36" si="1">B36*B37</f>
+        <v>164.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="119" t="s">
+        <v>276</v>
+      </c>
+      <c r="B37" s="120">
+        <v>4.5</v>
+      </c>
+      <c r="C37" s="198"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="119" t="s">
+        <v>280</v>
+      </c>
+      <c r="B38" s="120">
+        <v>27</v>
+      </c>
+      <c r="C38" s="120">
+        <f>B38*B39</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="119" t="s">
+        <v>277</v>
+      </c>
+      <c r="B39" s="120">
+        <v>3</v>
+      </c>
+      <c r="C39" s="198"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="119" t="s">
+        <v>278</v>
+      </c>
+      <c r="B40" s="120">
+        <v>523.20000000000005</v>
+      </c>
+      <c r="C40" s="120">
+        <f>B40*B41</f>
+        <v>261.60000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="205" t="s">
+        <v>279</v>
+      </c>
+      <c r="B41" s="210">
+        <v>0.5</v>
+      </c>
+      <c r="C41" s="232"/>
+      <c r="D41" s="222"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="200"/>
+      <c r="B42" s="200"/>
+      <c r="C42" s="32"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="224" t="s">
+        <v>338</v>
+      </c>
+      <c r="B43" s="219"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="206" t="s">
+        <v>306</v>
+      </c>
+      <c r="B44" s="211">
+        <f>SUM(C34,C36,C38)</f>
+        <v>803.25</v>
+      </c>
+      <c r="C44" s="202"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="B45" s="212">
+        <f>(0.045*280*((C10)^2))</f>
+        <v>113.39999999999999</v>
+      </c>
+      <c r="C45" s="202"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="119" t="s">
+        <v>308</v>
+      </c>
+      <c r="B46" s="212">
+        <f>B44+B45</f>
+        <v>916.65</v>
+      </c>
+      <c r="C46" s="202"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="205" t="s">
+        <v>309</v>
+      </c>
+      <c r="B47" s="107">
+        <f>B46-355</f>
+        <v>561.65</v>
+      </c>
+      <c r="C47" s="229" t="s">
+        <v>342</v>
+      </c>
+      <c r="D47" s="229"/>
+      <c r="E47" s="229"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C48" s="231" t="s">
+        <v>341</v>
+      </c>
+      <c r="D48" s="230"/>
+      <c r="E48" s="230"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C49" s="230"/>
+      <c r="D49" s="230"/>
+      <c r="E49" s="230"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="224" t="s">
+        <v>339</v>
+      </c>
+      <c r="B51" s="219"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="206" t="s">
+        <v>306</v>
+      </c>
+      <c r="B52" s="211">
+        <f>SUM(C38,C40,C36,C34)</f>
+        <v>1064.8499999999999</v>
+      </c>
+      <c r="C52" s="185"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="119" t="s">
+        <v>307</v>
+      </c>
+      <c r="B53" s="212">
+        <f>C13*B35</f>
+        <v>453.59999999999997</v>
+      </c>
+      <c r="C53" s="185"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="205" t="s">
+        <v>308</v>
+      </c>
+      <c r="B54" s="225">
+        <f>B44+B45</f>
+        <v>916.65</v>
+      </c>
+      <c r="C54" s="203" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="227"/>
+      <c r="B55" s="228"/>
+      <c r="C55" s="226"/>
+      <c r="D55" s="222"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="14">
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:D8"/>

</xml_diff>

<commit_message>
Cambios sistema de captura
</commit_message>
<xml_diff>
--- a/3C/ITSIT/CTI3.xlsx
+++ b/3C/ITSIT/CTI3.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="344">
   <si>
     <t>TECHNICAL CHARACTERISTICS OF ELEMENTS FROM CATALOGUE</t>
   </si>
@@ -931,9 +931,6 @@
     <t>Ma&gt;Mtotal-Mmastil</t>
   </si>
   <si>
-    <t>MOMENTO FLECTOR  MASTIL</t>
-  </si>
-  <si>
     <t>AREA EFECTIVA EN TORRE-MASTIL</t>
   </si>
   <si>
@@ -1054,19 +1051,25 @@
     <t>ATTENUATION OF DISPERSION+INTERIOR. BEST AND WORST OUTLET ON EACH FLOOR (dB)</t>
   </si>
   <si>
-    <t>MOMENTO FLECTOR BASE MASTIL</t>
-  </si>
-  <si>
     <t>MOMENTO FLECTOR BASE TORRE</t>
   </si>
   <si>
     <t>Es menor que 5108 Nm, cumple</t>
   </si>
   <si>
-    <t>SE PODRIA COGER UN MASTIL DE 1,5M DE LONGITUD Y CUMPLIRIA</t>
-  </si>
-  <si>
-    <t>NO CUMPLE HABRIA QUE REDUCIR DISTANCIA ENTRE ANTENAS (4,5 3 y 1,5)</t>
+    <t>MOMENTO FLECTOR BASE MASTIL (con cables)</t>
+  </si>
+  <si>
+    <t>CARGAS Y DISTANCIAS ANTENAS</t>
+  </si>
+  <si>
+    <t>Cables a 25, 30 y 35 grados. Sujetos al mastil a una altura total de 4,5m. Situados a 1,9, 2,25 y 2,6 metros de la base de torreta</t>
+  </si>
+  <si>
+    <t>Momento_torreta (Nm)</t>
+  </si>
+  <si>
+    <t>Puede soportar hasta 130km/h</t>
   </si>
 </sst>
 </file>
@@ -2035,7 +2038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="234">
+  <cellXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2513,6 +2516,40 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2540,38 +2577,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3250,7 +3262,7 @@
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="28" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="30"/>
@@ -3335,7 +3347,7 @@
         <v>5.335</v>
       </c>
       <c r="P19" s="209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3472,7 +3484,7 @@
         <v>3.0350000000000001</v>
       </c>
       <c r="P22" s="209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3573,7 +3585,7 @@
         <v>5.335</v>
       </c>
       <c r="P25" s="209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3668,7 +3680,7 @@
     </row>
     <row r="28" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="55" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D28" s="59">
         <v>2</v>
@@ -3710,7 +3722,7 @@
         <v>3.0350000000000001</v>
       </c>
       <c r="P28" s="209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3947,12 +3959,12 @@
         <v>6.6000000000000005</v>
       </c>
       <c r="P34" s="209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="55" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D35" s="61">
         <v>13</v>
@@ -4039,7 +4051,7 @@
         <v>3.15</v>
       </c>
       <c r="P36" s="209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4230,12 +4242,12 @@
         <v>6.6000000000000005</v>
       </c>
       <c r="P41" s="209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="55" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D42" s="61">
         <v>13</v>
@@ -4322,7 +4334,7 @@
         <v>3.15</v>
       </c>
       <c r="P43" s="209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4378,7 +4390,7 @@
         <v>5.335</v>
       </c>
       <c r="P45" s="209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4515,7 +4527,7 @@
         <v>3.0350000000000001</v>
       </c>
       <c r="P48" s="209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4616,7 +4628,7 @@
         <v>5.335</v>
       </c>
       <c r="P51" s="209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4709,7 +4721,7 @@
       </c>
       <c r="P53" s="209"/>
       <c r="Q53" s="209" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4756,7 +4768,7 @@
         <v>3.0350000000000001</v>
       </c>
       <c r="P54" s="209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q54">
         <f>(D54*N6)+(E51*N5)</f>
@@ -4952,7 +4964,7 @@
       </c>
       <c r="P59" s="209"/>
       <c r="Q59" s="209" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4999,7 +5011,7 @@
         <v>6.6000000000000005</v>
       </c>
       <c r="P60" s="209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q60">
         <f>(D60*N5)+(E57*N6)</f>
@@ -5095,7 +5107,7 @@
         <v>3.15</v>
       </c>
       <c r="P62" s="209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="63" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5286,12 +5298,12 @@
         <v>6.37</v>
       </c>
       <c r="P67" s="209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="55" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D68" s="61">
         <v>13</v>
@@ -5378,7 +5390,7 @@
         <v>3.15</v>
       </c>
       <c r="P69" s="209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5434,7 +5446,7 @@
         <v>5.335</v>
       </c>
       <c r="P71" s="209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5484,7 +5496,7 @@
     </row>
     <row r="73" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="55" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D73" s="59">
         <v>15</v>
@@ -5529,7 +5541,7 @@
     </row>
     <row r="74" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="55" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D74" s="59">
         <v>2</v>
@@ -5571,7 +5583,7 @@
         <v>3.0350000000000001</v>
       </c>
       <c r="P74" s="209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="75" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5672,7 +5684,7 @@
         <v>5.335</v>
       </c>
       <c r="P77" s="209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="78" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5722,7 +5734,7 @@
     </row>
     <row r="79" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="55" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D79" s="59">
         <v>15</v>
@@ -5809,7 +5821,7 @@
         <v>3.0350000000000001</v>
       </c>
       <c r="P80" s="209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="81" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5958,7 +5970,7 @@
     </row>
     <row r="85" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B85" s="52"/>
       <c r="C85" s="52"/>
@@ -6007,7 +6019,7 @@
     </row>
     <row r="86" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="55" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B86" s="52"/>
       <c r="C86" s="52"/>
@@ -6053,7 +6065,7 @@
         <v>6.6000000000000005</v>
       </c>
       <c r="P86" s="209" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="87" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6153,7 +6165,7 @@
         <v>3.15</v>
       </c>
       <c r="P88" s="209" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6272,7 +6284,7 @@
     </row>
     <row r="92" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="55" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D92" s="59">
         <v>13</v>
@@ -6316,7 +6328,7 @@
     </row>
     <row r="93" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D93" s="59">
         <v>32</v>
@@ -6358,7 +6370,7 @@
         <v>6.37</v>
       </c>
       <c r="P93" s="52" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="94" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6449,7 +6461,7 @@
         <v>3.15</v>
       </c>
       <c r="P95" s="52" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="96" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6503,7 +6515,7 @@
         <v>5.335</v>
       </c>
       <c r="P97" s="52" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="98" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6552,7 +6564,7 @@
     </row>
     <row r="99" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="55" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D99" s="59">
         <v>15</v>
@@ -6638,7 +6650,7 @@
         <v>3.0350000000000001</v>
       </c>
       <c r="P100" s="52" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="101" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6736,7 +6748,7 @@
         <v>5.335</v>
       </c>
       <c r="P103" s="52" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="104" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6785,7 +6797,7 @@
     </row>
     <row r="105" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="55" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D105" s="59">
         <v>15</v>
@@ -6871,7 +6883,7 @@
         <v>3.0350000000000001</v>
       </c>
       <c r="P106" s="52" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="107" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7015,7 +7027,7 @@
     </row>
     <row r="111" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="55" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D111" s="59">
         <v>13</v>
@@ -7059,7 +7071,7 @@
     </row>
     <row r="112" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="55" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D112" s="59">
         <v>34</v>
@@ -7101,7 +7113,7 @@
         <v>6.6000000000000005</v>
       </c>
       <c r="P112" s="52" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="113" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7192,7 +7204,7 @@
         <v>3.15</v>
       </c>
       <c r="P114" s="52" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="115" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7292,7 +7304,7 @@
     </row>
     <row r="118" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A118" s="55" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D118" s="59">
         <v>13</v>
@@ -7336,7 +7348,7 @@
     </row>
     <row r="119" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A119" s="55" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D119" s="59">
         <v>34</v>
@@ -7378,12 +7390,12 @@
         <v>6.6000000000000005</v>
       </c>
       <c r="P119" s="52" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="120" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="55" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D120" s="61">
         <v>13</v>
@@ -7469,7 +7481,7 @@
         <v>3.15</v>
       </c>
       <c r="P121" s="52" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="122" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7523,7 +7535,7 @@
         <v>3.7250000000000001</v>
       </c>
       <c r="P123" s="52" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="124" spans="1:16" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7618,7 +7630,7 @@
         <v>4.53</v>
       </c>
       <c r="P125" s="52" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="126" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.35">
@@ -10833,7 +10845,7 @@
     </row>
     <row r="225" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A225" s="55" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G225" s="58">
         <f t="shared" si="190"/>
@@ -10874,7 +10886,7 @@
     </row>
     <row r="226" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A226" s="55" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G226" s="58">
         <f t="shared" si="190"/>
@@ -11041,7 +11053,7 @@
     </row>
     <row r="231" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A231" s="55" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G231" s="58">
         <f t="shared" si="196"/>
@@ -11249,7 +11261,7 @@
     </row>
     <row r="237" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A237" s="55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G237" s="58">
         <f t="shared" si="202"/>
@@ -11290,7 +11302,7 @@
     </row>
     <row r="238" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A238" s="55" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G238" s="58">
         <f t="shared" si="202"/>
@@ -11498,7 +11510,7 @@
     </row>
     <row r="244" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A244" s="55" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G244" s="58">
         <f t="shared" si="210"/>
@@ -11539,7 +11551,7 @@
     </row>
     <row r="245" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A245" s="55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G245" s="58">
         <f t="shared" si="210"/>
@@ -11747,7 +11759,7 @@
     </row>
     <row r="251" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A251" s="55" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G251" s="58">
         <f t="shared" si="216"/>
@@ -11955,7 +11967,7 @@
     </row>
     <row r="257" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A257" s="55" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G257" s="58">
         <f t="shared" si="222"/>
@@ -12163,7 +12175,7 @@
     </row>
     <row r="263" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A263" s="55" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G263" s="58">
         <f t="shared" si="232"/>
@@ -12204,7 +12216,7 @@
     </row>
     <row r="264" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A264" s="55" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G264" s="58">
         <f t="shared" si="232"/>
@@ -12412,7 +12424,7 @@
     </row>
     <row r="270" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A270" s="55" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G270" s="58">
         <f t="shared" si="241"/>
@@ -12453,7 +12465,7 @@
     </row>
     <row r="271" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A271" s="55" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G271" s="58">
         <f t="shared" si="241"/>
@@ -12494,7 +12506,7 @@
     </row>
     <row r="272" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A272" s="55" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G272" s="58">
         <f t="shared" si="241"/>
@@ -12665,16 +12677,16 @@
       <c r="A280" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="C280" s="213" t="s">
+      <c r="C280" s="227" t="s">
         <v>170</v>
       </c>
-      <c r="D280" s="214"/>
-      <c r="E280" s="215"/>
-      <c r="G280" s="213" t="s">
+      <c r="D280" s="228"/>
+      <c r="E280" s="229"/>
+      <c r="G280" s="227" t="s">
         <v>171</v>
       </c>
-      <c r="H280" s="214"/>
-      <c r="I280" s="215"/>
+      <c r="H280" s="228"/>
+      <c r="I280" s="229"/>
     </row>
     <row r="281" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A281" s="81" t="s">
@@ -13020,12 +13032,12 @@
     <row r="310" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="311" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A311" s="126" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A312" s="82" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B312" s="21">
         <f>N161+N158+N155+N152+N149+N146</f>
@@ -13034,7 +13046,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A313" s="82" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B313" s="21">
         <f>Q60</f>
@@ -13043,7 +13055,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A314" s="83" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B314" s="90">
         <f>B312+B313</f>
@@ -13053,12 +13065,12 @@
     <row r="315" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="316" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A316" s="126" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A317" s="82" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B317" s="21">
         <f>N161+N158+N155+N152</f>
@@ -13067,7 +13079,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A318" s="82" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B318" s="21">
         <f>(E45*N6)+(D48*N5)</f>
@@ -13076,7 +13088,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A319" s="83" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B319" s="90">
         <f>B317+B318</f>
@@ -15269,10 +15281,10 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="32"/>
-      <c r="B2" s="216" t="s">
+      <c r="B2" s="230" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="217"/>
+      <c r="C2" s="231"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="118"/>
@@ -15407,7 +15419,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="119" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B15" s="120">
         <v>54</v>
@@ -15429,7 +15441,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="119" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B17" s="120">
         <v>50</v>
@@ -15440,7 +15452,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="119" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B18" s="120">
         <v>3</v>
@@ -15558,7 +15570,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="119" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B28" s="196">
         <f>B26-B15+B22+B23+B27</f>
@@ -15703,8 +15715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15832,14 +15844,14 @@
       <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="218" t="s">
+      <c r="A8" s="232" t="s">
         <v>272</v>
       </c>
-      <c r="B8" s="219"/>
-      <c r="C8" s="218" t="s">
-        <v>298</v>
-      </c>
-      <c r="D8" s="219"/>
+      <c r="B8" s="233"/>
+      <c r="C8" s="232" t="s">
+        <v>297</v>
+      </c>
+      <c r="D8" s="233"/>
       <c r="E8" s="32"/>
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
@@ -15852,10 +15864,10 @@
       <c r="B9" s="120">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="C9" s="220">
+      <c r="C9" s="234">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D9" s="221"/>
+      <c r="D9" s="235"/>
       <c r="E9" s="32"/>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
@@ -15868,10 +15880,10 @@
       <c r="B10" s="120">
         <v>6</v>
       </c>
-      <c r="C10" s="220">
+      <c r="C10" s="234">
         <v>3</v>
       </c>
-      <c r="D10" s="221"/>
+      <c r="D10" s="235"/>
       <c r="E10" s="32"/>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -15884,10 +15896,10 @@
       <c r="B11" s="120">
         <v>0.7</v>
       </c>
-      <c r="C11" s="220">
+      <c r="C11" s="234">
         <v>0.7</v>
       </c>
-      <c r="D11" s="221"/>
+      <c r="D11" s="235"/>
       <c r="E11" s="32"/>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
@@ -15901,11 +15913,11 @@
         <f>B9*B10*B11</f>
         <v>0.189</v>
       </c>
-      <c r="C12" s="220">
+      <c r="C12" s="234">
         <f>C9*C10*C11</f>
         <v>9.4500000000000001E-2</v>
       </c>
-      <c r="D12" s="221"/>
+      <c r="D12" s="235"/>
       <c r="E12" s="32"/>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
@@ -15919,11 +15931,11 @@
         <f>800*B12</f>
         <v>151.19999999999999</v>
       </c>
-      <c r="C13" s="220">
+      <c r="C13" s="234">
         <f>800*C12</f>
         <v>75.599999999999994</v>
       </c>
-      <c r="D13" s="221"/>
+      <c r="D13" s="235"/>
       <c r="E13" s="32"/>
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
@@ -15948,22 +15960,22 @@
       <c r="F15" s="32"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="218" t="s">
-        <v>297</v>
-      </c>
-      <c r="B16" s="219"/>
+      <c r="A16" s="232" t="s">
+        <v>340</v>
+      </c>
+      <c r="B16" s="233"/>
       <c r="C16" s="119" t="s">
         <v>295</v>
       </c>
       <c r="D16" s="32"/>
       <c r="E16" s="119" t="s">
+        <v>309</v>
+      </c>
+      <c r="F16" s="119" t="s">
         <v>310</v>
       </c>
-      <c r="F16" s="119" t="s">
-        <v>311</v>
-      </c>
       <c r="H16" s="119" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I16" s="120">
         <f>-SUM(E17,E19,E21,E23,E24)</f>
@@ -15990,7 +16002,7 @@
         <v>19.62</v>
       </c>
       <c r="H17" s="119" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I17" s="120">
         <f>-SUM(F24,F25,F23,F21,F19,F17)</f>
@@ -16124,28 +16136,28 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="208" t="s">
-        <v>305</v>
-      </c>
-      <c r="E26" s="222"/>
-      <c r="F26" s="222"/>
+        <v>304</v>
+      </c>
+      <c r="E26" s="214"/>
+      <c r="F26" s="214"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="206" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B27" s="120">
         <f>SUM(C17,C19,C21,C23)</f>
         <v>1064.8499999999999</v>
       </c>
       <c r="C27" s="202"/>
-      <c r="D27" s="223"/>
-      <c r="E27" s="222"/>
-      <c r="F27" s="222"/>
+      <c r="D27" s="215"/>
+      <c r="E27" s="214"/>
+      <c r="F27" s="214"/>
       <c r="H27" s="32"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B28" s="212">
         <f>0.045*280*((B10)^2-(3)^2)</f>
@@ -16153,13 +16165,13 @@
       </c>
       <c r="C28" s="202"/>
       <c r="D28" s="32"/>
-      <c r="E28" s="222"/>
-      <c r="F28" s="222"/>
+      <c r="E28" s="214"/>
+      <c r="F28" s="214"/>
       <c r="H28" s="32"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="119" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B29" s="212">
         <f>B27+B28</f>
@@ -16167,15 +16179,15 @@
       </c>
       <c r="C29" s="201"/>
       <c r="D29" s="32"/>
-      <c r="E29" s="222"/>
-      <c r="F29" s="222"/>
+      <c r="E29" s="214"/>
+      <c r="F29" s="214"/>
       <c r="H29" s="32"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="205" t="s">
-        <v>309</v>
-      </c>
-      <c r="B30" s="233">
+        <v>308</v>
+      </c>
+      <c r="B30" s="221">
         <f>B29-355</f>
         <v>1050.05</v>
       </c>
@@ -16183,26 +16195,26 @@
         <v>296</v>
       </c>
       <c r="D30" s="202"/>
-      <c r="E30" s="222"/>
-      <c r="F30" s="222"/>
+      <c r="E30" s="214"/>
+      <c r="F30" s="214"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="197"/>
       <c r="B31" s="197"/>
       <c r="C31" s="197"/>
-      <c r="E31" s="222"/>
-      <c r="F31" s="222"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="218" t="s">
-        <v>297</v>
-      </c>
-      <c r="B33" s="219"/>
+      <c r="E31" s="214"/>
+      <c r="F31" s="214"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="232" t="s">
+        <v>340</v>
+      </c>
+      <c r="B33" s="233"/>
       <c r="C33" s="119" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="119" t="s">
         <v>273</v>
       </c>
@@ -16214,7 +16226,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="119" t="s">
         <v>274</v>
       </c>
@@ -16223,7 +16235,7 @@
       </c>
       <c r="C35" s="198"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="119" t="s">
         <v>275</v>
       </c>
@@ -16235,7 +16247,7 @@
         <v>164.25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="119" t="s">
         <v>276</v>
       </c>
@@ -16244,7 +16256,7 @@
       </c>
       <c r="C37" s="198"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="119" t="s">
         <v>280</v>
       </c>
@@ -16256,7 +16268,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="119" t="s">
         <v>277</v>
       </c>
@@ -16265,7 +16277,7 @@
       </c>
       <c r="C39" s="198"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="119" t="s">
         <v>278</v>
       </c>
@@ -16277,92 +16289,94 @@
         <v>261.60000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="205" t="s">
         <v>279</v>
       </c>
       <c r="B41" s="210">
         <v>0.5</v>
       </c>
-      <c r="C41" s="232"/>
-      <c r="D41" s="222"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C41" s="220"/>
+      <c r="D41" s="214"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="200"/>
       <c r="B42" s="200"/>
       <c r="C42" s="32"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="224" t="s">
-        <v>338</v>
-      </c>
-      <c r="B43" s="219"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="236" t="s">
+        <v>339</v>
+      </c>
+      <c r="B43" s="233"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="206" t="s">
+        <v>305</v>
+      </c>
+      <c r="B44" s="226">
+        <f>SUM(B34*1.9,B36*2.25,B38*2.26)</f>
+        <v>319.84499999999997</v>
+      </c>
+      <c r="C44" s="237" t="s">
+        <v>341</v>
+      </c>
+      <c r="D44" s="238"/>
+      <c r="E44" s="238"/>
+      <c r="F44" s="238"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="119" t="s">
         <v>306</v>
       </c>
-      <c r="B44" s="211">
-        <f>SUM(C34,C36,C38)</f>
-        <v>803.25</v>
-      </c>
-      <c r="C44" s="202"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="119" t="s">
+      <c r="B45" s="213">
+        <v>113.4</v>
+      </c>
+      <c r="C45" s="185"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="119" t="s">
         <v>307</v>
-      </c>
-      <c r="B45" s="212">
-        <f>(0.045*280*((C10)^2))</f>
-        <v>113.39999999999999</v>
-      </c>
-      <c r="C45" s="202"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="119" t="s">
-        <v>308</v>
       </c>
       <c r="B46" s="212">
         <f>B44+B45</f>
-        <v>916.65</v>
+        <v>433.245</v>
       </c>
       <c r="C46" s="202"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="205" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B47" s="107">
         <f>B46-355</f>
-        <v>561.65</v>
-      </c>
-      <c r="C47" s="229" t="s">
-        <v>342</v>
-      </c>
-      <c r="D47" s="229"/>
-      <c r="E47" s="229"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C48" s="231" t="s">
-        <v>341</v>
-      </c>
-      <c r="D48" s="230"/>
-      <c r="E48" s="230"/>
+        <v>78.245000000000005</v>
+      </c>
+      <c r="C47" s="222" t="s">
+        <v>343</v>
+      </c>
+      <c r="D47" s="222"/>
+      <c r="E47" s="222"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C48" s="223"/>
+      <c r="D48" s="224"/>
+      <c r="E48" s="224"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C49" s="230"/>
-      <c r="D49" s="230"/>
-      <c r="E49" s="230"/>
+      <c r="C49" s="224"/>
+      <c r="D49" s="224"/>
+      <c r="E49" s="224"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="224" t="s">
-        <v>339</v>
-      </c>
-      <c r="B51" s="219"/>
+      <c r="A51" s="236" t="s">
+        <v>337</v>
+      </c>
+      <c r="B51" s="233"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="206" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B52" s="211">
         <f>SUM(C38,C40,C36,C34)</f>
@@ -16371,41 +16385,33 @@
       <c r="C52" s="185"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="119" t="s">
-        <v>307</v>
-      </c>
-      <c r="B53" s="212">
-        <f>C13*B35</f>
-        <v>453.59999999999997</v>
-      </c>
-      <c r="C53" s="185"/>
+      <c r="A53" s="205" t="s">
+        <v>342</v>
+      </c>
+      <c r="B53" s="216">
+        <f>B41*B40</f>
+        <v>261.60000000000002</v>
+      </c>
+      <c r="C53" s="203" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="205" t="s">
-        <v>308</v>
-      </c>
-      <c r="B54" s="225">
-        <f>B44+B45</f>
-        <v>916.65</v>
-      </c>
-      <c r="C54" s="203" t="s">
-        <v>340</v>
-      </c>
+      <c r="A54" s="218"/>
+      <c r="B54" s="219"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="227"/>
-      <c r="B55" s="228"/>
-      <c r="C55" s="226"/>
-      <c r="D55" s="222"/>
+      <c r="A55" s="217"/>
+      <c r="B55" s="225"/>
+      <c r="C55" s="217"/>
+      <c r="D55" s="214"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="12">
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C44:F44"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:D8"/>

</xml_diff>